<commit_message>
updated code to reflect continued changes in paper
</commit_message>
<xml_diff>
--- a/r_map/data_boot_cq_remov_As.xlsx
+++ b/r_map/data_boot_cq_remov_As.xlsx
@@ -594,16 +594,16 @@
         <v>2207648</v>
       </c>
       <c r="C2">
-        <v>24084085054.395599</v>
+        <v>24489996600.256199</v>
       </c>
       <c r="E2">
-        <v>22231463127.134399</v>
+        <v>22606150707.928799</v>
       </c>
       <c r="F2">
-        <v>10909.38639420578</v>
+        <v>11093.252457029472</v>
       </c>
       <c r="H2">
-        <v>10070.20282542072</v>
+        <v>10239.925344950281</v>
       </c>
       <c r="I2" t="s">
         <v>9</v>
@@ -629,16 +629,16 @@
         <v>505392</v>
       </c>
       <c r="C3">
-        <v>1067922008.2181365</v>
+        <v>1064403666.0361398</v>
       </c>
       <c r="E3">
-        <v>985774161.43212605</v>
+        <v>982526460.95643663</v>
       </c>
       <c r="F3">
-        <v>2113.0568117780585</v>
+        <v>2106.0952014201648</v>
       </c>
       <c r="H3">
-        <v>1950.5139801028231</v>
+        <v>1944.0878782339978</v>
       </c>
       <c r="I3" t="s">
         <v>9</v>
@@ -664,16 +664,16 @@
         <v>2726384</v>
       </c>
       <c r="C4">
-        <v>16552545721.731565</v>
+        <v>16695116825.836149</v>
       </c>
       <c r="E4">
-        <v>3347001011.9341197</v>
+        <v>3415474812.5422392</v>
       </c>
       <c r="F4">
-        <v>6071.2451810645771</v>
+        <v>6123.5382931517161</v>
       </c>
       <c r="H4">
-        <v>1227.6337492936136</v>
+        <v>1252.7489937375803</v>
       </c>
       <c r="I4" t="s">
         <v>9</v>
@@ -699,16 +699,16 @@
         <v>541762</v>
       </c>
       <c r="C5">
-        <v>381062162.22547197</v>
+        <v>386165673.32670599</v>
       </c>
       <c r="E5">
-        <v>351749688.20812798</v>
+        <v>356460621.53234392</v>
       </c>
       <c r="F5">
-        <v>703.37558231376875</v>
+        <v>712.79579100547107</v>
       </c>
       <c r="H5">
-        <v>649.26976828963268</v>
+        <v>657.9653455435116</v>
       </c>
       <c r="I5" t="s">
         <v>10</v>
@@ -737,13 +737,13 @@
         <v>432021780.16881657</v>
       </c>
       <c r="E6">
-        <v>53340214.985781841</v>
+        <v>46049106.462545462</v>
       </c>
       <c r="F6">
         <v>1332.8164204849004</v>
       </c>
       <c r="H6">
-        <v>164.55817199184875</v>
+        <v>142.06460891382622</v>
       </c>
       <c r="I6" t="s">
         <v>10</v>
@@ -810,22 +810,22 @@
         <v>8921964</v>
       </c>
       <c r="C8">
-        <v>47165166540.988541</v>
+        <v>46792899440.812332</v>
       </c>
       <c r="D8">
-        <v>2528628.1009751223</v>
+        <v>2513916.3805485684</v>
       </c>
       <c r="E8">
-        <v>92359293.071044385</v>
+        <v>91692104.01712352</v>
       </c>
       <c r="F8">
-        <v>5286.4107657224959</v>
+        <v>5244.6859728208192</v>
       </c>
       <c r="G8">
-        <v>0.28341608428089626</v>
+        <v>0.28176715132997271</v>
       </c>
       <c r="H8">
-        <v>10.351901562373978</v>
+        <v>10.277121048361494</v>
       </c>
       <c r="I8" t="s">
         <v>12</v>
@@ -851,22 +851,22 @@
         <v>7744214</v>
       </c>
       <c r="C9">
-        <v>21972273651.400116</v>
+        <v>21784161853.381332</v>
       </c>
       <c r="D9">
-        <v>1177336.5170392073</v>
+        <v>1173109.896345186</v>
       </c>
       <c r="E9">
-        <v>33743964.852051541</v>
+        <v>33984087.793017775</v>
       </c>
       <c r="F9">
-        <v>2837.2503202261864</v>
+        <v>2812.9596952487791</v>
       </c>
       <c r="G9">
-        <v>0.1520278903758609</v>
+        <v>0.15148211249652788</v>
       </c>
       <c r="H9">
-        <v>4.3573130665102404</v>
+        <v>4.3883198208388583</v>
       </c>
       <c r="I9" t="s">
         <v>13</v>
@@ -895,13 +895,13 @@
         <v>2725800951.7334266</v>
       </c>
       <c r="E10">
-        <v>295384898.90312731</v>
+        <v>290542523.51127279</v>
       </c>
       <c r="F10">
         <v>1352.9394590990962</v>
       </c>
       <c r="H10">
-        <v>146.61301115692083</v>
+        <v>144.2095191707418</v>
       </c>
       <c r="I10" t="s">
         <v>14</v>
@@ -927,22 +927,22 @@
         <v>9164672</v>
       </c>
       <c r="C11">
-        <v>21343552476.579674</v>
+        <v>21544833433.989388</v>
       </c>
       <c r="D11">
-        <v>1145122.4987554362</v>
+        <v>1150546.950597795</v>
       </c>
       <c r="E11">
-        <v>42191510.909001902</v>
+        <v>41209642.098474637</v>
       </c>
       <c r="F11">
-        <v>2328.8943103015222</v>
+        <v>2350.8570120119289</v>
       </c>
       <c r="G11">
-        <v>0.12494964345209912</v>
+        <v>0.1255415306295517</v>
       </c>
       <c r="H11">
-        <v>4.6037120487238283</v>
+        <v>4.4965757747221762</v>
       </c>
       <c r="I11" t="s">
         <v>11</v>
@@ -968,19 +968,19 @@
         <v>3900879</v>
       </c>
       <c r="C12">
-        <v>8270587995.3031025</v>
+        <v>8256298781.1743488</v>
       </c>
       <c r="D12">
-        <v>450107.06426380656</v>
+        <v>445348.69476852019</v>
       </c>
       <c r="E12">
         <v>17890710.71209925</v>
       </c>
       <c r="F12">
-        <v>2120.1857312936654</v>
+        <v>2116.522655835864</v>
       </c>
       <c r="G12">
-        <v>0.11538606151685468</v>
+        <v>0.11416624170309313</v>
       </c>
       <c r="H12">
         <v>4.5863280332712835</v>
@@ -1009,16 +1009,16 @@
         <v>9744872</v>
       </c>
       <c r="C13">
-        <v>53492679802.303589</v>
+        <v>53392914693.218559</v>
       </c>
       <c r="E13">
-        <v>2059255465.6211224</v>
+        <v>2068114844.4619861</v>
       </c>
       <c r="F13">
-        <v>5489.3157962776313</v>
+        <v>5479.078092890144</v>
       </c>
       <c r="H13">
-        <v>211.31683059778746</v>
+        <v>212.22596299489476</v>
       </c>
       <c r="I13" t="s">
         <v>13</v>
@@ -1044,22 +1044,22 @@
         <v>2258981</v>
       </c>
       <c r="C14">
-        <v>13531680395.927164</v>
+        <v>13526427942.052128</v>
       </c>
       <c r="D14">
-        <v>754835.58477789757</v>
+        <v>756325.87087792146</v>
       </c>
       <c r="E14">
-        <v>16681566.711594814</v>
+        <v>29952375.22545905</v>
       </c>
       <c r="F14">
-        <v>5990.1700793088403</v>
+        <v>5987.8449363018672</v>
       </c>
       <c r="G14">
-        <v>0.33414870898776822</v>
+        <v>0.33480842507215486</v>
       </c>
       <c r="H14">
-        <v>7.3845537928804248</v>
+        <v>13.259241766734227</v>
       </c>
       <c r="I14" t="s">
         <v>13</v>
@@ -1085,22 +1085,22 @@
         <v>12851943</v>
       </c>
       <c r="C15">
-        <v>49088018425.203873</v>
+        <v>48803596110.329269</v>
       </c>
       <c r="D15">
-        <v>2654786.4093342964</v>
+        <v>2638777.1500995876</v>
       </c>
       <c r="E15">
-        <v>99143190.654371977</v>
+        <v>98127301.468019545</v>
       </c>
       <c r="F15">
-        <v>3819.5017224402472</v>
+        <v>3797.3710364517856</v>
       </c>
       <c r="G15">
-        <v>0.20656692994470147</v>
+        <v>0.20532126154773545</v>
       </c>
       <c r="H15">
-        <v>7.7142569535495129</v>
+        <v>7.6352113815023559</v>
       </c>
       <c r="I15" t="s">
         <v>15</v>
@@ -1126,22 +1126,22 @@
         <v>1157290</v>
       </c>
       <c r="C16">
-        <v>7469294374.84202</v>
+        <v>7511221436.8078976</v>
       </c>
       <c r="D16">
-        <v>408678.60251389042</v>
+        <v>412470.81961736432</v>
       </c>
       <c r="E16">
-        <v>15381292.756044278</v>
+        <v>12398810.798662223</v>
       </c>
       <c r="F16">
-        <v>6454.1250463082024</v>
+        <v>6490.3537028816427</v>
       </c>
       <c r="G16">
-        <v>0.35313413449860487</v>
+        <v>0.3564109424754075</v>
       </c>
       <c r="H16">
-        <v>13.290785158468731</v>
+        <v>10.713659323645953</v>
       </c>
       <c r="I16" t="s">
         <v>15</v>
@@ -1167,16 +1167,16 @@
         <v>2981276</v>
       </c>
       <c r="C17">
-        <v>3456705506.3836575</v>
+        <v>3453224787.2175846</v>
       </c>
       <c r="E17">
-        <v>592994525.50538635</v>
+        <v>607119127.88716745</v>
       </c>
       <c r="F17">
-        <v>1159.4718189069572</v>
+        <v>1158.3042922619659</v>
       </c>
       <c r="H17">
-        <v>198.90628224471212</v>
+        <v>203.64405304546358</v>
       </c>
       <c r="I17" t="s">
         <v>16</v>
@@ -1202,16 +1202,16 @@
         <v>1265697</v>
       </c>
       <c r="C18">
-        <v>1527314314.6308203</v>
+        <v>1555481430.9353902</v>
       </c>
       <c r="E18">
-        <v>188275720.71873254</v>
+        <v>179075706.30720007</v>
       </c>
       <c r="F18">
-        <v>1206.6982181602866</v>
+        <v>1228.9524514440582</v>
       </c>
       <c r="H18">
-        <v>148.75260091375151</v>
+        <v>141.48386723457517</v>
       </c>
       <c r="I18" t="s">
         <v>16</v>
@@ -1237,16 +1237,16 @@
         <v>1796131</v>
       </c>
       <c r="C19">
-        <v>1466549872.5235019</v>
+        <v>1475809598.0331714</v>
       </c>
       <c r="E19">
-        <v>987202691.1960479</v>
+        <v>1007399964.0421307</v>
       </c>
       <c r="F19">
-        <v>816.50496123250582</v>
+        <v>821.6603343704727</v>
       </c>
       <c r="H19">
-        <v>549.62733297072873</v>
+        <v>560.87221034664549</v>
       </c>
       <c r="I19" t="s">
         <v>16</v>
@@ -1272,13 +1272,13 @@
         <v>2372033</v>
       </c>
       <c r="C20">
-        <v>2466599396.6861267</v>
+        <v>2476372139.8220057</v>
       </c>
       <c r="E20">
         <v>267296191.5877637</v>
       </c>
       <c r="F20">
-        <v>1039.8672348513392</v>
+        <v>1043.9872210133694</v>
       </c>
       <c r="H20">
         <v>112.68654002189838</v>
@@ -1307,16 +1307,16 @@
         <v>4881045</v>
       </c>
       <c r="C21">
-        <v>4404243924.2620392</v>
+        <v>4451605629.5937185</v>
       </c>
       <c r="E21">
-        <v>845813240.06744075</v>
+        <v>878317342.40708661</v>
       </c>
       <c r="F21">
-        <v>902.31577956401532</v>
+        <v>912.01896921534603</v>
       </c>
       <c r="H21">
-        <v>173.28527806390653</v>
+        <v>179.94452876527191</v>
       </c>
       <c r="I21" t="s">
         <v>16</v>
@@ -1342,16 +1342,16 @@
         <v>2219933</v>
       </c>
       <c r="C22">
-        <v>2497257144.9289165</v>
+        <v>2497373125.1473665</v>
       </c>
       <c r="E22">
-        <v>370353748.36265945</v>
+        <v>385529621.68322295</v>
       </c>
       <c r="F22">
-        <v>1124.924556249633</v>
+        <v>1124.9768011680383</v>
       </c>
       <c r="H22">
-        <v>166.83104776705397</v>
+        <v>173.66723305758461</v>
       </c>
       <c r="I22" t="s">
         <v>16</v>
@@ -1377,7 +1377,7 @@
         <v>1056327</v>
       </c>
       <c r="C23">
-        <v>1850866915.7476006</v>
+        <v>1819572174.5542016</v>
       </c>
       <c r="D23">
         <v>107407.98622454359</v>
@@ -1386,7 +1386,7 @@
         <v>4172291.8777323002</v>
       </c>
       <c r="F23">
-        <v>1752.1723062532724</v>
+        <v>1722.5463086281063</v>
       </c>
       <c r="G23">
         <v>0.10168062183825993</v>
@@ -1418,22 +1418,22 @@
         <v>1066912</v>
       </c>
       <c r="C24">
-        <v>4783468571.0279751</v>
+        <v>4783345373.3237896</v>
       </c>
       <c r="D24">
-        <v>263195.82531060057</v>
+        <v>263709.42790217476</v>
       </c>
       <c r="E24">
-        <v>7317601.229988643</v>
+        <v>8000925.9035675367</v>
       </c>
       <c r="F24">
-        <v>4483.4705871036931</v>
+        <v>4483.3551158144155</v>
       </c>
       <c r="G24">
-        <v>0.24668934767872192</v>
+        <v>0.24717073938822953</v>
       </c>
       <c r="H24">
-        <v>6.8586736581729735</v>
+        <v>7.4991432316512858</v>
       </c>
       <c r="I24" t="s">
         <v>16</v>
@@ -1459,22 +1459,22 @@
         <v>4489538</v>
       </c>
       <c r="C25">
-        <v>20333988577.790474</v>
+        <v>20641604641.679642</v>
       </c>
       <c r="D25">
-        <v>1085329.2823945817</v>
+        <v>1107709.1369018322</v>
       </c>
       <c r="E25">
-        <v>36235429.303873554</v>
+        <v>36670940.48189272</v>
       </c>
       <c r="F25">
-        <v>4529.1940012069117</v>
+        <v>4597.7124242360005</v>
       </c>
       <c r="G25">
-        <v>0.24174631830593296</v>
+        <v>0.24673120862365622</v>
       </c>
       <c r="H25">
-        <v>8.0710819919273558</v>
+        <v>8.1680877813914741</v>
       </c>
       <c r="I25" t="s">
         <v>17</v>
@@ -1503,13 +1503,13 @@
         <v>11970845499.812359</v>
       </c>
       <c r="E26">
-        <v>351729878.83625013</v>
+        <v>364885089.91303986</v>
       </c>
       <c r="F26">
         <v>3999.670392906402</v>
       </c>
       <c r="H26">
-        <v>117.51914956248973</v>
+        <v>121.91453736171368</v>
       </c>
       <c r="I26" t="s">
         <v>17</v>
@@ -1538,13 +1538,13 @@
         <v>2873990191.3786931</v>
       </c>
       <c r="E27">
-        <v>540694123.3489635</v>
+        <v>537048913.61971426</v>
       </c>
       <c r="F27">
         <v>12523.160480791188</v>
       </c>
       <c r="H27">
-        <v>2356.0272745647535</v>
+        <v>2340.1435925109777</v>
       </c>
       <c r="I27" t="s">
         <v>17</v>
@@ -1570,22 +1570,22 @@
         <v>6529869</v>
       </c>
       <c r="C28">
-        <v>52456806971.763428</v>
+        <v>52658524924.199966</v>
       </c>
       <c r="D28">
-        <v>2823066.1380097992</v>
+        <v>2831085.7968436782</v>
       </c>
       <c r="E28">
-        <v>101461226.68924181</v>
+        <v>101663403.00501882</v>
       </c>
       <c r="F28">
-        <v>8033.3628395551932</v>
+        <v>8064.2544167731339</v>
       </c>
       <c r="G28">
-        <v>0.43233120572706729</v>
+        <v>0.4335593557609928</v>
       </c>
       <c r="H28">
-        <v>15.53801870898816</v>
+        <v>15.568980481081446</v>
       </c>
       <c r="I28" t="s">
         <v>17</v>
@@ -1611,22 +1611,22 @@
         <v>1441562</v>
       </c>
       <c r="C29">
-        <v>3748570265.9031715</v>
+        <v>3957418149.832819</v>
       </c>
       <c r="D29">
-        <v>204810.59024930157</v>
+        <v>204444.41470190609</v>
       </c>
       <c r="E29">
-        <v>6827505.9797880286</v>
+        <v>6813151.3831430636</v>
       </c>
       <c r="F29">
-        <v>2600.3531349350023</v>
+        <v>2745.2292373361806</v>
       </c>
       <c r="G29">
-        <v>0.14207546414882022</v>
+        <v>0.14182145110783032</v>
       </c>
       <c r="H29">
-        <v>4.7361861507087646</v>
+        <v>4.7262284821208276</v>
       </c>
       <c r="I29" t="s">
         <v>17</v>
@@ -1652,16 +1652,16 @@
         <v>1650341</v>
       </c>
       <c r="C30">
-        <v>3726515723.0853968</v>
+        <v>3652662052.6035676</v>
       </c>
       <c r="E30">
-        <v>368016770.79774249</v>
+        <v>386051923.54400325</v>
       </c>
       <c r="F30">
-        <v>2258.027718565676</v>
+        <v>2213.27716672104</v>
       </c>
       <c r="H30">
-        <v>222.99438164460707</v>
+        <v>233.92251876672955</v>
       </c>
       <c r="I30" t="s">
         <v>17</v>
@@ -1690,7 +1690,7 @@
         <v>17618775425.398262</v>
       </c>
       <c r="D31">
-        <v>1123156.7189226472</v>
+        <v>1001771.10858335</v>
       </c>
       <c r="E31">
         <v>27461256.78923342</v>
@@ -1699,7 +1699,7 @@
         <v>3534.8921161808921</v>
       </c>
       <c r="G31">
-        <v>0.22534130409721814</v>
+        <v>0.20098745278541572</v>
       </c>
       <c r="H31">
         <v>5.509609934907604</v>
@@ -1728,16 +1728,16 @@
         <v>2093626</v>
       </c>
       <c r="C32">
-        <v>7332187550.6209698</v>
+        <v>7333268464.4968204</v>
       </c>
       <c r="E32">
-        <v>988318752.52384675</v>
+        <v>989118636.36655855</v>
       </c>
       <c r="F32">
-        <v>3502.1477334638421</v>
+        <v>3502.6640214139584</v>
       </c>
       <c r="H32">
-        <v>472.06079429843095</v>
+        <v>472.44285099944238</v>
       </c>
       <c r="I32" t="s">
         <v>17</v>
@@ -1769,7 +1769,7 @@
         <v>10855.626528652858</v>
       </c>
       <c r="E33">
-        <v>272450.74517261999</v>
+        <v>142867.81315380899</v>
       </c>
       <c r="F33">
         <v>2492.8202765253423</v>
@@ -1778,7 +1778,7 @@
         <v>0.16141235508152463</v>
       </c>
       <c r="H33">
-        <v>4.0510712399652062</v>
+        <v>2.1243020958427601</v>
       </c>
       <c r="I33" t="s">
         <v>17</v>
@@ -1804,16 +1804,16 @@
         <v>245567</v>
       </c>
       <c r="C34">
-        <v>199431423.14097902</v>
+        <v>195962861.44996679</v>
       </c>
       <c r="E34">
-        <v>23442697.911787689</v>
+        <v>23151629.179194972</v>
       </c>
       <c r="F34">
-        <v>812.12631640643497</v>
+        <v>798.00161035467625</v>
       </c>
       <c r="H34">
-        <v>95.463551339502814</v>
+        <v>94.278258801854363</v>
       </c>
       <c r="I34" t="s">
         <v>18</v>
@@ -1842,13 +1842,13 @@
         <v>759718359.54945791</v>
       </c>
       <c r="E35">
-        <v>218471340.96321055</v>
+        <v>218725648.1850158</v>
       </c>
       <c r="F35">
         <v>1058.2141025169174</v>
       </c>
       <c r="H35">
-        <v>304.30942084926778</v>
+        <v>304.66364618172622</v>
       </c>
       <c r="I35" t="s">
         <v>18</v>
@@ -1874,16 +1874,16 @@
         <v>1081826</v>
       </c>
       <c r="C36">
-        <v>1240902706.6982441</v>
+        <v>1218432074.6694152</v>
       </c>
       <c r="E36">
-        <v>150199061.71746653</v>
+        <v>150435537.72460911</v>
       </c>
       <c r="F36">
-        <v>1147.0446325917885</v>
+        <v>1126.2736102380745</v>
       </c>
       <c r="H36">
-        <v>138.83846544404233</v>
+        <v>139.0570551314251</v>
       </c>
       <c r="I36" t="s">
         <v>18</v>
@@ -1909,16 +1909,16 @@
         <v>250729</v>
       </c>
       <c r="C37">
-        <v>206834876.68540317</v>
+        <v>209233470.48696238</v>
       </c>
       <c r="E37">
-        <v>148938817.39775997</v>
+        <v>144642505.35743999</v>
       </c>
       <c r="F37">
-        <v>824.93399919994567</v>
+        <v>834.50047855239075</v>
       </c>
       <c r="H37">
-        <v>594.02309823658197</v>
+        <v>576.88781655668072</v>
       </c>
       <c r="I37" t="s">
         <v>18</v>
@@ -1944,13 +1944,13 @@
         <v>750815</v>
       </c>
       <c r="C38">
-        <v>1068168288.8890224</v>
+        <v>1071185994.6574724</v>
       </c>
       <c r="E38">
         <v>6962793.207994638</v>
       </c>
       <c r="F38">
-        <v>1422.6784079820227</v>
+        <v>1426.6976480990288</v>
       </c>
       <c r="H38">
         <v>9.2736469143459281</v>
@@ -1979,16 +1979,16 @@
         <v>384251</v>
       </c>
       <c r="C39">
-        <v>447042711.97035843</v>
+        <v>445278504.75586146</v>
       </c>
       <c r="E39">
-        <v>54890555.663870595</v>
+        <v>48253173.448854558</v>
       </c>
       <c r="F39">
-        <v>1163.4132688538441</v>
+        <v>1158.8219803093848</v>
       </c>
       <c r="H39">
-        <v>142.85078155651019</v>
+        <v>125.57722282792903</v>
       </c>
       <c r="I39" t="s">
         <v>19</v>
@@ -2014,16 +2014,16 @@
         <v>1245893</v>
       </c>
       <c r="C40">
-        <v>6864737570.0919342</v>
+        <v>6869043625.123291</v>
       </c>
       <c r="E40">
-        <v>793622831.16816247</v>
+        <v>837703239.33825016</v>
       </c>
       <c r="F40">
-        <v>5509.8933617027578</v>
+        <v>5513.3495614176272</v>
       </c>
       <c r="H40">
-        <v>636.99116310001136</v>
+        <v>672.37173604655482</v>
       </c>
       <c r="I40" t="s">
         <v>20</v>
@@ -2049,22 +2049,22 @@
         <v>827980</v>
       </c>
       <c r="C41">
-        <v>5753124097.5693321</v>
+        <v>5729991978.6079082</v>
       </c>
       <c r="D41">
-        <v>313573.52196090628</v>
+        <v>308405.71364815813</v>
       </c>
       <c r="E41">
-        <v>10694663.26472136</v>
+        <v>10683232.709778557</v>
       </c>
       <c r="F41">
-        <v>6948.3853445365003</v>
+        <v>6920.4473279643335</v>
       </c>
       <c r="G41">
-        <v>0.3787211308979761</v>
+        <v>0.37247966575057145</v>
       </c>
       <c r="H41">
-        <v>12.916571976039711</v>
+        <v>12.902766624530251</v>
       </c>
       <c r="I41" t="s">
         <v>20</v>
@@ -2090,22 +2090,22 @@
         <v>2177256</v>
       </c>
       <c r="C42">
-        <v>11190598469.691425</v>
+        <v>11317198653.203259</v>
       </c>
       <c r="D42">
-        <v>584211.33657097653</v>
+        <v>591692.07258807123</v>
       </c>
       <c r="E42">
-        <v>9057426.5150538553</v>
+        <v>8730124.7591729704</v>
       </c>
       <c r="F42">
-        <v>5139.7715609425004</v>
+        <v>5197.9182297365387</v>
       </c>
       <c r="G42">
-        <v>0.26832459599191671</v>
+        <v>0.2717604510393225</v>
       </c>
       <c r="H42">
-        <v>4.160019085975124</v>
+        <v>4.0096914461014093</v>
       </c>
       <c r="I42" t="s">
         <v>20</v>
@@ -2131,22 +2131,22 @@
         <v>2300225</v>
       </c>
       <c r="C43">
-        <v>25272296266.940968</v>
+        <v>24853341782.411163</v>
       </c>
       <c r="D43">
-        <v>1358025.3552846813</v>
+        <v>1331214.5355124227</v>
       </c>
       <c r="E43">
-        <v>48418629.55642724</v>
+        <v>47861704.482322343</v>
       </c>
       <c r="F43">
-        <v>10986.880095182414</v>
+        <v>10804.743789155915</v>
       </c>
       <c r="G43">
-        <v>0.5903880512926698</v>
+        <v>0.57873231336605024</v>
       </c>
       <c r="H43">
-        <v>21.049518875947889</v>
+        <v>20.807401224802941</v>
       </c>
       <c r="I43" t="s">
         <v>20</v>
@@ -2172,22 +2172,22 @@
         <v>1488285</v>
       </c>
       <c r="C44">
-        <v>7473220580.2195177</v>
+        <v>7546898230.5114403</v>
       </c>
       <c r="D44">
-        <v>404332.64818848472</v>
+        <v>406410.43134602427</v>
       </c>
       <c r="E44">
-        <v>13286701.345431294</v>
+        <v>13072663.988330644</v>
       </c>
       <c r="F44">
-        <v>5021.3639055822769</v>
+        <v>5070.8689736921624</v>
       </c>
       <c r="G44">
-        <v>0.27167689534496736</v>
+        <v>0.27307298759714993</v>
       </c>
       <c r="H44">
-        <v>8.9275248661588975</v>
+        <v>8.7837101014460579</v>
       </c>
       <c r="I44" t="s">
         <v>20</v>
@@ -2213,16 +2213,16 @@
         <v>48329</v>
       </c>
       <c r="C45">
-        <v>179022210.86207873</v>
+        <v>176393038.35173696</v>
       </c>
       <c r="E45">
-        <v>28776907.387949288</v>
+        <v>28499052.961971123</v>
       </c>
       <c r="F45">
-        <v>3704.2399152078196</v>
+        <v>3649.8383651997137</v>
       </c>
       <c r="H45">
-        <v>595.43767485255819</v>
+        <v>589.68844714293948</v>
       </c>
       <c r="I45" t="s">
         <v>20</v>
@@ -2248,16 +2248,16 @@
         <v>1336530</v>
       </c>
       <c r="C46">
-        <v>2596527297.2654991</v>
+        <v>2611721519.3241863</v>
       </c>
       <c r="E46">
-        <v>359889250.31108928</v>
+        <v>364104164.88919008</v>
       </c>
       <c r="F46">
-        <v>1942.7377591715103</v>
+        <v>1954.1061699506831</v>
       </c>
       <c r="H46">
-        <v>269.2713596485595</v>
+        <v>272.42498476591629</v>
       </c>
       <c r="I46" t="s">
         <v>22</v>
@@ -2283,22 +2283,22 @@
         <v>4238250</v>
       </c>
       <c r="C47">
-        <v>23438672061.672489</v>
+        <v>23588494151.957512</v>
       </c>
       <c r="D47">
-        <v>1256967.9167340761</v>
+        <v>1263487.7970551956</v>
       </c>
       <c r="E47">
-        <v>40909182.495422229</v>
+        <v>41456553.622950301</v>
       </c>
       <c r="F47">
-        <v>5530.2712349843659</v>
+        <v>5565.6212238441603</v>
       </c>
       <c r="G47">
-        <v>0.29657710534632842</v>
+        <v>0.2981154478983532</v>
       </c>
       <c r="H47">
-        <v>9.6523759795722839</v>
+        <v>9.7815262485578476</v>
       </c>
       <c r="I47" t="s">
         <v>22</v>
@@ -2324,16 +2324,16 @@
         <v>1825199</v>
       </c>
       <c r="C48">
-        <v>1445420650.1292064</v>
+        <v>1452848163.5803692</v>
       </c>
       <c r="E48">
-        <v>231211939.24813265</v>
+        <v>238203670.48760289</v>
       </c>
       <c r="F48">
-        <v>791.92496277348732</v>
+        <v>795.99438942294466</v>
       </c>
       <c r="H48">
-        <v>126.677660489696</v>
+        <v>130.50832840013771</v>
       </c>
       <c r="I48" t="s">
         <v>23</v>
@@ -2359,16 +2359,16 @@
         <v>7101778</v>
       </c>
       <c r="C49">
-        <v>6727007253.5105085</v>
+        <v>6640991260.8969269</v>
       </c>
       <c r="E49">
-        <v>1062824026.8675784</v>
+        <v>1035510420.7218255</v>
       </c>
       <c r="F49">
-        <v>947.22860296541353</v>
+        <v>935.11670751985298</v>
       </c>
       <c r="H49">
-        <v>149.65604766406079</v>
+        <v>145.81002401396177</v>
       </c>
       <c r="I49" t="s">
         <v>23</v>
@@ -2394,16 +2394,16 @@
         <v>992174</v>
       </c>
       <c r="C50">
-        <v>1311106091.2369776</v>
+        <v>1262441723.3042908</v>
       </c>
       <c r="E50">
-        <v>155838285.71373361</v>
+        <v>145994069.66887155</v>
       </c>
       <c r="F50">
-        <v>1321.4477412600791</v>
+        <v>1272.3995219631747</v>
       </c>
       <c r="H50">
-        <v>157.06749593693604</v>
+        <v>147.14563138005184</v>
       </c>
       <c r="I50" t="s">
         <v>23</v>
@@ -2429,16 +2429,16 @@
         <v>1769518</v>
       </c>
       <c r="C51">
-        <v>1925502246.0301332</v>
+        <v>1924911193.9643822</v>
       </c>
       <c r="E51">
-        <v>365412852.50498283</v>
+        <v>374315169.42319262</v>
       </c>
       <c r="F51">
-        <v>1088.150697551612</v>
+        <v>1087.8166788720896</v>
       </c>
       <c r="H51">
-        <v>206.50417373826252</v>
+        <v>211.53510132318098</v>
       </c>
       <c r="I51" t="s">
         <v>23</v>
@@ -2464,22 +2464,22 @@
         <v>16149545</v>
       </c>
       <c r="C52">
-        <v>41239125967.339584</v>
+        <v>41323369052.987656</v>
       </c>
       <c r="D52">
-        <v>2213588.6478221295</v>
+        <v>2223614.6916434523</v>
       </c>
       <c r="E52">
-        <v>80857474.355393857</v>
+        <v>81742873.504515424</v>
       </c>
       <c r="F52">
-        <v>2553.5781947627374</v>
+        <v>2558.7946318603808</v>
       </c>
       <c r="G52">
-        <v>0.13706817423166595</v>
+        <v>0.13768899938936063</v>
       </c>
       <c r="H52">
-        <v>5.0067958171820841</v>
+        <v>5.0616208385137433</v>
       </c>
       <c r="I52" t="s">
         <v>23</v>
@@ -2505,16 +2505,16 @@
         <v>1806150</v>
       </c>
       <c r="C53">
-        <v>3485844399.2180147</v>
+        <v>3490156013.5056229</v>
       </c>
       <c r="E53">
-        <v>621193261.40749085</v>
+        <v>629798549.12257349</v>
       </c>
       <c r="F53">
-        <v>1929.9861026038893</v>
+        <v>1932.3732876591773</v>
       </c>
       <c r="H53">
-        <v>343.9322655413398</v>
+        <v>348.69670244585086</v>
       </c>
       <c r="I53" t="s">
         <v>23</v>
@@ -2540,16 +2540,16 @@
         <v>5446539</v>
       </c>
       <c r="C54">
-        <v>33384812827.421848</v>
+        <v>33243273010.595436</v>
       </c>
       <c r="E54">
-        <v>6756343731.6628542</v>
+        <v>6570449177.0224743</v>
       </c>
       <c r="F54">
-        <v>6129.5462728572857</v>
+        <v>6103.559161257348</v>
       </c>
       <c r="H54">
-        <v>1240.4838617079313</v>
+        <v>1206.353094510564</v>
       </c>
       <c r="I54" t="s">
         <v>23</v>
@@ -2575,16 +2575,16 @@
         <v>2101351</v>
       </c>
       <c r="C55">
-        <v>3893642514.2965918</v>
+        <v>3870491746.6758318</v>
       </c>
       <c r="E55">
-        <v>419618667.1243121</v>
+        <v>458979752.53187871</v>
       </c>
       <c r="F55">
-        <v>1852.9234355881485</v>
+        <v>1841.9063481902031</v>
       </c>
       <c r="H55">
-        <v>199.68994571792723</v>
+        <v>218.42126923673325</v>
       </c>
       <c r="I55" t="s">
         <v>23</v>
@@ -2613,7 +2613,7 @@
         <v>335427299.71135944</v>
       </c>
       <c r="D56">
-        <v>20629.331577249039</v>
+        <v>20843.380496407706</v>
       </c>
       <c r="E56">
         <v>491415.29596222768</v>
@@ -2622,7 +2622,7 @@
         <v>1632.9886503934113</v>
       </c>
       <c r="G56">
-        <v>0.10043149248686285</v>
+        <v>0.10147356466141712</v>
       </c>
       <c r="H56">
         <v>2.3923979998842673</v>
@@ -2651,16 +2651,16 @@
         <v>500876</v>
       </c>
       <c r="C57">
-        <v>597385801.15770984</v>
+        <v>592479094.42275906</v>
       </c>
       <c r="E57">
-        <v>113418494.0260421</v>
+        <v>114915277.84759404</v>
       </c>
       <c r="F57">
-        <v>1192.6820234104043</v>
+        <v>1182.8857729712722</v>
       </c>
       <c r="H57">
-        <v>226.44026470831523</v>
+        <v>229.42859679360566</v>
       </c>
       <c r="I57" t="s">
         <v>23</v>
@@ -2686,16 +2686,16 @@
         <v>869762</v>
       </c>
       <c r="C58">
-        <v>994354404.31126797</v>
+        <v>999089425.28417861</v>
       </c>
       <c r="E58">
-        <v>106307059.01640002</v>
+        <v>104564320.34400003</v>
       </c>
       <c r="F58">
-        <v>1143.2488477437137</v>
+        <v>1148.6928898758265</v>
       </c>
       <c r="H58">
-        <v>122.22545824765858</v>
+        <v>120.22176221081172</v>
       </c>
       <c r="I58" t="s">
         <v>23</v>
@@ -2756,13 +2756,13 @@
         <v>1615868</v>
       </c>
       <c r="C60">
-        <v>1376705267.3093872</v>
+        <v>1379079582.1570895</v>
       </c>
       <c r="E60">
         <v>271344968.69019115</v>
       </c>
       <c r="F60">
-        <v>851.99116964342829</v>
+        <v>853.46054390401287</v>
       </c>
       <c r="H60">
         <v>167.92520718907184</v>
@@ -2791,16 +2791,16 @@
         <v>1420063</v>
       </c>
       <c r="C61">
-        <v>1675909303.0307131</v>
+        <v>1657651426.6561434</v>
       </c>
       <c r="E61">
-        <v>318291312.16623044</v>
+        <v>320464621.5114491</v>
       </c>
       <c r="F61">
-        <v>1180.1654595822249</v>
+        <v>1167.3083705836596</v>
       </c>
       <c r="H61">
-        <v>224.13886719549092</v>
+        <v>225.66929883494541</v>
       </c>
       <c r="I61" t="s">
         <v>26</v>
@@ -2826,16 +2826,16 @@
         <v>2037047</v>
       </c>
       <c r="C62">
-        <v>1792563861.0395324</v>
+        <v>1792791688.2216315</v>
       </c>
       <c r="E62">
-        <v>239810839.06435636</v>
+        <v>249104741.49709928</v>
       </c>
       <c r="F62">
-        <v>879.98159150944105</v>
+        <v>880.09343339728116</v>
       </c>
       <c r="H62">
-        <v>117.7247452142029</v>
+        <v>122.28718409398472</v>
       </c>
       <c r="I62" t="s">
         <v>26</v>
@@ -2861,16 +2861,16 @@
         <v>233500</v>
       </c>
       <c r="C63">
-        <v>103383468.94915494</v>
+        <v>108642531.42007363</v>
       </c>
       <c r="E63">
-        <v>13050815.69684455</v>
+        <v>13491556.189420912</v>
       </c>
       <c r="F63">
-        <v>442.75575567089913</v>
+        <v>465.27850715234956</v>
       </c>
       <c r="H63">
-        <v>55.892144311968096</v>
+        <v>57.779683894736245</v>
       </c>
       <c r="I63" t="s">
         <v>26</v>
@@ -2896,16 +2896,16 @@
         <v>16042082</v>
       </c>
       <c r="C64">
-        <v>16751342482.000801</v>
+        <v>16593312563.508049</v>
       </c>
       <c r="E64">
-        <v>3355556366.7098646</v>
+        <v>3308273876.0329723</v>
       </c>
       <c r="F64">
-        <v>1044.212495734706</v>
+        <v>1034.3615350867829</v>
       </c>
       <c r="H64">
-        <v>209.17212408650352</v>
+        <v>206.22472045916311</v>
       </c>
       <c r="I64" t="s">
         <v>26</v>
@@ -2931,16 +2931,16 @@
         <v>2119428</v>
       </c>
       <c r="C65">
-        <v>2333915779.3683033</v>
+        <v>2387037998.0693507</v>
       </c>
       <c r="E65">
-        <v>449430193.61059439</v>
+        <v>454876547.31497413</v>
       </c>
       <c r="F65">
-        <v>1101.2007859518244</v>
+        <v>1126.2651989448809</v>
       </c>
       <c r="H65">
-        <v>212.05258853360169</v>
+        <v>214.62231664155337</v>
       </c>
       <c r="I65" t="s">
         <v>26</v>
@@ -2966,22 +2966,22 @@
         <v>4495381</v>
       </c>
       <c r="C66">
-        <v>8629310069.9598694</v>
+        <v>8498466398.8455076</v>
       </c>
       <c r="D66">
-        <v>464489.58591147873</v>
+        <v>455150.65394512261</v>
       </c>
       <c r="E66">
-        <v>15374952.875029996</v>
+        <v>14942248.839058546</v>
       </c>
       <c r="F66">
-        <v>1919.5948174270143</v>
+        <v>1890.488570122423</v>
       </c>
       <c r="G66">
-        <v>0.10332596634444972</v>
+        <v>0.1012485157420745</v>
       </c>
       <c r="H66">
-        <v>3.4201668056678614</v>
+        <v>3.3239115525599603</v>
       </c>
       <c r="I66" t="s">
         <v>26</v>
@@ -3042,16 +3042,16 @@
         <v>6594728</v>
       </c>
       <c r="C68">
-        <v>6909665163.4713612</v>
+        <v>6853213794.7086449</v>
       </c>
       <c r="E68">
-        <v>1154267398.9358191</v>
+        <v>1165054944.7202663</v>
       </c>
       <c r="F68">
-        <v>1047.7558988742767</v>
+        <v>1039.1958234985043</v>
       </c>
       <c r="H68">
-        <v>175.02881073121122</v>
+        <v>176.66459400907306</v>
       </c>
       <c r="I68" t="s">
         <v>26</v>
@@ -3077,16 +3077,16 @@
         <v>7672769</v>
       </c>
       <c r="C69">
-        <v>7994873401.2145519</v>
+        <v>8027033799.419981</v>
       </c>
       <c r="E69">
-        <v>1426530969.1666131</v>
+        <v>1433370570.4947736</v>
       </c>
       <c r="F69">
-        <v>1041.9802031332563</v>
+        <v>1046.1717014313842</v>
       </c>
       <c r="H69">
-        <v>185.92127159915975</v>
+        <v>186.8126839860256</v>
       </c>
       <c r="I69" t="s">
         <v>26</v>
@@ -3112,16 +3112,16 @@
         <v>306727</v>
       </c>
       <c r="C70">
-        <v>148424605.75192791</v>
+        <v>148460082.78541085</v>
       </c>
       <c r="E70">
-        <v>137007328.38639498</v>
+        <v>137040076.41730234</v>
       </c>
       <c r="F70">
-        <v>483.89807793877912</v>
+        <v>484.0137411620459</v>
       </c>
       <c r="H70">
-        <v>446.67514886656534</v>
+        <v>446.78191491881165</v>
       </c>
       <c r="I70" t="s">
         <v>10</v>
@@ -3147,16 +3147,16 @@
         <v>3095082</v>
       </c>
       <c r="C71">
-        <v>3544641959.9051905</v>
+        <v>3620155522.1083002</v>
       </c>
       <c r="E71">
-        <v>737404902.68164706</v>
+        <v>740855393.14294648</v>
       </c>
       <c r="F71">
-        <v>1145.2497736425694</v>
+        <v>1169.6476933755876</v>
       </c>
       <c r="H71">
-        <v>238.2505221773275</v>
+        <v>239.36535224040796</v>
       </c>
       <c r="I71" t="s">
         <v>10</v>
@@ -3182,22 +3182,22 @@
         <v>134547</v>
       </c>
       <c r="C72">
-        <v>730501907.89701748</v>
+        <v>734105918.78363085</v>
       </c>
       <c r="D72">
-        <v>39763.544122286716</v>
+        <v>40201.684324322523</v>
       </c>
       <c r="E72">
-        <v>783767.0170886534</v>
+        <v>850028.29028394958</v>
       </c>
       <c r="F72">
-        <v>5429.3437081244283</v>
+        <v>5456.1299678449232</v>
       </c>
       <c r="G72">
-        <v>0.29553646028738445</v>
+        <v>0.29879287033023794</v>
       </c>
       <c r="H72">
-        <v>5.8252284858722483</v>
+        <v>6.3177052649553653</v>
       </c>
       <c r="I72" t="s">
         <v>27</v>
@@ -3223,22 +3223,22 @@
         <v>531521</v>
       </c>
       <c r="C73">
-        <v>3107929882.4681911</v>
+        <v>3090617833.4185128</v>
       </c>
       <c r="D73">
-        <v>165361.28319528868</v>
+        <v>167427.12120602158</v>
       </c>
       <c r="E73">
-        <v>5396303.956573749</v>
+        <v>5440037.6823242381</v>
       </c>
       <c r="F73">
-        <v>5847.2381758541824</v>
+        <v>5814.6674043330604</v>
       </c>
       <c r="G73">
-        <v>0.31110959528464288</v>
+        <v>0.31499624888954825</v>
       </c>
       <c r="H73">
-        <v>10.152569619213068</v>
+        <v>10.234849953857399</v>
       </c>
       <c r="I73" t="s">
         <v>28</v>
@@ -3264,22 +3264,22 @@
         <v>1438500</v>
       </c>
       <c r="C74">
-        <v>9691444192.5479088</v>
+        <v>9487808336.2581596</v>
       </c>
       <c r="D74">
-        <v>522492.71715450345</v>
+        <v>514924.05627434654</v>
       </c>
       <c r="E74">
-        <v>17476024.651721567</v>
+        <v>17651246.005232722</v>
       </c>
       <c r="F74">
-        <v>6737.1874817851294</v>
+        <v>6595.6262330609388</v>
       </c>
       <c r="G74">
-        <v>0.363220519398334</v>
+        <v>0.35795902417403302</v>
       </c>
       <c r="H74">
-        <v>12.14878321287561</v>
+        <v>12.270591592097826</v>
       </c>
       <c r="I74" t="s">
         <v>29</v>
@@ -3305,22 +3305,22 @@
         <v>4871389</v>
       </c>
       <c r="C75">
-        <v>24968555821.711536</v>
+        <v>24565420776.181534</v>
       </c>
       <c r="D75">
-        <v>1336146.3063091377</v>
+        <v>1311959.4437370128</v>
       </c>
       <c r="E75">
-        <v>43283172.872251511</v>
+        <v>44147585.836821184</v>
       </c>
       <c r="F75">
-        <v>5125.5516284393507</v>
+        <v>5042.795961517656</v>
       </c>
       <c r="G75">
-        <v>0.2742844610252102</v>
+        <v>0.26931937559020902</v>
       </c>
       <c r="H75">
-        <v>8.8851809765657208</v>
+        <v>9.0626278945945771</v>
       </c>
       <c r="I75" t="s">
         <v>29</v>
@@ -3346,22 +3346,22 @@
         <v>1656996</v>
       </c>
       <c r="C76">
-        <v>8661643337.6331825</v>
+        <v>8644975135.1264191</v>
       </c>
       <c r="D76">
-        <v>469276.46910951554</v>
+        <v>466722.13124276488</v>
       </c>
       <c r="E76">
-        <v>17692197.096368648</v>
+        <v>17458157.455905475</v>
       </c>
       <c r="F76">
-        <v>5227.3169866633252</v>
+        <v>5217.2576971377221</v>
       </c>
       <c r="G76">
-        <v>0.28320917437912679</v>
+        <v>0.28166762698447367</v>
       </c>
       <c r="H76">
-        <v>10.677272061229267</v>
+        <v>10.536028726626663</v>
       </c>
       <c r="I76" t="s">
         <v>29</v>
@@ -3387,22 +3387,22 @@
         <v>967351</v>
       </c>
       <c r="C77">
-        <v>6540344287.2977095</v>
+        <v>6558933080.8941069</v>
       </c>
       <c r="D77">
-        <v>348876.10298312013</v>
+        <v>351611.49830091372</v>
       </c>
       <c r="E77">
-        <v>3764836.7824022206</v>
+        <v>4080397.1592935342</v>
       </c>
       <c r="F77">
-        <v>6761.0870173263993</v>
+        <v>6780.3032000733001</v>
       </c>
       <c r="G77">
-        <v>0.36065099739713935</v>
+        <v>0.36347871486245809</v>
       </c>
       <c r="H77">
-        <v>3.8919035411161209</v>
+        <v>4.2181143755405586</v>
       </c>
       <c r="I77" t="s">
         <v>29</v>
@@ -3428,22 +3428,22 @@
         <v>7658910</v>
       </c>
       <c r="C78">
-        <v>34849090934.366158</v>
+        <v>34544595359.319397</v>
       </c>
       <c r="D78">
-        <v>1888991.2783132931</v>
+        <v>1875371.0734675978</v>
       </c>
       <c r="E78">
-        <v>71587525.360736728</v>
+        <v>71281092.829448938</v>
       </c>
       <c r="F78">
-        <v>4550.1371519401791</v>
+        <v>4510.3801140527039</v>
       </c>
       <c r="G78">
-        <v>0.24663970177391994</v>
+        <v>0.24486135409184834</v>
       </c>
       <c r="H78">
-        <v>9.3469599930978085</v>
+        <v>9.306950052872919</v>
       </c>
       <c r="I78" t="s">
         <v>29</v>
@@ -3469,16 +3469,16 @@
         <v>500630</v>
       </c>
       <c r="C79">
-        <v>2668830887.3280163</v>
+        <v>2635422020.5322065</v>
       </c>
       <c r="E79">
-        <v>370830652.42778182</v>
+        <v>365982394.75107121</v>
       </c>
       <c r="F79">
-        <v>5330.9447842279051</v>
+        <v>5264.2111350342702</v>
       </c>
       <c r="H79">
-        <v>740.72798759119871</v>
+        <v>731.04367447230732</v>
       </c>
       <c r="I79" t="s">
         <v>30</v>
@@ -3504,22 +3504,22 @@
         <v>3581670</v>
       </c>
       <c r="C80">
-        <v>20541106322.99263</v>
+        <v>20654862044.130875</v>
       </c>
       <c r="D80">
-        <v>1066678.151772955</v>
+        <v>1088947.4190375598</v>
       </c>
       <c r="E80">
-        <v>33227543.3549079</v>
+        <v>34228093.86286816</v>
       </c>
       <c r="F80">
-        <v>5735.0639011948697</v>
+        <v>5766.8244266308393</v>
       </c>
       <c r="G80">
-        <v>0.29781586571988899</v>
+        <v>0.30403343106359876</v>
       </c>
       <c r="H80">
-        <v>9.2771091013152809</v>
+        <v>9.5564621706824369</v>
       </c>
       <c r="I80" t="s">
         <v>30</v>
@@ -3586,22 +3586,22 @@
         <v>6114392</v>
       </c>
       <c r="C82">
-        <v>31804742952.707085</v>
+        <v>31635494237.889412</v>
       </c>
       <c r="D82">
-        <v>1737884.2536454792</v>
+        <v>1721292.5851834579</v>
       </c>
       <c r="E82">
-        <v>61643092.555606171</v>
+        <v>60693204.517227612</v>
       </c>
       <c r="F82">
-        <v>5201.6198753215504</v>
+        <v>5173.9394919215865</v>
       </c>
       <c r="G82">
-        <v>0.28422846517617439</v>
+        <v>0.28151492170987041</v>
       </c>
       <c r="H82">
-        <v>10.081638952099599</v>
+        <v>9.9262861323296931</v>
       </c>
       <c r="I82" t="s">
         <v>31</v>
@@ -3627,22 +3627,22 @@
         <v>6233147</v>
       </c>
       <c r="C83">
-        <v>26416304118.477699</v>
+        <v>26367415818.41082</v>
       </c>
       <c r="D83">
-        <v>1426544.7793504712</v>
+        <v>1428098.6672663814</v>
       </c>
       <c r="E83">
-        <v>53012647.248738773</v>
+        <v>52680920.29199706</v>
       </c>
       <c r="F83">
-        <v>4238.0364394546923</v>
+        <v>4230.19316220375</v>
       </c>
       <c r="G83">
-        <v>0.22886429268401198</v>
+        <v>0.22911358696760745</v>
       </c>
       <c r="H83">
-        <v>8.5049570062664621</v>
+        <v>8.4517371870095577</v>
       </c>
       <c r="I83" t="s">
         <v>31</v>
@@ -3668,16 +3668,16 @@
         <v>2753681</v>
       </c>
       <c r="C84">
-        <v>11313711287.944427</v>
+        <v>11437396970.378136</v>
       </c>
       <c r="E84">
-        <v>1324106101.3839788</v>
+        <v>1300314039.863884</v>
       </c>
       <c r="F84">
-        <v>4108.5773144908317</v>
+        <v>4153.4938035226796</v>
       </c>
       <c r="H84">
-        <v>480.84948887833372</v>
+        <v>472.20939530173752</v>
       </c>
       <c r="I84" t="s">
         <v>31</v>
@@ -3703,22 +3703,22 @@
         <v>5168266</v>
       </c>
       <c r="C85">
-        <v>17677907394.639282</v>
+        <v>17881642194.368938</v>
       </c>
       <c r="D85">
-        <v>937740.26356720435</v>
+        <v>944491.10491384612</v>
       </c>
       <c r="E85">
-        <v>30556455.983138844</v>
+        <v>31176434.861021161</v>
       </c>
       <c r="F85">
-        <v>3420.4716619924911</v>
+        <v>3459.8920013731758</v>
       </c>
       <c r="G85">
-        <v>0.18144195046601788</v>
+        <v>0.18274816058497106</v>
       </c>
       <c r="H85">
-        <v>5.9123226209987729</v>
+        <v>6.0322813998004676</v>
       </c>
       <c r="I85" t="s">
         <v>31</v>
@@ -3744,22 +3744,22 @@
         <v>9849064</v>
       </c>
       <c r="C86">
-        <v>52147585006.132858</v>
+        <v>52822821282.466522</v>
       </c>
       <c r="D86">
-        <v>2805859.0563013176</v>
+        <v>2847115.6997426669</v>
       </c>
       <c r="E86">
-        <v>99807490.715359315</v>
+        <v>100631847.85891131</v>
       </c>
       <c r="F86">
-        <v>5294.6741950435953</v>
+        <v>5363.2326160604216</v>
       </c>
       <c r="G86">
-        <v>0.28488585882895245</v>
+        <v>0.28907474859973159</v>
       </c>
       <c r="H86">
-        <v>10.13370313314639</v>
+        <v>10.217402167242625</v>
       </c>
       <c r="I86" t="s">
         <v>31</v>
@@ -3785,22 +3785,22 @@
         <v>6246911</v>
       </c>
       <c r="C87">
-        <v>30035589163.120358</v>
+        <v>30425784094.951523</v>
       </c>
       <c r="D87">
-        <v>1618800.6104301754</v>
+        <v>1633182.2256828856</v>
       </c>
       <c r="E87">
-        <v>58132267.983666748</v>
+        <v>60063231.836836092</v>
       </c>
       <c r="F87">
-        <v>4808.0706069160187</v>
+        <v>4870.5326672577094</v>
       </c>
       <c r="G87">
-        <v>0.25913617313103632</v>
+        <v>0.26143836940895837</v>
       </c>
       <c r="H87">
-        <v>9.3057621572752911</v>
+        <v>9.6148691468208991</v>
       </c>
       <c r="I87" t="s">
         <v>31</v>
@@ -3826,22 +3826,22 @@
         <v>3681044</v>
       </c>
       <c r="C88">
-        <v>16287921286.987217</v>
+        <v>16472738806.95776</v>
       </c>
       <c r="D88">
-        <v>836792.50013261382</v>
+        <v>835927.16664469312</v>
       </c>
       <c r="E88">
-        <v>30393162.598968979</v>
+        <v>30604512.125774756</v>
       </c>
       <c r="F88">
-        <v>4424.810267681456</v>
+        <v>4475.018176082046</v>
       </c>
       <c r="G88">
-        <v>0.22732477529000303</v>
+        <v>0.22708969701114501</v>
       </c>
       <c r="H88">
-        <v>8.2566691946548261</v>
+        <v>8.3140848427171079</v>
       </c>
       <c r="I88" t="s">
         <v>31</v>
@@ -3867,16 +3867,16 @@
         <v>4626240</v>
       </c>
       <c r="C89">
-        <v>4949916620.7859049</v>
+        <v>4870474390.8155861</v>
       </c>
       <c r="E89">
-        <v>933845451.84661663</v>
+        <v>895335631.5217967</v>
       </c>
       <c r="F89">
-        <v>1069.9653759394032</v>
+        <v>1052.7932815451827</v>
       </c>
       <c r="H89">
-        <v>201.85841025251966</v>
+        <v>193.53419440448329</v>
       </c>
       <c r="I89" t="s">
         <v>14</v>
@@ -3902,16 +3902,16 @@
         <v>6322841</v>
       </c>
       <c r="C90">
-        <v>7046098602.0218496</v>
+        <v>6836220987.3682289</v>
       </c>
       <c r="E90">
-        <v>1197294607.089335</v>
+        <v>1147106954.2016745</v>
       </c>
       <c r="F90">
-        <v>1114.3880736557901</v>
+        <v>1081.1945116709765</v>
       </c>
       <c r="H90">
-        <v>189.36022700702659</v>
+        <v>181.42271080384188</v>
       </c>
       <c r="I90" t="s">
         <v>14</v>
@@ -3937,16 +3937,16 @@
         <v>9036684</v>
       </c>
       <c r="C91">
-        <v>82053892780.295288</v>
+        <v>82303537815.805603</v>
       </c>
       <c r="E91">
-        <v>8526226965.1197357</v>
+        <v>8527263608.4027729</v>
       </c>
       <c r="F91">
-        <v>9080.0887560409647</v>
+        <v>9107.7144908249102</v>
       </c>
       <c r="H91">
-        <v>943.51279353352788</v>
+        <v>943.62750854215699</v>
       </c>
       <c r="I91" t="s">
         <v>32</v>
@@ -3972,16 +3972,16 @@
         <v>916991</v>
       </c>
       <c r="C92">
-        <v>8697526307.6366558</v>
+        <v>8495972103.3315926</v>
       </c>
       <c r="E92">
-        <v>1644030181.9432619</v>
+        <v>1631884722.8534508</v>
       </c>
       <c r="F92">
-        <v>9484.8546034112187</v>
+        <v>9265.0550586991503</v>
       </c>
       <c r="H92">
-        <v>1792.8531271771062</v>
+        <v>1779.60822173113</v>
       </c>
       <c r="I92" t="s">
         <v>32</v>
@@ -4007,16 +4007,16 @@
         <v>317344</v>
       </c>
       <c r="C93">
-        <v>2106556398.5663023</v>
+        <v>2100449710.859055</v>
       </c>
       <c r="E93">
-        <v>391220611.58720756</v>
+        <v>399203579.01554155</v>
       </c>
       <c r="F93">
-        <v>6638.0848497728093</v>
+        <v>6618.8417328169271</v>
       </c>
       <c r="H93">
-        <v>1232.7966231824375</v>
+        <v>1257.9521875804853</v>
       </c>
       <c r="I93" t="s">
         <v>32</v>
@@ -4042,22 +4042,22 @@
         <v>4078252</v>
       </c>
       <c r="C94">
-        <v>22592578151.843788</v>
+        <v>22612142938.095116</v>
       </c>
       <c r="D94">
-        <v>1206607.2842896339</v>
+        <v>1198858.1543142733</v>
       </c>
       <c r="E94">
-        <v>40032645.159782432</v>
+        <v>40088073.491488911</v>
       </c>
       <c r="F94">
-        <v>5539.7700171161041</v>
+        <v>5544.567363197546</v>
       </c>
       <c r="G94">
-        <v>0.29586383683245515</v>
+        <v>0.29396372620286171</v>
       </c>
       <c r="H94">
-        <v>9.8161283706309543</v>
+        <v>9.8297195689449577</v>
       </c>
       <c r="I94" t="s">
         <v>32</v>
@@ -4083,22 +4083,22 @@
         <v>3399679</v>
       </c>
       <c r="C95">
-        <v>17672031822.874939</v>
+        <v>17557633161.803688</v>
       </c>
       <c r="D95">
-        <v>963242.49503951147</v>
+        <v>974670.54434581241</v>
       </c>
       <c r="E95">
-        <v>11544132.300828867</v>
+        <v>14490718.853361756</v>
       </c>
       <c r="F95">
-        <v>5198.1471847415414</v>
+        <v>5164.4973427796231</v>
       </c>
       <c r="G95">
-        <v>0.28333336619119376</v>
+        <v>0.28669487452956954</v>
       </c>
       <c r="H95">
-        <v>3.3956536193060778</v>
+        <v>4.2623785520226338</v>
       </c>
       <c r="I95" t="s">
         <v>32</v>
@@ -4124,22 +4124,22 @@
         <v>3734928</v>
       </c>
       <c r="C96">
-        <v>18566869048.173409</v>
+        <v>18309168793.659142</v>
       </c>
       <c r="D96">
-        <v>983628.19174977986</v>
+        <v>974071.61647393787</v>
       </c>
       <c r="E96">
-        <v>15460596.442555193</v>
+        <v>11709695.200701537</v>
       </c>
       <c r="F96">
-        <v>4971.1451059226338</v>
+        <v>4902.1477237738291</v>
       </c>
       <c r="G96">
-        <v>0.26335934501274988</v>
+        <v>0.26080064099600786</v>
       </c>
       <c r="H96">
-        <v>4.1394630478968253</v>
+        <v>3.1351863277422045</v>
       </c>
       <c r="I96" t="s">
         <v>12</v>
@@ -4165,13 +4165,13 @@
         <v>984434</v>
       </c>
       <c r="C97">
-        <v>1134412525.4587009</v>
+        <v>1129935685.3088884</v>
       </c>
       <c r="E97">
         <v>122446922.6044364</v>
       </c>
       <c r="F97">
-        <v>1152.3500056465957</v>
+        <v>1147.8023771109981</v>
       </c>
       <c r="H97">
         <v>124.38306946370848</v>
@@ -4200,22 +4200,22 @@
         <v>3857821</v>
       </c>
       <c r="C98">
-        <v>20604730624.334023</v>
+        <v>20217226472.667526</v>
       </c>
       <c r="D98">
-        <v>1115774.4754967894</v>
+        <v>1096273.3649266246</v>
       </c>
       <c r="E98">
-        <v>41278226.796595536</v>
+        <v>40424673.655641302</v>
       </c>
       <c r="F98">
-        <v>5341.0281670233071</v>
+        <v>5240.5817876639494</v>
       </c>
       <c r="G98">
-        <v>0.28922401415119814</v>
+        <v>0.28416905940597675</v>
       </c>
       <c r="H98">
-        <v>10.699881305170855</v>
+        <v>10.478628649603312</v>
       </c>
       <c r="I98" t="s">
         <v>33</v>
@@ -4244,13 +4244,13 @@
         <v>1254194545.9763114</v>
       </c>
       <c r="E99">
-        <v>209290795.14918676</v>
+        <v>207983417.62787086</v>
       </c>
       <c r="F99">
         <v>3190.1658068705397</v>
       </c>
       <c r="H99">
-        <v>532.35149245362197</v>
+        <v>529.02605057655944</v>
       </c>
       <c r="I99" t="s">
         <v>34</v>
@@ -4276,22 +4276,22 @@
         <v>2485399</v>
       </c>
       <c r="C100">
-        <v>14463873644.275688</v>
+        <v>14574004943.308626</v>
       </c>
       <c r="D100">
-        <v>767620.42082623322</v>
+        <v>780913.01797771908</v>
       </c>
       <c r="E100">
-        <v>21599762.548174575</v>
+        <v>21639918.820788123</v>
       </c>
       <c r="F100">
-        <v>5819.5378867842501</v>
+        <v>5863.8492022040027</v>
       </c>
       <c r="G100">
-        <v>0.30885198747816073</v>
+        <v>0.3142002624036298</v>
       </c>
       <c r="H100">
-        <v>8.6906619613891287</v>
+        <v>8.7068188330276648</v>
       </c>
       <c r="I100" t="s">
         <v>34</v>
@@ -4317,16 +4317,16 @@
         <v>261201</v>
       </c>
       <c r="C101">
-        <v>454117091.57326138</v>
+        <v>451267294.77967322</v>
       </c>
       <c r="E101">
-        <v>75058957.551032722</v>
+        <v>73692767.079367891</v>
       </c>
       <c r="F101">
-        <v>1738.5733269522757</v>
+        <v>1727.6629675218442</v>
       </c>
       <c r="H101">
-        <v>287.36091190704752</v>
+        <v>282.13049367869149</v>
       </c>
       <c r="I101" t="s">
         <v>34</v>
@@ -4352,22 +4352,22 @@
         <v>14072154</v>
       </c>
       <c r="C102">
-        <v>58529872610.941666</v>
+        <v>59251372717.045059</v>
       </c>
       <c r="D102">
-        <v>3133817.9168014778</v>
+        <v>3176413.4940072023</v>
       </c>
       <c r="E102">
-        <v>113468467.01397368</v>
+        <v>112274104.13882339</v>
       </c>
       <c r="F102">
-        <v>4159.2689087215549</v>
+        <v>4210.5403847232665</v>
       </c>
       <c r="G102">
-        <v>0.22269639152623527</v>
+        <v>0.22572333233470881</v>
       </c>
       <c r="H102">
-        <v>8.0633332334178327</v>
+        <v>7.9784590290031918</v>
       </c>
       <c r="I102" t="s">
         <v>35</v>
@@ -4393,16 +4393,16 @@
         <v>543145</v>
       </c>
       <c r="C103">
-        <v>937225645.65279019</v>
+        <v>909637100.43715906</v>
       </c>
       <c r="E103">
-        <v>131314692.5835264</v>
+        <v>131479841.05870774</v>
       </c>
       <c r="F103">
-        <v>1725.5532972830279</v>
+        <v>1674.7592271624687</v>
       </c>
       <c r="H103">
-        <v>241.76728605349658</v>
+        <v>242.07134569720375</v>
       </c>
       <c r="I103" t="s">
         <v>35</v>
@@ -4428,22 +4428,22 @@
         <v>7296430</v>
       </c>
       <c r="C104">
-        <v>31947411078.619793</v>
+        <v>31840794115.400566</v>
       </c>
       <c r="D104">
-        <v>1729024.8770000853</v>
+        <v>1720049.0081303755</v>
       </c>
       <c r="E104">
-        <v>64449170.917796329</v>
+        <v>63579559.958945036</v>
       </c>
       <c r="F104">
-        <v>4378.4989479265605</v>
+        <v>4363.8867385009607</v>
       </c>
       <c r="G104">
-        <v>0.23696861026557992</v>
+        <v>0.23573843758254043</v>
       </c>
       <c r="H104">
-        <v>8.8329732372949969</v>
+        <v>8.7137901629899872</v>
       </c>
       <c r="I104" t="s">
         <v>35</v>
@@ -4469,19 +4469,19 @@
         <v>11269955</v>
       </c>
       <c r="C105">
-        <v>50127538350.192825</v>
+        <v>23674031314.164902</v>
       </c>
       <c r="D105">
-        <v>2178275.7067344799</v>
+        <v>1532914.8212880685</v>
       </c>
       <c r="E105">
         <v>62233078.422057107</v>
       </c>
       <c r="F105">
-        <v>4447.8916153784839</v>
+        <v>2100.6322841719334</v>
       </c>
       <c r="G105">
-        <v>0.19328166853678475</v>
+        <v>0.13601782982168684</v>
       </c>
       <c r="H105">
         <v>5.5220343312867808</v>
@@ -4510,22 +4510,22 @@
         <v>5367819</v>
       </c>
       <c r="C106">
-        <v>21935904065.080479</v>
+        <v>21367290039.988956</v>
       </c>
       <c r="D106">
-        <v>1176980.4356601038</v>
+        <v>1152157.4797304422</v>
       </c>
       <c r="E106">
-        <v>41980091.909992188</v>
+        <v>40347212.674162969</v>
       </c>
       <c r="F106">
-        <v>4086.5580722972363</v>
+        <v>3980.6278937477132</v>
       </c>
       <c r="G106">
-        <v>0.21926604374329756</v>
+        <v>0.21464164118246948</v>
       </c>
       <c r="H106">
-        <v>7.8206981103483901</v>
+        <v>7.5165002162261754</v>
       </c>
       <c r="I106" t="s">
         <v>35</v>
@@ -4551,22 +4551,22 @@
         <v>9846148</v>
       </c>
       <c r="C107">
-        <v>65651413371.848007</v>
+        <v>64751543928.953117</v>
       </c>
       <c r="D107">
-        <v>3507487.5595305767</v>
+        <v>3471704.768468041</v>
       </c>
       <c r="E107">
-        <v>127926502.44336167</v>
+        <v>125064165.26713824</v>
       </c>
       <c r="F107">
-        <v>6667.7256295404059</v>
+        <v>6576.3325849817738</v>
       </c>
       <c r="G107">
-        <v>0.35622941677604036</v>
+        <v>0.35259522490095019</v>
       </c>
       <c r="H107">
-        <v>12.992543118726397</v>
+        <v>12.701836826659344</v>
       </c>
       <c r="I107" t="s">
         <v>35</v>
@@ -4592,22 +4592,22 @@
         <v>5178344</v>
       </c>
       <c r="C108">
-        <v>6055109133.3037968</v>
+        <v>6168763447.6665649</v>
       </c>
       <c r="D108">
-        <v>348199.9087503886</v>
+        <v>359752.9139138445</v>
       </c>
       <c r="E108">
-        <v>12373195.861787563</v>
+        <v>12882517.553766755</v>
       </c>
       <c r="F108">
-        <v>1169.3138063643121</v>
+        <v>1191.2618102749768</v>
       </c>
       <c r="G108">
-        <v>6.7241556132691963E-2</v>
+        <v>6.9472579248084809E-2</v>
       </c>
       <c r="H108">
-        <v>2.3894117234752197</v>
+        <v>2.4877678180064429</v>
       </c>
       <c r="I108" t="s">
         <v>36</v>
@@ -4633,16 +4633,16 @@
         <v>3896653</v>
       </c>
       <c r="C109">
-        <v>4115947643.7327304</v>
+        <v>4202198108.4142833</v>
       </c>
       <c r="E109">
-        <v>727108354.96352363</v>
+        <v>727895999.88177586</v>
       </c>
       <c r="F109">
-        <v>1056.2776936341857</v>
+        <v>1078.4121933398442</v>
       </c>
       <c r="H109">
-        <v>186.59817924858172</v>
+        <v>186.80031295621546</v>
       </c>
       <c r="I109" t="s">
         <v>36</v>
@@ -4668,16 +4668,16 @@
         <v>12685</v>
       </c>
       <c r="C110">
-        <v>11733040.498061748</v>
+        <v>11969413.938737301</v>
       </c>
       <c r="E110">
-        <v>1470616.4980982819</v>
+        <v>1440640.9737680266</v>
       </c>
       <c r="F110">
-        <v>924.95392180226634</v>
+        <v>943.5880125137802</v>
       </c>
       <c r="H110">
-        <v>115.93350398882789</v>
+        <v>113.57043545668321</v>
       </c>
       <c r="I110" t="s">
         <v>36</v>
@@ -4703,16 +4703,16 @@
         <v>1522254</v>
       </c>
       <c r="C111">
-        <v>2075061360.1643276</v>
+        <v>2102852360.5236712</v>
       </c>
       <c r="E111">
-        <v>362384467.00754398</v>
+        <v>369529530.52269113</v>
       </c>
       <c r="F111">
-        <v>1363.1505387171442</v>
+        <v>1381.4070191463916</v>
       </c>
       <c r="H111">
-        <v>238.05781887092692</v>
+        <v>242.75155823055229</v>
       </c>
       <c r="I111" t="s">
         <v>37</v>
@@ -4741,13 +4741,13 @@
         <v>2382796238.1820059</v>
       </c>
       <c r="E112">
-        <v>268469331.11990654</v>
+        <v>272516722.56718874</v>
       </c>
       <c r="F112">
         <v>486.35234110645246</v>
       </c>
       <c r="H112">
-        <v>54.7972527458206</v>
+        <v>55.623365475989168</v>
       </c>
       <c r="I112" t="s">
         <v>37</v>
@@ -4773,22 +4773,22 @@
         <v>214384</v>
       </c>
       <c r="C113">
-        <v>1765599070.0349221</v>
+        <v>1768172297.0904531</v>
       </c>
       <c r="D113">
-        <v>95923.073900619842</v>
+        <v>95329.298664062691</v>
       </c>
       <c r="E113">
-        <v>1160864.9603071313</v>
+        <v>1124980.9661242373</v>
       </c>
       <c r="F113">
-        <v>8235.6848926921884</v>
+        <v>8247.6877802935524</v>
       </c>
       <c r="G113">
-        <v>0.44743578765495484</v>
+        <v>0.44466610691125591</v>
       </c>
       <c r="H113">
-        <v>5.4148861869688565</v>
+        <v>5.2475043199316991</v>
       </c>
       <c r="I113" t="s">
         <v>23</v>
@@ -4814,22 +4814,22 @@
         <v>17815891</v>
       </c>
       <c r="C114">
-        <v>20808754147.598839</v>
+        <v>20791303397.678978</v>
       </c>
       <c r="D114">
-        <v>1115154.4318327329</v>
+        <v>1115229.7306077764</v>
       </c>
       <c r="E114">
-        <v>39873786.184496999</v>
+        <v>40619606.970262103</v>
       </c>
       <c r="F114">
-        <v>1167.9884069563986</v>
+        <v>1167.0089022030377</v>
       </c>
       <c r="G114">
-        <v>6.2593245088484933E-2</v>
+        <v>6.2597471583530476E-2</v>
       </c>
       <c r="H114">
-        <v>2.2381022753505282</v>
+        <v>2.2799649464773948</v>
       </c>
       <c r="I114" t="s">
         <v>9</v>
@@ -4855,22 +4855,22 @@
         <v>7047532</v>
       </c>
       <c r="C115">
-        <v>31551248931.637199</v>
+        <v>31276630382.081257</v>
       </c>
       <c r="D115">
-        <v>1675447.7263068666</v>
+        <v>1670980.4498084495</v>
       </c>
       <c r="E115">
-        <v>55117749.678540722</v>
+        <v>54273663.907323487</v>
       </c>
       <c r="F115">
-        <v>4476.9216984949053</v>
+        <v>4437.9550716593067</v>
       </c>
       <c r="G115">
-        <v>0.23773538400490649</v>
+        <v>0.23710150586169026</v>
       </c>
       <c r="H115">
-        <v>7.8208583768815414</v>
+        <v>7.701087970558131</v>
       </c>
       <c r="I115" t="s">
         <v>35</v>
@@ -4896,16 +4896,16 @@
         <v>6223129</v>
       </c>
       <c r="C116">
-        <v>6797579904.0951548</v>
+        <v>6978667731.8964291</v>
       </c>
       <c r="E116">
-        <v>1169762237.3230693</v>
+        <v>1207116314.7636905</v>
       </c>
       <c r="F116">
-        <v>1092.3090143391137</v>
+        <v>1121.408174552774</v>
       </c>
       <c r="H116">
-        <v>187.97010914012378</v>
+        <v>193.9725682632789</v>
       </c>
       <c r="I116" t="s">
         <v>38</v>
@@ -4931,22 +4931,22 @@
         <v>2129192</v>
       </c>
       <c r="C117">
-        <v>2570897507.5027194</v>
+        <v>2546611132.2940063</v>
       </c>
       <c r="D117">
-        <v>156061.68130127474</v>
+        <v>156010.79083798052</v>
       </c>
       <c r="E117">
-        <v>3516939.1267356579</v>
+        <v>3539397.2309932294</v>
       </c>
       <c r="F117">
-        <v>1207.452173173072</v>
+        <v>1196.04579215684</v>
       </c>
       <c r="G117">
-        <v>7.3296199356974262E-2</v>
+        <v>7.3272298053900495E-2</v>
       </c>
       <c r="H117">
-        <v>1.6517717175039441</v>
+        <v>1.6623194296208277</v>
       </c>
       <c r="I117" t="s">
         <v>16</v>
@@ -4972,16 +4972,16 @@
         <v>4998069</v>
       </c>
       <c r="C118">
-        <v>4490032254.8848228</v>
+        <v>4445136855.7396097</v>
       </c>
       <c r="E118">
-        <v>769986601.00690114</v>
+        <v>739652487.25537252</v>
       </c>
       <c r="F118">
-        <v>898.35339505813613</v>
+        <v>889.37084616871232</v>
       </c>
       <c r="H118">
-        <v>154.05681694408403</v>
+        <v>147.98765028161327</v>
       </c>
       <c r="I118" t="s">
         <v>16</v>
@@ -5007,22 +5007,22 @@
         <v>5936999</v>
       </c>
       <c r="C119">
-        <v>27891064534.874908</v>
+        <v>28277359765.1633</v>
       </c>
       <c r="D119">
-        <v>1485974.511117442</v>
+        <v>1497208.6164817205</v>
       </c>
       <c r="E119">
-        <v>40836722.113402143</v>
+        <v>15453041.902800141</v>
       </c>
       <c r="F119">
-        <v>4697.8388466757206</v>
+        <v>4762.9045861660579</v>
       </c>
       <c r="G119">
-        <v>0.25029051059591589</v>
+        <v>0.25218273011023257</v>
       </c>
       <c r="H119">
-        <v>6.8783441117982571</v>
+        <v>2.6028372082933044</v>
       </c>
       <c r="I119" t="s">
         <v>31</v>
@@ -5054,7 +5054,7 @@
         <v>2912286.3224935019</v>
       </c>
       <c r="E120">
-        <v>110865184.11362399</v>
+        <v>99687862.924653471</v>
       </c>
       <c r="F120">
         <v>6089.6131676719833</v>
@@ -5063,7 +5063,7 @@
         <v>0.32966171594392746</v>
       </c>
       <c r="H120">
-        <v>12.549592583343351</v>
+        <v>11.284354734182431</v>
       </c>
       <c r="I120" t="s">
         <v>30</v>
@@ -5089,22 +5089,22 @@
         <v>4469578</v>
       </c>
       <c r="C121">
-        <v>11453394610.491039</v>
+        <v>11434825092.026379</v>
       </c>
       <c r="D121">
-        <v>611565.14624633687</v>
+        <v>607056.61007253022</v>
       </c>
       <c r="E121">
-        <v>23434128.247685619</v>
+        <v>22385207.035526067</v>
       </c>
       <c r="F121">
-        <v>2562.5225939654792</v>
+        <v>2558.367947046987</v>
       </c>
       <c r="G121">
-        <v>0.13682838653813331</v>
+        <v>0.13581967024012787</v>
       </c>
       <c r="H121">
-        <v>5.2430292630949991</v>
+        <v>5.0083491183118554</v>
       </c>
       <c r="I121" t="s">
         <v>15</v>
@@ -5133,13 +5133,13 @@
         <v>3088209608.0306726</v>
       </c>
       <c r="E122">
-        <v>380691049.71561331</v>
+        <v>334657775.46218193</v>
       </c>
       <c r="F122">
         <v>1231.1520967754905</v>
       </c>
       <c r="H122">
-        <v>151.76708953376999</v>
+        <v>133.41536820916281</v>
       </c>
       <c r="I122" t="s">
         <v>21</v>
@@ -5165,16 +5165,16 @@
         <v>1204962</v>
       </c>
       <c r="C123">
-        <v>1574810759.4612119</v>
+        <v>1553656924.9392414</v>
       </c>
       <c r="E123">
-        <v>191523037.85176781</v>
+        <v>175264180.07569098</v>
       </c>
       <c r="F123">
-        <v>1306.9381104642403</v>
+        <v>1289.3825074477381</v>
       </c>
       <c r="H123">
-        <v>158.94529275758723</v>
+        <v>145.45203921425818</v>
       </c>
       <c r="I123" t="s">
         <v>19</v>
@@ -5200,22 +5200,22 @@
         <v>11346108</v>
       </c>
       <c r="C124">
-        <v>15535577936.77359</v>
+        <v>15348729524.664711</v>
       </c>
       <c r="D124">
-        <v>900071.43977187364</v>
+        <v>890976.237584944</v>
       </c>
       <c r="E124">
-        <v>32528072.823919203</v>
+        <v>31712610.205231484</v>
       </c>
       <c r="F124">
-        <v>1369.2429101480077</v>
+        <v>1352.7748479623772</v>
       </c>
       <c r="G124">
-        <v>7.9328650826510166E-2</v>
+        <v>7.8527036547241039E-2</v>
       </c>
       <c r="H124">
-        <v>2.8668925788401807</v>
+        <v>2.7950210067832497</v>
       </c>
       <c r="I124" t="s">
         <v>19</v>
@@ -5247,7 +5247,7 @@
         <v>166007.6145713944</v>
       </c>
       <c r="E125">
-        <v>2665551.5215987503</v>
+        <v>2307951.7246571379</v>
       </c>
       <c r="F125">
         <v>5449.6816672136183</v>
@@ -5256,7 +5256,7 @@
         <v>0.269982443117462</v>
       </c>
       <c r="H125">
-        <v>4.3350548341696715</v>
+        <v>3.7534811088567057</v>
       </c>
       <c r="I125" t="s">
         <v>28</v>
@@ -5282,22 +5282,22 @@
         <v>4882435</v>
       </c>
       <c r="C126">
-        <v>14240852840.476206</v>
+        <v>14188397546.644491</v>
       </c>
       <c r="D126">
-        <v>763971.80185561313</v>
+        <v>767496.70050947159</v>
       </c>
       <c r="E126">
-        <v>28335860.302446555</v>
+        <v>28367745.774446502</v>
       </c>
       <c r="F126">
-        <v>2916.7521616726499</v>
+        <v>2906.0084868809295</v>
       </c>
       <c r="G126">
-        <v>0.15647352230098571</v>
+        <v>0.15719547736108552</v>
       </c>
       <c r="H126">
-        <v>5.8036328804063047</v>
+        <v>5.8101635299694729</v>
       </c>
       <c r="I126" t="s">
         <v>17</v>
@@ -5323,22 +5323,22 @@
         <v>4906656</v>
       </c>
       <c r="C127">
-        <v>21551796642.652214</v>
+        <v>21510143179.794708</v>
       </c>
       <c r="D127">
-        <v>1144457.0986090377</v>
+        <v>1151022.4960646876</v>
       </c>
       <c r="E127">
-        <v>24473176.201482914</v>
+        <v>26938271.25323401</v>
       </c>
       <c r="F127">
-        <v>4392.3594078435935</v>
+        <v>4383.8702325564927</v>
       </c>
       <c r="G127">
-        <v>0.23324583965312373</v>
+        <v>0.23458389910861643</v>
       </c>
       <c r="H127">
-        <v>4.9877505579121335</v>
+        <v>5.4901487394335389</v>
       </c>
       <c r="I127" t="s">
         <v>32</v>
@@ -5364,16 +5364,16 @@
         <v>5621453</v>
       </c>
       <c r="C128">
-        <v>5452563338.0343895</v>
+        <v>5501660764.7951031</v>
       </c>
       <c r="E128">
-        <v>1013325142.858845</v>
+        <v>981248422.79496741</v>
       </c>
       <c r="F128">
-        <v>969.95622627003911</v>
+        <v>978.69016512191843</v>
       </c>
       <c r="H128">
-        <v>180.26036024117695</v>
+        <v>174.5542340734624</v>
       </c>
       <c r="I128" t="s">
         <v>14</v>
@@ -5399,16 +5399,16 @@
         <v>4776449</v>
       </c>
       <c r="C129">
-        <v>5305072294.2163801</v>
+        <v>5410995948.0123682</v>
       </c>
       <c r="E129">
-        <v>653969061.96089768</v>
+        <v>622013137.04520023</v>
       </c>
       <c r="F129">
-        <v>1110.6728647613279</v>
+        <v>1132.8490994067702</v>
       </c>
       <c r="H129">
-        <v>136.9153239071322</v>
+        <v>130.22501382202557</v>
       </c>
       <c r="I129" t="s">
         <v>10</v>
@@ -5434,16 +5434,16 @@
         <v>2383346</v>
       </c>
       <c r="C130">
-        <v>2611246893.4207964</v>
+        <v>2600941881.2041764</v>
       </c>
       <c r="E130">
-        <v>320624381.33412009</v>
+        <v>274537723.73895293</v>
       </c>
       <c r="F130">
-        <v>1095.6222442821129</v>
+        <v>1091.2984859118972</v>
       </c>
       <c r="H130">
-        <v>134.52699747922463</v>
+        <v>115.19004111822326</v>
       </c>
       <c r="I130" t="s">
         <v>39</v>
@@ -5469,22 +5469,22 @@
         <v>14585886</v>
       </c>
       <c r="C131">
-        <v>146625212808.10345</v>
+        <v>147534337801.79388</v>
       </c>
       <c r="D131">
-        <v>7766688.5301814042</v>
+        <v>7804160.0061536226</v>
       </c>
       <c r="E131">
-        <v>275914017.59500515</v>
+        <v>276054926.53172398</v>
       </c>
       <c r="F131">
-        <v>10052.54071011548</v>
+        <v>10114.869799599002</v>
       </c>
       <c r="G131">
-        <v>0.5324797225332355</v>
+        <v>0.53504874548955228</v>
       </c>
       <c r="H131">
-        <v>18.9165072039508</v>
+        <v>18.926167840042353</v>
       </c>
       <c r="I131" t="s">
         <v>17</v>
@@ -5510,22 +5510,22 @@
         <v>2184313</v>
       </c>
       <c r="C132">
-        <v>2900844442.3442383</v>
+        <v>2928509049.4982243</v>
       </c>
       <c r="D132">
-        <v>177711.87355975038</v>
+        <v>178608.37987524411</v>
       </c>
       <c r="E132">
-        <v>4006144.9470944591</v>
+        <v>4128938.6619479293</v>
       </c>
       <c r="F132">
-        <v>1328.0351498820171</v>
+        <v>1340.7002794463176</v>
       </c>
       <c r="G132">
-        <v>8.1358245617615413E-2</v>
+        <v>8.1768675036610644E-2</v>
       </c>
       <c r="H132">
-        <v>1.8340526046836965</v>
+        <v>1.8902687764747677</v>
       </c>
       <c r="I132" t="s">
         <v>11</v>
@@ -5551,22 +5551,22 @@
         <v>1131899</v>
       </c>
       <c r="C133">
-        <v>2291179570.7231746</v>
+        <v>2090378378.7495551</v>
       </c>
       <c r="D133">
-        <v>120621.13265553108</v>
+        <v>120178.51792175425</v>
       </c>
       <c r="E133">
-        <v>1990865.5133692876</v>
+        <v>3106625.8735267706</v>
       </c>
       <c r="F133">
-        <v>2024.1908250852546</v>
+        <v>1846.7887848205141</v>
       </c>
       <c r="G133">
-        <v>0.10656527892994966</v>
+        <v>0.10617424162558166</v>
       </c>
       <c r="H133">
-        <v>1.7588720489807728</v>
+        <v>2.7446140278653579</v>
       </c>
       <c r="I133" t="s">
         <v>17</v>
@@ -5592,16 +5592,16 @@
         <v>3041196</v>
       </c>
       <c r="C134">
-        <v>1976458744.1114879</v>
+        <v>2002929173.720124</v>
       </c>
       <c r="E134">
-        <v>1824423456.1029119</v>
+        <v>1848857698.8185761</v>
       </c>
       <c r="F134">
-        <v>649.89522020661866</v>
+        <v>658.59917404867167</v>
       </c>
       <c r="H134">
-        <v>599.9032801907249</v>
+        <v>607.93769912185076</v>
       </c>
       <c r="I134" t="s">
         <v>38</v>
@@ -5662,22 +5662,22 @@
         <v>9975515</v>
       </c>
       <c r="C136">
-        <v>27856127405.400986</v>
+        <v>28102138351.202431</v>
       </c>
       <c r="D136">
-        <v>1526955.3468176289</v>
+        <v>1555296.6203911132</v>
       </c>
       <c r="E136">
-        <v>57022516.655294813</v>
+        <v>57737469.38077531</v>
       </c>
       <c r="F136">
-        <v>2792.4500544985381</v>
+        <v>2817.1115327080788</v>
       </c>
       <c r="G136">
-        <v>0.15307032737834878</v>
+        <v>0.15591141112926132</v>
       </c>
       <c r="H136">
-        <v>5.7162478985089802</v>
+        <v>5.7879186569089729</v>
       </c>
       <c r="I136" t="s">
         <v>11</v>
@@ -5703,22 +5703,22 @@
         <v>2161126</v>
       </c>
       <c r="C137">
-        <v>5376472977.0508986</v>
+        <v>5375976620.770298</v>
       </c>
       <c r="D137">
-        <v>282841.00141234341</v>
+        <v>280947.3438665166</v>
       </c>
       <c r="E137">
-        <v>7137539.4713745853</v>
+        <v>6434807.4180273507</v>
       </c>
       <c r="F137">
-        <v>2487.8109730996243</v>
+        <v>2487.5812982539187</v>
       </c>
       <c r="G137">
-        <v>0.13087668253139492</v>
+        <v>0.13000044600199923</v>
       </c>
       <c r="H137">
-        <v>3.3026947393972335</v>
+        <v>2.9775253354165141</v>
       </c>
       <c r="I137" t="s">
         <v>11</v>
@@ -5744,16 +5744,16 @@
         <v>7465222</v>
       </c>
       <c r="C138">
-        <v>8141046755.1777763</v>
+        <v>8040436531.9909592</v>
       </c>
       <c r="E138">
-        <v>1411396606.6005249</v>
+        <v>1409349735.0201974</v>
       </c>
       <c r="F138">
-        <v>1090.5297598889592</v>
+        <v>1077.0525688306334</v>
       </c>
       <c r="H138">
-        <v>189.06291153840098</v>
+        <v>188.78872390133841</v>
       </c>
       <c r="I138" t="s">
         <v>26</v>
@@ -5779,22 +5779,22 @@
         <v>6659324</v>
       </c>
       <c r="C139">
-        <v>9067252174.15411</v>
+        <v>8981596994.2914848</v>
       </c>
       <c r="D139">
         <v>547814.85761291161</v>
       </c>
       <c r="E139">
-        <v>17108730.129270419</v>
+        <v>17174113.738967519</v>
       </c>
       <c r="F139">
-        <v>1361.5874785720157</v>
+        <v>1348.7250348971584</v>
       </c>
       <c r="G139">
         <v>8.2262832926121576E-2</v>
       </c>
       <c r="H139">
-        <v>2.5691391692715988</v>
+        <v>2.5789575246627914</v>
       </c>
       <c r="I139" t="s">
         <v>36</v>
@@ -5820,22 +5820,22 @@
         <v>8727176</v>
       </c>
       <c r="C140">
-        <v>11290198675.85006</v>
+        <v>11420363327.756954</v>
       </c>
       <c r="D140">
-        <v>659662.07301539928</v>
+        <v>659900.16843034641</v>
       </c>
       <c r="E140">
-        <v>22271055.296176083</v>
+        <v>23919427.711029597</v>
       </c>
       <c r="F140">
-        <v>1293.6829365936999</v>
+        <v>1308.5978015977853</v>
       </c>
       <c r="G140">
-        <v>7.5587116956894101E-2</v>
+        <v>7.5614399025566395E-2</v>
       </c>
       <c r="H140">
-        <v>2.551920036467247</v>
+        <v>2.7407981357348121</v>
       </c>
       <c r="I140" t="s">
         <v>11</v>
@@ -5905,13 +5905,13 @@
         <v>2227363705.5917497</v>
       </c>
       <c r="E142">
-        <v>235105353.98384598</v>
+        <v>275004789.94685459</v>
       </c>
       <c r="F142">
         <v>1109.8788529063911</v>
       </c>
       <c r="H142">
-        <v>117.15125820568122</v>
+        <v>137.03285190637013</v>
       </c>
       <c r="I142" t="s">
         <v>11</v>
@@ -5937,19 +5937,19 @@
         <v>5178428</v>
       </c>
       <c r="C143">
-        <v>19980480085.140694</v>
+        <v>18816877343.144329</v>
       </c>
       <c r="D143">
-        <v>1115698.2819154211</v>
+        <v>1103732.8629141673</v>
       </c>
       <c r="E143">
         <v>34784653.65595942</v>
       </c>
       <c r="F143">
-        <v>3858.4064672021495</v>
+        <v>3633.7045418309049</v>
       </c>
       <c r="G143">
-        <v>0.21545115272731824</v>
+        <v>0.21314052506169195</v>
       </c>
       <c r="H143">
         <v>6.7172226119508505</v>
@@ -5978,22 +5978,22 @@
         <v>3910602</v>
       </c>
       <c r="C144">
-        <v>24137162461.745937</v>
+        <v>24683489495.479115</v>
       </c>
       <c r="D144">
-        <v>1310318.0040793526</v>
+        <v>1332561.6365911453</v>
       </c>
       <c r="E144">
-        <v>46572322.219610982</v>
+        <v>46134931.224729419</v>
       </c>
       <c r="F144">
-        <v>6172.2370268684817</v>
+        <v>6311.9411015181586</v>
       </c>
       <c r="G144">
-        <v>0.33506810564699563</v>
+        <v>0.34075613846439634</v>
       </c>
       <c r="H144">
-        <v>11.909246254057811</v>
+        <v>11.797398769992299</v>
       </c>
       <c r="I144" t="s">
         <v>12</v>
@@ -6019,22 +6019,22 @@
         <v>7463219</v>
       </c>
       <c r="C145">
-        <v>36114649935.972176</v>
+        <v>36153851543.962112</v>
       </c>
       <c r="D145">
-        <v>1926960.0936788397</v>
+        <v>1933878.3568729642</v>
       </c>
       <c r="E145">
-        <v>43747437.657347538</v>
+        <v>42464456.673304446</v>
       </c>
       <c r="F145">
-        <v>4839.0178468529703</v>
+        <v>4844.2704875687168</v>
       </c>
       <c r="G145">
-        <v>0.25819423142732911</v>
+        <v>0.25912121255894593</v>
       </c>
       <c r="H145">
-        <v>5.8617384344942227</v>
+        <v>5.6898312475226103</v>
       </c>
       <c r="I145" t="s">
         <v>35</v>
@@ -6060,22 +6060,22 @@
         <v>2584028</v>
       </c>
       <c r="C146">
-        <v>12337454419.71706</v>
+        <v>12331541918.530838</v>
       </c>
       <c r="D146">
-        <v>651001.19157366978</v>
+        <v>647726.89256207761</v>
       </c>
       <c r="E146">
-        <v>22735919.126683772</v>
+        <v>22250078.339433193</v>
       </c>
       <c r="F146">
-        <v>4774.5049278556817</v>
+        <v>4772.2168329951674</v>
       </c>
       <c r="G146">
-        <v>0.25193271573437659</v>
+        <v>0.25066558588454835</v>
       </c>
       <c r="H146">
-        <v>8.7986349709383074</v>
+        <v>8.6106181277575899</v>
       </c>
       <c r="I146" t="s">
         <v>20</v>
@@ -6101,16 +6101,16 @@
         <v>5184267</v>
       </c>
       <c r="C147">
-        <v>5977148880.1886787</v>
+        <v>5927296836.063343</v>
       </c>
       <c r="E147">
-        <v>1079655954.6293058</v>
+        <v>1072145762.6568449</v>
       </c>
       <c r="F147">
-        <v>1152.9400164360129</v>
+        <v>1143.3239908483383</v>
       </c>
       <c r="H147">
-        <v>208.25624039604941</v>
+        <v>206.80758970493704</v>
       </c>
       <c r="I147" t="s">
         <v>38</v>
@@ -6142,7 +6142,7 @@
         <v>666236.06754905742</v>
       </c>
       <c r="E148">
-        <v>9354949.0672551934</v>
+        <v>22642717.274608072</v>
       </c>
       <c r="F148">
         <v>2857.853740773463</v>
@@ -6151,7 +6151,7 @@
         <v>0.1623140579092775</v>
       </c>
       <c r="H148">
-        <v>2.2791317051129067</v>
+        <v>5.5164100263357652</v>
       </c>
       <c r="I148" t="s">
         <v>11</v>
@@ -6177,22 +6177,22 @@
         <v>5491581</v>
       </c>
       <c r="C149">
-        <v>18080180048.928005</v>
+        <v>17970619105.13818</v>
       </c>
       <c r="D149">
-        <v>975247.57714710501</v>
+        <v>966305.67906167998</v>
       </c>
       <c r="E149">
-        <v>34119551.408353955</v>
+        <v>33382272.622331116</v>
       </c>
       <c r="F149">
-        <v>3292.3451459475891</v>
+        <v>3272.3944352524677</v>
       </c>
       <c r="G149">
-        <v>0.17758958251678433</v>
+        <v>0.17596129039372815</v>
       </c>
       <c r="H149">
-        <v>6.2130653100362085</v>
+        <v>6.0788091120446222</v>
       </c>
       <c r="I149" t="s">
         <v>17</v>
@@ -6221,13 +6221,13 @@
         <v>1490654522.3913691</v>
       </c>
       <c r="E150">
-        <v>174777391.20240006</v>
+        <v>161536679.74767277</v>
       </c>
       <c r="F150">
         <v>1147.5365144305708</v>
       </c>
       <c r="H150">
-        <v>134.54723095725652</v>
+        <v>124.35425891504011</v>
       </c>
       <c r="I150" t="s">
         <v>26</v>
@@ -6253,22 +6253,22 @@
         <v>3250811</v>
       </c>
       <c r="C151">
-        <v>11430428734.411934</v>
+        <v>10226518753.765198</v>
       </c>
       <c r="D151">
-        <v>617566.48656140699</v>
+        <v>573126.45152054587</v>
       </c>
       <c r="E151">
-        <v>12713272.236616379</v>
+        <v>12507838.493962234</v>
       </c>
       <c r="F151">
-        <v>3516.1775736614445</v>
+        <v>3145.8361478920788</v>
       </c>
       <c r="G151">
-        <v>0.18997305182042479</v>
+        <v>0.1763026061867472</v>
       </c>
       <c r="H151">
-        <v>3.9108001777453003</v>
+        <v>3.8476055648766518</v>
       </c>
       <c r="I151" t="s">
         <v>20</v>
@@ -6294,22 +6294,22 @@
         <v>4583206</v>
       </c>
       <c r="C152">
-        <v>18544380470.442627</v>
+        <v>18615214200.146648</v>
       </c>
       <c r="D152">
-        <v>1081499.1944933967</v>
+        <v>876813.02018039604</v>
       </c>
       <c r="E152">
-        <v>65988593.098840229</v>
+        <v>3385378.456294965</v>
       </c>
       <c r="F152">
-        <v>4046.1590577518505</v>
+        <v>4061.6141190569765</v>
       </c>
       <c r="G152">
-        <v>0.2359700162928301</v>
+        <v>0.19130997388736096</v>
       </c>
       <c r="H152">
-        <v>14.397911221716901</v>
+        <v>0.73864854782764833</v>
       </c>
       <c r="I152" t="s">
         <v>11</v>
@@ -6335,22 +6335,22 @@
         <v>12498933</v>
       </c>
       <c r="C153">
-        <v>70130177611.739685</v>
+        <v>70751145818.678345</v>
       </c>
       <c r="D153">
-        <v>3770096.1778332042</v>
+        <v>3801789.546693502</v>
       </c>
       <c r="E153">
-        <v>139439140.63018888</v>
+        <v>140806834.14877334</v>
       </c>
       <c r="F153">
-        <v>5610.8931547788661</v>
+        <v>5660.5748521636488</v>
       </c>
       <c r="G153">
-        <v>0.30163344165723621</v>
+        <v>0.30416912761221315</v>
       </c>
       <c r="H153">
-        <v>11.156083533705548</v>
+        <v>11.265508355695109</v>
       </c>
       <c r="I153" t="s">
         <v>29</v>
@@ -6376,22 +6376,22 @@
         <v>13439341</v>
       </c>
       <c r="C154">
-        <v>15538691216.952995</v>
+        <v>15179951011.781172</v>
       </c>
       <c r="D154">
-        <v>896057.76476757927</v>
+        <v>829901.84480830259</v>
       </c>
       <c r="E154">
-        <v>29005573.521986548</v>
+        <v>28116293.687446728</v>
       </c>
       <c r="F154">
-        <v>1156.2093124174016</v>
+        <v>1129.5160240209079</v>
       </c>
       <c r="G154">
-        <v>6.6674233860691476E-2</v>
+        <v>6.1751677021090731E-2</v>
       </c>
       <c r="H154">
-        <v>2.1582586171439919</v>
+        <v>2.0920887182970302</v>
       </c>
       <c r="I154" t="s">
         <v>37</v>
@@ -6417,22 +6417,22 @@
         <v>14171621</v>
       </c>
       <c r="C155">
-        <v>78458473909.25531</v>
+        <v>79337497904.338455</v>
       </c>
       <c r="D155">
-        <v>4208422.6648895573</v>
+        <v>4272000.3159768172</v>
       </c>
       <c r="E155">
-        <v>141942013.28385779</v>
+        <v>143726525.33927959</v>
       </c>
       <c r="F155">
-        <v>5536.3090721418039</v>
+        <v>5598.3361327782095</v>
       </c>
       <c r="G155">
-        <v>0.29696127668737105</v>
+        <v>0.30144754195563211</v>
       </c>
       <c r="H155">
-        <v>10.015933483110915</v>
+        <v>10.141855002986574</v>
       </c>
       <c r="I155" t="s">
         <v>31</v>
@@ -6458,22 +6458,22 @@
         <v>1940463</v>
       </c>
       <c r="C156">
-        <v>10247569454.784153</v>
+        <v>10418693209.484459</v>
       </c>
       <c r="D156">
-        <v>550269.883050462</v>
+        <v>555793.05143970135</v>
       </c>
       <c r="E156">
-        <v>9130246.9677386675</v>
+        <v>10176827.835570175</v>
       </c>
       <c r="F156">
-        <v>5280.9919358339503</v>
+        <v>5369.1790101045262</v>
       </c>
       <c r="G156">
-        <v>0.28357659128283408</v>
+        <v>0.28642290599702303</v>
       </c>
       <c r="H156">
-        <v>4.7051899303097597</v>
+        <v>5.2445358842555478</v>
       </c>
       <c r="I156" t="s">
         <v>32</v>
@@ -6499,16 +6499,16 @@
         <v>166824</v>
       </c>
       <c r="C157">
-        <v>427933615.80421412</v>
+        <v>423243963.01646668</v>
       </c>
       <c r="E157">
-        <v>84210568.583888099</v>
+        <v>83341407.504733786</v>
       </c>
       <c r="F157">
-        <v>2565.1801647497614</v>
+        <v>2537.0687851656039</v>
       </c>
       <c r="H157">
-        <v>504.78689267664186</v>
+        <v>499.57684448720681</v>
       </c>
       <c r="I157" t="s">
         <v>36</v>
@@ -6534,16 +6534,16 @@
         <v>97358</v>
       </c>
       <c r="C158">
-        <v>34671837.052631997</v>
+        <v>14189541.854279999</v>
       </c>
       <c r="E158">
-        <v>32004772.663967997</v>
+        <v>13098038.634719998</v>
       </c>
       <c r="F158">
-        <v>356.12725253838408</v>
+        <v>145.74602861891162</v>
       </c>
       <c r="H158">
-        <v>328.73284849696989</v>
+        <v>134.53479564822612</v>
       </c>
       <c r="I158" t="s">
         <v>22</v>
@@ -6604,16 +6604,16 @@
         <v>334348.61</v>
       </c>
       <c r="C160">
-        <v>1320983250.5161543</v>
+        <v>1346990316.7086997</v>
       </c>
       <c r="E160">
-        <v>137757814.33286089</v>
+        <v>135319369.82411471</v>
       </c>
       <c r="F160">
-        <v>3950.9159332714271</v>
+        <v>4028.700214152826</v>
       </c>
       <c r="H160">
-        <v>412.01850467648393</v>
+        <v>404.72538475369981</v>
       </c>
       <c r="I160" t="s">
         <v>35</v>
@@ -6674,22 +6674,22 @@
         <v>11106837</v>
       </c>
       <c r="C162">
-        <v>18577249960.309849</v>
+        <v>18263142973.661293</v>
       </c>
       <c r="D162">
-        <v>1010209.2640425027</v>
+        <v>1004547.349931256</v>
       </c>
       <c r="E162">
-        <v>38092344.214238651</v>
+        <v>37897296.776849344</v>
       </c>
       <c r="F162">
-        <v>1672.5958938903891</v>
+        <v>1644.3153864292142</v>
       </c>
       <c r="G162">
-        <v>9.0953820970137836E-2</v>
+        <v>9.0444052607529579E-2</v>
       </c>
       <c r="H162">
-        <v>3.4296302551517277</v>
+        <v>3.4120692305873712</v>
       </c>
       <c r="I162" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
continued implementation of DSI with code changes to accomodate edits in paper
</commit_message>
<xml_diff>
--- a/r_map/data_boot_cq_remov_As.xlsx
+++ b/r_map/data_boot_cq_remov_As.xlsx
@@ -606,22 +606,22 @@
         <v>2207648</v>
       </c>
       <c r="C2">
-        <v>24084085054.395599</v>
+        <v>24670401731.749802</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>22231463127.134399</v>
+        <v>22772678521.615196</v>
       </c>
       <c r="F2">
-        <v>10909.38639420578</v>
+        <v>11174.970707173336</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>10070.20282542072</v>
+        <v>10315.357575852307</v>
       </c>
       <c r="I2" t="s">
         <v>9</v>
@@ -647,22 +647,22 @@
         <v>5806845</v>
       </c>
       <c r="C3">
-        <v>24772791993.021297</v>
+        <v>25049326432.412323</v>
       </c>
       <c r="D3">
-        <v>9673616.4871618971</v>
+        <v>9808116.7589789145</v>
       </c>
       <c r="E3">
-        <v>1211928766.5127215</v>
+        <v>1235240043.5723443</v>
       </c>
       <c r="F3">
-        <v>4266.1362569555922</v>
+        <v>4313.7584062278784</v>
       </c>
       <c r="G3">
-        <v>1.6658988636965335</v>
+        <v>1.6890612301480261</v>
       </c>
       <c r="H3">
-        <v>208.70692544965837</v>
+        <v>212.7213734088553</v>
       </c>
       <c r="I3" t="s">
         <v>9</v>
@@ -688,22 +688,22 @@
         <v>2726384</v>
       </c>
       <c r="C4">
-        <v>17369792251.826015</v>
+        <v>17472869346.310638</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1385395943.2065969</v>
+        <v>1398071375.2651119</v>
       </c>
       <c r="F4">
-        <v>6370.9999221775124</v>
+        <v>6408.8071769459611</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4">
-        <v>508.14409973305186</v>
+        <v>512.79327316515651</v>
       </c>
       <c r="I4" t="s">
         <v>9</v>
@@ -729,22 +729,22 @@
         <v>1657543</v>
       </c>
       <c r="C5">
-        <v>13633442265.456619</v>
+        <v>13675122881.28898</v>
       </c>
       <c r="D5">
-        <v>5550454.570667211</v>
+        <v>5568845.3817810519</v>
       </c>
       <c r="E5">
-        <v>199213544.09527925</v>
+        <v>139914902.18216446</v>
       </c>
       <c r="F5">
-        <v>8225.0911532651753</v>
+        <v>8250.2371771284252</v>
       </c>
       <c r="G5">
-        <v>3.3486036686029932</v>
+        <v>3.3596988927473084</v>
       </c>
       <c r="H5">
-        <v>120.18604892619935</v>
+        <v>84.411024137632907</v>
       </c>
       <c r="I5" t="s">
         <v>9</v>
@@ -770,22 +770,22 @@
         <v>541762</v>
       </c>
       <c r="C6">
-        <v>386165673.32670599</v>
+        <v>381062162.22547197</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>356460621.53234392</v>
+        <v>351749688.20812798</v>
       </c>
       <c r="F6">
-        <v>712.79579100547107</v>
+        <v>703.37558231376875</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6">
-        <v>657.9653455435116</v>
+        <v>649.26976828963268</v>
       </c>
       <c r="I6" t="s">
         <v>10</v>
@@ -811,22 +811,22 @@
         <v>324142</v>
       </c>
       <c r="C7">
-        <v>433733463.83028477</v>
+        <v>437903977.90557593</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>40676710.708581835</v>
+        <v>42595423.477854565</v>
       </c>
       <c r="F7">
-        <v>1338.0970803854013</v>
+        <v>1350.9633984660302</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>125.49040454054654</v>
+        <v>131.4097632452893</v>
       </c>
       <c r="I7" t="s">
         <v>10</v>
@@ -852,22 +852,22 @@
         <v>2081937</v>
       </c>
       <c r="C8">
-        <v>2718848006.3654871</v>
+        <v>2715522728.2048087</v>
       </c>
       <c r="D8">
-        <v>203164.51408060998</v>
+        <v>201265.78030415569</v>
       </c>
       <c r="E8">
-        <v>3302101.6639514952</v>
+        <v>3290161.0767286243</v>
       </c>
       <c r="F8">
-        <v>1305.9223244341626</v>
+        <v>1304.3251204070098</v>
       </c>
       <c r="G8">
-        <v>9.7584371707986353E-2</v>
+        <v>9.6672368234079945E-2</v>
       </c>
       <c r="H8">
-        <v>1.5860718474917805</v>
+        <v>1.5803365215799634</v>
       </c>
       <c r="I8" t="s">
         <v>11</v>
@@ -893,22 +893,22 @@
         <v>8921964</v>
       </c>
       <c r="C9">
-        <v>46650191727.175949</v>
+        <v>46741639338.62944</v>
       </c>
       <c r="D9">
-        <v>2646248.0567307342</v>
+        <v>2670401.6281375219</v>
       </c>
       <c r="E9">
-        <v>50048979.760964021</v>
+        <v>49356758.568895653</v>
       </c>
       <c r="F9">
-        <v>5228.6908720070996</v>
+        <v>5238.9405896089065</v>
       </c>
       <c r="G9">
-        <v>0.29659927530874752</v>
+        <v>0.29930647872346516</v>
       </c>
       <c r="H9">
-        <v>5.609637044149026</v>
+        <v>5.5320508543741775</v>
       </c>
       <c r="I9" t="s">
         <v>12</v>
@@ -934,22 +934,22 @@
         <v>7744214</v>
       </c>
       <c r="C10">
-        <v>21845771405.552444</v>
+        <v>21803593855.615612</v>
       </c>
       <c r="D10">
-        <v>1543645.7585957521</v>
+        <v>1515611.4747721422</v>
       </c>
       <c r="E10">
-        <v>24115011.192159534</v>
+        <v>23451542.381827917</v>
       </c>
       <c r="F10">
-        <v>2820.9152543502082</v>
+        <v>2815.4689237171924</v>
       </c>
       <c r="G10">
-        <v>0.19932891299178354</v>
+        <v>0.19570888340277556</v>
       </c>
       <c r="H10">
-        <v>3.1139391540780683</v>
+        <v>3.0282663136411152</v>
       </c>
       <c r="I10" t="s">
         <v>13</v>
@@ -975,22 +975,22 @@
         <v>1912394</v>
       </c>
       <c r="C11">
-        <v>1557857405.0563226</v>
+        <v>1561641708.5455222</v>
       </c>
       <c r="D11">
-        <v>636176.29107324989</v>
+        <v>639238.88130846806</v>
       </c>
       <c r="E11">
-        <v>17138117.366225459</v>
+        <v>17452980.024991795</v>
       </c>
       <c r="F11">
-        <v>814.61111311598063</v>
+        <v>816.58994357100164</v>
       </c>
       <c r="G11">
-        <v>0.33265963555274169</v>
+        <v>0.33426107868382143</v>
       </c>
       <c r="H11">
-        <v>8.9616038150221442</v>
+        <v>9.1262470102875213</v>
       </c>
       <c r="I11" t="s">
         <v>14</v>
@@ -1016,22 +1016,22 @@
         <v>2014725</v>
       </c>
       <c r="C12">
-        <v>2776763320.9511518</v>
+        <v>2747253885.3131909</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12">
-        <v>268751834.24792737</v>
+        <v>268822223.47071826</v>
       </c>
       <c r="F12">
-        <v>1378.2344096346408</v>
+        <v>1363.5875294708662</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12">
-        <v>133.39380523293619</v>
+        <v>133.42874261783533</v>
       </c>
       <c r="I12" t="s">
         <v>15</v>
@@ -1057,22 +1057,22 @@
         <v>9164672</v>
       </c>
       <c r="C13">
-        <v>21595338983.16539</v>
+        <v>21346324048.401039</v>
       </c>
       <c r="D13">
-        <v>1358331.5338211404</v>
+        <v>1322080.6468099304</v>
       </c>
       <c r="E13">
-        <v>24381500.489247091</v>
+        <v>23444116.072725877</v>
       </c>
       <c r="F13">
-        <v>2356.3679074565234</v>
+        <v>2329.1967293975213</v>
       </c>
       <c r="G13">
-        <v>0.14821387321020768</v>
+        <v>0.14425837027336388</v>
       </c>
       <c r="H13">
-        <v>2.6603789518323286</v>
+        <v>2.5580965770216193</v>
       </c>
       <c r="I13" t="s">
         <v>11</v>
@@ -1098,22 +1098,22 @@
         <v>3900879</v>
       </c>
       <c r="C14">
-        <v>8271701610.075038</v>
+        <v>8266720195.6695395</v>
       </c>
       <c r="D14">
-        <v>638324.57592388778</v>
+        <v>628394.48166302126</v>
       </c>
       <c r="E14">
-        <v>11409451.373729937</v>
+        <v>11449357.606600318</v>
       </c>
       <c r="F14">
-        <v>2120.4712092005516</v>
+        <v>2119.1942112712391</v>
       </c>
       <c r="G14">
-        <v>0.16363608712905162</v>
+        <v>0.1610904828534854</v>
       </c>
       <c r="H14">
-        <v>2.9248411380434862</v>
+        <v>2.9350711997476258</v>
       </c>
       <c r="I14" t="s">
         <v>13</v>
@@ -1139,22 +1139,22 @@
         <v>9744872</v>
       </c>
       <c r="C15">
-        <v>53923436619.399551</v>
+        <v>54056000683.853531</v>
       </c>
       <c r="D15">
-        <v>2337737.9337056568</v>
+        <v>2333517.3057768052</v>
       </c>
       <c r="E15">
-        <v>968361858.11733317</v>
+        <v>955580113.92257977</v>
       </c>
       <c r="F15">
-        <v>5533.5192313864718</v>
+        <v>5547.1227004165403</v>
       </c>
       <c r="G15">
-        <v>0.23989416522922588</v>
+        <v>0.23946105251837121</v>
       </c>
       <c r="H15">
-        <v>99.371429210905305</v>
+        <v>98.05979123405416</v>
       </c>
       <c r="I15" t="s">
         <v>13</v>
@@ -1180,22 +1180,22 @@
         <v>2476429</v>
       </c>
       <c r="C16">
-        <v>14978677822.881842</v>
+        <v>14978520147.514009</v>
       </c>
       <c r="D16">
-        <v>751975.94563126413</v>
+        <v>749192.30494902667</v>
       </c>
       <c r="E16">
-        <v>14496630.901147492</v>
+        <v>11123746.620528977</v>
       </c>
       <c r="F16">
-        <v>6048.4987951933372</v>
+        <v>6048.4351247356617</v>
       </c>
       <c r="G16">
-        <v>0.30365334343575534</v>
+        <v>0.30252928912923677</v>
       </c>
       <c r="H16">
-        <v>5.8538447503027511</v>
+        <v>4.491849603008597</v>
       </c>
       <c r="I16" t="s">
         <v>13</v>
@@ -1221,22 +1221,22 @@
         <v>12851943</v>
       </c>
       <c r="C17">
-        <v>48805939946.803238</v>
+        <v>49205859023.803238</v>
       </c>
       <c r="D17">
-        <v>2835786.6261227988</v>
+        <v>2815478.3036453421</v>
       </c>
       <c r="E17">
-        <v>53698168.882559121</v>
+        <v>52239988.709367499</v>
       </c>
       <c r="F17">
-        <v>3797.5534086015819</v>
+        <v>3828.6708106162032</v>
       </c>
       <c r="G17">
-        <v>0.2206504204168038</v>
+        <v>0.21907024514856174</v>
       </c>
       <c r="H17">
-        <v>4.1782140554590947</v>
+        <v>4.0647541550229018</v>
       </c>
       <c r="I17" t="s">
         <v>16</v>
@@ -1262,22 +1262,22 @@
         <v>1157290</v>
       </c>
       <c r="C18">
-        <v>7429133665.8172436</v>
+        <v>7446101080.531992</v>
       </c>
       <c r="D18">
-        <v>439814.37543029943</v>
+        <v>444097.69797489443</v>
       </c>
       <c r="E18">
-        <v>8776238.3434517682</v>
+        <v>9643809.0281445757</v>
       </c>
       <c r="F18">
-        <v>6419.4226735020984</v>
+        <v>6434.0840070613176</v>
       </c>
       <c r="G18">
-        <v>0.38003817144388996</v>
+        <v>0.38373933756871176</v>
       </c>
       <c r="H18">
-        <v>7.5834391928140468</v>
+        <v>8.3330963096065602</v>
       </c>
       <c r="I18" t="s">
         <v>16</v>
@@ -1303,22 +1303,22 @@
         <v>2981276</v>
       </c>
       <c r="C19">
-        <v>3526738626.7850881</v>
+        <v>3504312096.1184244</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19">
-        <v>331593886.78000915</v>
+        <v>335989692.05569589</v>
       </c>
       <c r="F19">
-        <v>1182.9628074640148</v>
+        <v>1175.4403470589186</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
       <c r="H19">
-        <v>111.22549095756621</v>
+        <v>112.69996204836315</v>
       </c>
       <c r="I19" t="s">
         <v>17</v>
@@ -1344,22 +1344,22 @@
         <v>1265697</v>
       </c>
       <c r="C20">
-        <v>1555481430.9353902</v>
+        <v>1559950862.1053076</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="E20">
-        <v>150625829.71680838</v>
+        <v>147826995.55659369</v>
       </c>
       <c r="F20">
-        <v>1228.9524514440582</v>
+        <v>1232.483652963788</v>
       </c>
       <c r="G20">
         <v>0</v>
       </c>
       <c r="H20">
-        <v>119.00623112546556</v>
+        <v>116.79493240214181</v>
       </c>
       <c r="I20" t="s">
         <v>17</v>
@@ -1385,22 +1385,22 @@
         <v>5057931</v>
       </c>
       <c r="C21">
-        <v>5426301544.5791168</v>
+        <v>5329222116.3236465</v>
       </c>
       <c r="D21">
         <v>0</v>
       </c>
       <c r="E21">
-        <v>509892415.12094128</v>
+        <v>504539669.58954716</v>
       </c>
       <c r="F21">
-        <v>1072.8302826944687</v>
+        <v>1053.6367768408954</v>
       </c>
       <c r="G21">
         <v>0</v>
       </c>
       <c r="H21">
-        <v>100.81047272510069</v>
+        <v>99.752185150320784</v>
       </c>
       <c r="I21" t="s">
         <v>17</v>
@@ -1426,22 +1426,22 @@
         <v>1796131</v>
       </c>
       <c r="C22">
-        <v>1506270060.5635018</v>
+        <v>1481062944.0727749</v>
       </c>
       <c r="D22">
         <v>0</v>
       </c>
       <c r="E22">
-        <v>812560052.87841034</v>
+        <v>801292816.06157172</v>
       </c>
       <c r="F22">
-        <v>838.61926583500974</v>
+        <v>824.58514666957751</v>
       </c>
       <c r="G22">
         <v>0</v>
       </c>
       <c r="H22">
-        <v>452.39464876359818</v>
+        <v>446.12158916113117</v>
       </c>
       <c r="I22" t="s">
         <v>17</v>
@@ -1467,22 +1467,22 @@
         <v>2372033</v>
       </c>
       <c r="C23">
-        <v>2466599396.6861267</v>
+        <v>2494706151.0615172</v>
       </c>
       <c r="D23">
         <v>0</v>
       </c>
       <c r="E23">
-        <v>236622858.12687278</v>
+        <v>243195715.29706374</v>
       </c>
       <c r="F23">
-        <v>1039.8672348513392</v>
+        <v>1051.7164605473522</v>
       </c>
       <c r="G23">
         <v>0</v>
       </c>
       <c r="H23">
-        <v>99.755297724303489</v>
+        <v>102.52627821664527</v>
       </c>
       <c r="I23" t="s">
         <v>17</v>
@@ -1508,22 +1508,22 @@
         <v>4881045</v>
       </c>
       <c r="C24">
-        <v>4465660355.4586887</v>
+        <v>4481265611.2870989</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
       <c r="E24">
-        <v>371057180.88269585</v>
+        <v>365749667.19750369</v>
       </c>
       <c r="F24">
-        <v>914.898419387383</v>
+        <v>918.0955330850461</v>
       </c>
       <c r="G24">
         <v>0</v>
       </c>
       <c r="H24">
-        <v>76.020028678837392</v>
+        <v>74.932656264694074</v>
       </c>
       <c r="I24" t="s">
         <v>17</v>
@@ -1549,22 +1549,22 @@
         <v>2219933</v>
       </c>
       <c r="C25">
-        <v>2549152188.5267029</v>
+        <v>2550820752.5756292</v>
       </c>
       <c r="D25">
         <v>0</v>
       </c>
       <c r="E25">
-        <v>247818457.01747075</v>
+        <v>242418225.067013</v>
       </c>
       <c r="F25">
-        <v>1148.3014075319854</v>
+        <v>1149.0530356437016</v>
       </c>
       <c r="G25">
         <v>0</v>
       </c>
       <c r="H25">
-        <v>111.63330470670545</v>
+        <v>109.20069437546674</v>
       </c>
       <c r="I25" t="s">
         <v>17</v>
@@ -1590,22 +1590,22 @@
         <v>1056327</v>
       </c>
       <c r="C26">
-        <v>1819628781.8491902</v>
+        <v>1819863796.4010401</v>
       </c>
       <c r="D26">
-        <v>144259.15187699517</v>
+        <v>139111.51352398287</v>
       </c>
       <c r="E26">
-        <v>2931148.6682764054</v>
+        <v>2853991.3829644029</v>
       </c>
       <c r="F26">
-        <v>1722.5998974268293</v>
+        <v>1722.8223801919671</v>
       </c>
       <c r="G26">
-        <v>0.13656675620049016</v>
+        <v>0.13169360768396801</v>
       </c>
       <c r="H26">
-        <v>2.7748497087326229</v>
+        <v>2.7018067160684174</v>
       </c>
       <c r="I26" t="s">
         <v>17</v>
@@ -1631,22 +1631,22 @@
         <v>1066912</v>
       </c>
       <c r="C27">
-        <v>4761102071.8789787</v>
+        <v>4868433165.813468</v>
       </c>
       <c r="D27">
-        <v>308551.07453337859</v>
+        <v>309160.91923057102</v>
       </c>
       <c r="E27">
-        <v>5862305.170181362</v>
+        <v>5756396.8486398673</v>
       </c>
       <c r="F27">
-        <v>4462.5068158189042</v>
+        <v>4563.1065784370858</v>
       </c>
       <c r="G27">
-        <v>0.2892001163482823</v>
+        <v>0.28977171428437493</v>
       </c>
       <c r="H27">
-        <v>5.4946473281595498</v>
+        <v>5.395381107945048</v>
       </c>
       <c r="I27" t="s">
         <v>17</v>
@@ -1672,22 +1672,22 @@
         <v>5225154</v>
       </c>
       <c r="C28">
-        <v>23719068760.783867</v>
+        <v>24128720840.365067</v>
       </c>
       <c r="D28">
-        <v>2511775.088271589</v>
+        <v>2558652.8772822507</v>
       </c>
       <c r="E28">
-        <v>40506041.637880266</v>
+        <v>40713610.228321567</v>
       </c>
       <c r="F28">
-        <v>4539.4008981905354</v>
+        <v>4617.8008993352287</v>
       </c>
       <c r="G28">
-        <v>0.48070833668664864</v>
+        <v>0.48967989790965982</v>
       </c>
       <c r="H28">
-        <v>7.7521239829257214</v>
+        <v>7.7918488581047693</v>
       </c>
       <c r="I28" t="s">
         <v>18</v>
@@ -1713,22 +1713,22 @@
         <v>2992958</v>
       </c>
       <c r="C29">
-        <v>11940006742.199289</v>
+        <v>11654198611.926296</v>
       </c>
       <c r="D29">
-        <v>525692.38420990668</v>
+        <v>525973.2243517146</v>
       </c>
       <c r="E29">
-        <v>180189796.15664744</v>
+        <v>184355029.97547048</v>
       </c>
       <c r="F29">
-        <v>3989.3666206472958</v>
+        <v>3893.8730887390657</v>
       </c>
       <c r="G29">
-        <v>0.17564308761095435</v>
+        <v>0.17573692125038662</v>
       </c>
       <c r="H29">
-        <v>60.20458561618554</v>
+        <v>61.596263621297219</v>
       </c>
       <c r="I29" t="s">
         <v>18</v>
@@ -1754,22 +1754,22 @@
         <v>229494</v>
       </c>
       <c r="C30">
-        <v>3286948154.0678282</v>
+        <v>3307189636.9419532</v>
       </c>
       <c r="D30">
         <v>0</v>
       </c>
       <c r="E30">
-        <v>206113422.8105678</v>
+        <v>205148328.74618286</v>
       </c>
       <c r="F30">
-        <v>14322.588625706241</v>
+        <v>14410.789114059422</v>
       </c>
       <c r="G30">
         <v>0</v>
       </c>
       <c r="H30">
-        <v>898.12118317066154</v>
+        <v>893.91587033291876</v>
       </c>
       <c r="I30" t="s">
         <v>18</v>
@@ -1795,22 +1795,22 @@
         <v>6529869</v>
       </c>
       <c r="C31">
-        <v>52334291713.730652</v>
+        <v>52558684137.476654</v>
       </c>
       <c r="D31">
-        <v>2840079.8724451596</v>
+        <v>2849280.8062308901</v>
       </c>
       <c r="E31">
-        <v>48275170.956477202</v>
+        <v>51688738.282548837</v>
       </c>
       <c r="F31">
-        <v>8014.6005553450841</v>
+        <v>8048.9645561766483</v>
       </c>
       <c r="G31">
-        <v>0.43493673034561026</v>
+        <v>0.43634578369503124</v>
       </c>
       <c r="H31">
-        <v>7.392976942795821</v>
+        <v>7.9157389348161251</v>
       </c>
       <c r="I31" t="s">
         <v>18</v>
@@ -1836,22 +1836,22 @@
         <v>1441562</v>
       </c>
       <c r="C32">
-        <v>3936838340.4354658</v>
+        <v>3718757343.6224527</v>
       </c>
       <c r="D32">
-        <v>279577.34444749577</v>
+        <v>273844.53008444933</v>
       </c>
       <c r="E32">
-        <v>4248324.9391146125</v>
+        <v>4382829.933755477</v>
       </c>
       <c r="F32">
-        <v>2730.9531885797946</v>
+        <v>2579.6721498086472</v>
       </c>
       <c r="G32">
-        <v>0.19394056200669535</v>
+        <v>0.18996375465255697</v>
       </c>
       <c r="H32">
-        <v>2.9470289443774269</v>
+        <v>3.0403339806095588</v>
       </c>
       <c r="I32" t="s">
         <v>18</v>
@@ -1877,22 +1877,22 @@
         <v>1650341</v>
       </c>
       <c r="C33">
-        <v>3903092514.5367212</v>
+        <v>3995500976.3396654</v>
       </c>
       <c r="D33">
         <v>0</v>
       </c>
       <c r="E33">
-        <v>326677318.69423842</v>
+        <v>330684480.58915412</v>
       </c>
       <c r="F33">
-        <v>2365.0218436897107</v>
+        <v>2421.0154000534831</v>
       </c>
       <c r="G33">
         <v>0</v>
       </c>
       <c r="H33">
-        <v>197.94534504944033</v>
+        <v>200.37342621261553</v>
       </c>
       <c r="I33" t="s">
         <v>18</v>
@@ -1918,22 +1918,22 @@
         <v>4984247</v>
       </c>
       <c r="C34">
-        <v>17621599176.992424</v>
+        <v>21413552310.887318</v>
       </c>
       <c r="D34">
-        <v>1196889.1331427954</v>
+        <v>1245327.9657646788</v>
       </c>
       <c r="E34">
-        <v>16476991.227370419</v>
+        <v>16547050.10476597</v>
       </c>
       <c r="F34">
-        <v>3535.4586514256666</v>
+        <v>4296.2462155040303</v>
       </c>
       <c r="G34">
-        <v>0.24013439405045445</v>
+        <v>0.24985277931945965</v>
       </c>
       <c r="H34">
-        <v>3.3058135416183063</v>
+        <v>3.3198696021216385</v>
       </c>
       <c r="I34" t="s">
         <v>18</v>
@@ -1959,22 +1959,22 @@
         <v>2093626</v>
       </c>
       <c r="C35">
-        <v>7482568042.5081577</v>
+        <v>7670393855.1317616</v>
       </c>
       <c r="D35">
         <v>0</v>
       </c>
       <c r="E35">
-        <v>670164925.45714951</v>
+        <v>677123088.38878059</v>
       </c>
       <c r="F35">
-        <v>3573.9755058965438</v>
+        <v>3663.6886698635581</v>
       </c>
       <c r="G35">
         <v>0</v>
       </c>
       <c r="H35">
-        <v>320.09772779720424</v>
+        <v>323.42122632637376</v>
       </c>
       <c r="I35" t="s">
         <v>18</v>
@@ -2000,7 +2000,7 @@
         <v>67254</v>
       </c>
       <c r="C36">
-        <v>167559997.9844797</v>
+        <v>167355064.27704313</v>
       </c>
       <c r="D36">
         <v>10781.717512572483</v>
@@ -2009,7 +2009,7 @@
         <v>173616.32428321111</v>
       </c>
       <c r="F36">
-        <v>2491.4502926886089</v>
+        <v>2488.4031325578126</v>
       </c>
       <c r="G36">
         <v>0.1603134016203123</v>
@@ -2041,22 +2041,22 @@
         <v>245567</v>
       </c>
       <c r="C37">
-        <v>203758068.09289023</v>
+        <v>203161781.17123124</v>
       </c>
       <c r="D37">
         <v>0</v>
       </c>
       <c r="E37">
-        <v>19527327.267273139</v>
+        <v>19587298.072820533</v>
       </c>
       <c r="F37">
-        <v>829.74531632055709</v>
+        <v>827.31711170976246</v>
       </c>
       <c r="G37">
         <v>0</v>
       </c>
       <c r="H37">
-        <v>79.519346114392974</v>
+        <v>79.763559732458077</v>
       </c>
       <c r="I37" t="s">
         <v>19</v>
@@ -2082,22 +2082,22 @@
         <v>717925</v>
       </c>
       <c r="C38">
-        <v>768965550.2500385</v>
+        <v>771182041.27960086</v>
       </c>
       <c r="D38">
         <v>0</v>
       </c>
       <c r="E38">
-        <v>164672742.52915719</v>
+        <v>163546280.6744445</v>
       </c>
       <c r="F38">
-        <v>1071.0945436501563</v>
+        <v>1074.1819010058166</v>
       </c>
       <c r="G38">
         <v>0</v>
       </c>
       <c r="H38">
-        <v>229.37318317255588</v>
+        <v>227.80413089730055</v>
       </c>
       <c r="I38" t="s">
         <v>19</v>
@@ -2123,22 +2123,22 @@
         <v>1081826</v>
       </c>
       <c r="C39">
-        <v>1228021528.4968178</v>
+        <v>1232316036.163868</v>
       </c>
       <c r="D39">
         <v>0</v>
       </c>
       <c r="E39">
-        <v>121214246.22414552</v>
+        <v>120131976.16857277</v>
       </c>
       <c r="F39">
-        <v>1135.137747194852</v>
+        <v>1139.1074314759194</v>
       </c>
       <c r="G39">
         <v>0</v>
       </c>
       <c r="H39">
-        <v>112.04597247999726</v>
+        <v>111.04556201142584</v>
       </c>
       <c r="I39" t="s">
         <v>19</v>
@@ -2164,22 +2164,22 @@
         <v>250729</v>
       </c>
       <c r="C40">
-        <v>213853454.668464</v>
+        <v>211553609.125772</v>
       </c>
       <c r="D40">
         <v>0</v>
       </c>
       <c r="E40">
-        <v>125489774.42519563</v>
+        <v>123942642.25674765</v>
       </c>
       <c r="F40">
-        <v>852.9266844619649</v>
+        <v>843.7540496941798</v>
       </c>
       <c r="G40">
         <v>0</v>
       </c>
       <c r="H40">
-        <v>500.49964074836032</v>
+        <v>494.32910535577315</v>
       </c>
       <c r="I40" t="s">
         <v>19</v>
@@ -2205,22 +2205,22 @@
         <v>750815</v>
       </c>
       <c r="C41">
-        <v>1069046027.5422956</v>
+        <v>1078935119.73879</v>
       </c>
       <c r="D41">
-        <v>75171.873464096658</v>
+        <v>76786.125852752331</v>
       </c>
       <c r="E41">
-        <v>4378066.0799112963</v>
+        <v>4377371.5499615343</v>
       </c>
       <c r="F41">
-        <v>1423.8474558210685</v>
+        <v>1437.0185994403282</v>
       </c>
       <c r="G41">
-        <v>0.10012036715315578</v>
+        <v>0.10227036733782933</v>
       </c>
       <c r="H41">
-        <v>5.8310849941880436</v>
+        <v>5.8301599594594329</v>
       </c>
       <c r="I41" t="s">
         <v>19</v>
@@ -2246,22 +2246,22 @@
         <v>384251</v>
       </c>
       <c r="C42">
-        <v>450846813.29588914</v>
+        <v>451341199.58545798</v>
       </c>
       <c r="D42">
         <v>0</v>
       </c>
       <c r="E42">
-        <v>41924888.406381831</v>
+        <v>43097994.246130235</v>
       </c>
       <c r="F42">
-        <v>1173.3133116007223</v>
+        <v>1174.5999349005156</v>
       </c>
       <c r="G42">
         <v>0</v>
       </c>
       <c r="H42">
-        <v>109.10807885049572</v>
+        <v>112.16104641531248</v>
       </c>
       <c r="I42" t="s">
         <v>20</v>
@@ -2287,22 +2287,22 @@
         <v>1245893</v>
       </c>
       <c r="C43">
-        <v>7150544287.2708693</v>
+        <v>7257153106.3116627</v>
       </c>
       <c r="D43">
         <v>0</v>
       </c>
       <c r="E43">
-        <v>587679037.19876909</v>
+        <v>597568456.12493277</v>
       </c>
       <c r="F43">
-        <v>5739.2924490874166</v>
+        <v>5824.8606471917437</v>
       </c>
       <c r="G43">
         <v>0</v>
       </c>
       <c r="H43">
-        <v>471.69302435985202</v>
+        <v>479.63063932852401</v>
       </c>
       <c r="I43" t="s">
         <v>21</v>
@@ -2328,22 +2328,22 @@
         <v>827980</v>
       </c>
       <c r="C44">
-        <v>5702155585.5517368</v>
+        <v>5780606616.3963718</v>
       </c>
       <c r="D44">
-        <v>368715.9270567646</v>
+        <v>366742.3910890214</v>
       </c>
       <c r="E44">
-        <v>6275117.7333829524</v>
+        <v>6384901.7706605047</v>
       </c>
       <c r="F44">
-        <v>6886.8276837021867</v>
+        <v>6981.5775941404045</v>
       </c>
       <c r="G44">
-        <v>0.4453198471663139</v>
+        <v>0.44293629204693519</v>
       </c>
       <c r="H44">
-        <v>7.5788276690052321</v>
+        <v>7.7114202887273908</v>
       </c>
       <c r="I44" t="s">
         <v>21</v>
@@ -2369,22 +2369,22 @@
         <v>2177256</v>
       </c>
       <c r="C45">
-        <v>11086117265.468529</v>
+        <v>11122552593.234623</v>
       </c>
       <c r="D45">
-        <v>658334.8644189043</v>
+        <v>653691.58476331155</v>
       </c>
       <c r="E45">
-        <v>10643315.216437191</v>
+        <v>10030286.072410025</v>
       </c>
       <c r="F45">
-        <v>5091.7840003511428</v>
+        <v>5108.5185174525286</v>
       </c>
       <c r="G45">
-        <v>0.30236906657687673</v>
+        <v>0.30023643740713613</v>
       </c>
       <c r="H45">
-        <v>4.8884078015801498</v>
+        <v>4.606847367700456</v>
       </c>
       <c r="I45" t="s">
         <v>21</v>
@@ -2410,22 +2410,22 @@
         <v>2300225</v>
       </c>
       <c r="C46">
-        <v>24310737344.527786</v>
+        <v>24536211546.49699</v>
       </c>
       <c r="D46">
-        <v>1582144.1762843346</v>
+        <v>1560435.975009206</v>
       </c>
       <c r="E46">
-        <v>28286341.097706962</v>
+        <v>26882696.935623042</v>
       </c>
       <c r="F46">
-        <v>10568.851892544331</v>
+        <v>10666.874565095584</v>
       </c>
       <c r="G46">
-        <v>0.68782148541309418</v>
+        <v>0.67838406025897724</v>
       </c>
       <c r="H46">
-        <v>12.29720618535446</v>
+        <v>11.686985810354658</v>
       </c>
       <c r="I46" t="s">
         <v>21</v>
@@ -2451,22 +2451,22 @@
         <v>12008149</v>
       </c>
       <c r="C47">
-        <v>73036165212.535141</v>
+        <v>73661016427.011932</v>
       </c>
       <c r="D47">
-        <v>4608698.7278117798</v>
+        <v>4505761.035570614</v>
       </c>
       <c r="E47">
-        <v>73986911.006608963</v>
+        <v>73176218.013401702</v>
       </c>
       <c r="F47">
-        <v>6082.2167690070419</v>
+        <v>6134.2523670394103</v>
       </c>
       <c r="G47">
-        <v>0.38379759676631092</v>
+        <v>0.37522527706565051</v>
       </c>
       <c r="H47">
-        <v>6.1613918187231826</v>
+        <v>6.0938799154975261</v>
       </c>
       <c r="I47" t="s">
         <v>21</v>
@@ -2492,22 +2492,22 @@
         <v>1488285</v>
       </c>
       <c r="C48">
-        <v>7562955562.3399963</v>
+        <v>7610533398.3831139</v>
       </c>
       <c r="D48">
-        <v>470598.15804080514</v>
+        <v>479420.29107349599</v>
       </c>
       <c r="E48">
-        <v>8046599.9405146362</v>
+        <v>7851675.7136930795</v>
       </c>
       <c r="F48">
-        <v>5081.6581248483972</v>
+        <v>5113.6263540807804</v>
       </c>
       <c r="G48">
-        <v>0.31620164017026653</v>
+        <v>0.32212935766569978</v>
       </c>
       <c r="H48">
-        <v>5.4066257071156638</v>
+        <v>5.2756533282893256</v>
       </c>
       <c r="I48" t="s">
         <v>21</v>
@@ -2533,22 +2533,22 @@
         <v>48329</v>
       </c>
       <c r="C49">
-        <v>183569558.06282288</v>
+        <v>186638374.23899785</v>
       </c>
       <c r="D49">
         <v>0</v>
       </c>
       <c r="E49">
-        <v>16081217.409228683</v>
+        <v>15849315.425414257</v>
       </c>
       <c r="F49">
-        <v>3798.3313965284378</v>
+        <v>3861.8298379647385</v>
       </c>
       <c r="G49">
         <v>0</v>
       </c>
       <c r="H49">
-        <v>332.74467523078653</v>
+        <v>327.94627295028363</v>
       </c>
       <c r="I49" t="s">
         <v>21</v>
@@ -2574,22 +2574,22 @@
         <v>1336530</v>
       </c>
       <c r="C50">
-        <v>2638937670.0913868</v>
+        <v>2646162022.0033622</v>
       </c>
       <c r="D50">
         <v>0</v>
       </c>
       <c r="E50">
-        <v>249326695.16489828</v>
+        <v>248900769.3409619</v>
       </c>
       <c r="F50">
-        <v>1974.4694620333153</v>
+        <v>1979.8747667492403</v>
       </c>
       <c r="G50">
         <v>0</v>
       </c>
       <c r="H50">
-        <v>186.54777308769596</v>
+        <v>186.2290927558393</v>
       </c>
       <c r="I50" t="s">
         <v>22</v>
@@ -2615,22 +2615,22 @@
         <v>4238250</v>
       </c>
       <c r="C51">
-        <v>23244280326.908901</v>
+        <v>23280385211.816986</v>
       </c>
       <c r="D51">
-        <v>1417946.9146312191</v>
+        <v>1493418.1715308931</v>
       </c>
       <c r="E51">
-        <v>24216894.190404572</v>
+        <v>24396320.721262217</v>
       </c>
       <c r="F51">
-        <v>5484.4051971707431</v>
+        <v>5492.9240162371225</v>
       </c>
       <c r="G51">
-        <v>0.33455952684037493</v>
+        <v>0.35236670124010927</v>
       </c>
       <c r="H51">
-        <v>5.7138899759109467</v>
+        <v>5.7562250271367228</v>
       </c>
       <c r="I51" t="s">
         <v>22</v>
@@ -2656,22 +2656,22 @@
         <v>1825199</v>
       </c>
       <c r="C52">
-        <v>1515842974.0806546</v>
+        <v>1466432823.0133204</v>
       </c>
       <c r="D52">
         <v>0</v>
       </c>
       <c r="E52">
-        <v>130712440.42785226</v>
+        <v>126826518.58768968</v>
       </c>
       <c r="F52">
-        <v>830.50833036871848</v>
+        <v>803.43722685215175</v>
       </c>
       <c r="G52">
         <v>0</v>
       </c>
       <c r="H52">
-        <v>71.615446002245378</v>
+        <v>69.486405913924827</v>
       </c>
       <c r="I52" t="s">
         <v>23</v>
@@ -2697,22 +2697,22 @@
         <v>7101778</v>
       </c>
       <c r="C53">
-        <v>6897926903.1154308</v>
+        <v>6870070980.0868759</v>
       </c>
       <c r="D53">
         <v>0</v>
       </c>
       <c r="E53">
-        <v>582212393.87606871</v>
+        <v>591845557.97644615</v>
       </c>
       <c r="F53">
-        <v>971.29576609060871</v>
+        <v>967.3733789041105</v>
       </c>
       <c r="G53">
         <v>0</v>
       </c>
       <c r="H53">
-        <v>81.981215672479308</v>
+        <v>83.337659664445454</v>
       </c>
       <c r="I53" t="s">
         <v>23</v>
@@ -2738,22 +2738,22 @@
         <v>992174</v>
       </c>
       <c r="C54">
-        <v>1357370009.6343436</v>
+        <v>1389183576.7812204</v>
       </c>
       <c r="D54">
         <v>0</v>
       </c>
       <c r="E54">
-        <v>118343268.5449585</v>
+        <v>123474053.2249352</v>
       </c>
       <c r="F54">
-        <v>1368.0765769253615</v>
+        <v>1400.1410808801888</v>
       </c>
       <c r="G54">
         <v>0</v>
       </c>
       <c r="H54">
-        <v>119.27672822000828</v>
+        <v>124.44798314099664</v>
       </c>
       <c r="I54" t="s">
         <v>23</v>
@@ -2779,22 +2779,22 @@
         <v>1769518</v>
       </c>
       <c r="C55">
-        <v>2007630817.0455651</v>
+        <v>2018322936.4008334</v>
       </c>
       <c r="D55">
         <v>0</v>
       </c>
       <c r="E55">
-        <v>191604239.05539438</v>
+        <v>193202520.74818236</v>
       </c>
       <c r="F55">
-        <v>1134.5636591690873</v>
+        <v>1140.6060500095696</v>
       </c>
       <c r="G55">
         <v>0</v>
       </c>
       <c r="H55">
-        <v>108.28046906298459</v>
+        <v>109.18369903452938</v>
       </c>
       <c r="I55" t="s">
         <v>23</v>
@@ -2820,22 +2820,22 @@
         <v>16149545</v>
       </c>
       <c r="C56">
-        <v>41208624388.292206</v>
+        <v>41327323171.237564</v>
       </c>
       <c r="D56">
-        <v>2461590.6964787683</v>
+        <v>2473614.0768450201</v>
       </c>
       <c r="E56">
-        <v>43911601.74420625</v>
+        <v>43107855.330394521</v>
       </c>
       <c r="F56">
-        <v>2551.6894988863282</v>
+        <v>2559.0394758017992</v>
       </c>
       <c r="G56">
-        <v>0.1524247708823232</v>
+        <v>0.15316927361390181</v>
       </c>
       <c r="H56">
-        <v>2.719061233254946</v>
+        <v>2.6692922512921893</v>
       </c>
       <c r="I56" t="s">
         <v>23</v>
@@ -2861,22 +2861,22 @@
         <v>1806150</v>
       </c>
       <c r="C57">
-        <v>3636127031.9477119</v>
+        <v>3640988883.5161839</v>
       </c>
       <c r="D57">
         <v>0</v>
       </c>
       <c r="E57">
-        <v>317006263.44653302</v>
+        <v>309558094.69011259</v>
       </c>
       <c r="F57">
-        <v>2013.1921667346078</v>
+        <v>2015.8839982926024</v>
       </c>
       <c r="G57">
         <v>0</v>
       </c>
       <c r="H57">
-        <v>175.51491484457716</v>
+        <v>171.39113290153784</v>
       </c>
       <c r="I57" t="s">
         <v>23</v>
@@ -2902,22 +2902,22 @@
         <v>5446539</v>
       </c>
       <c r="C58">
-        <v>34605436602.367111</v>
+        <v>35065210138.136719</v>
       </c>
       <c r="D58">
         <v>0</v>
       </c>
       <c r="E58">
-        <v>2754981916.4431038</v>
+        <v>2750281812.8034263</v>
       </c>
       <c r="F58">
-        <v>6353.6562581057642</v>
+        <v>6438.0719826180848</v>
       </c>
       <c r="G58">
         <v>0</v>
       </c>
       <c r="H58">
-        <v>505.82248955586363</v>
+        <v>504.95953720397966</v>
       </c>
       <c r="I58" t="s">
         <v>23</v>
@@ -2943,22 +2943,22 @@
         <v>2101351</v>
       </c>
       <c r="C59">
-        <v>4084225289.4211454</v>
+        <v>4142944769.5202408</v>
       </c>
       <c r="D59">
         <v>0</v>
       </c>
       <c r="E59">
-        <v>340466917.20926237</v>
+        <v>343073795.26559734</v>
       </c>
       <c r="F59">
-        <v>1943.6187906833011</v>
+        <v>1971.5624707724892</v>
       </c>
       <c r="G59">
         <v>0</v>
       </c>
       <c r="H59">
-        <v>162.02286872077173</v>
+        <v>163.26344112221011</v>
       </c>
       <c r="I59" t="s">
         <v>23</v>
@@ -2987,19 +2987,19 @@
         <v>330666585.89536315</v>
       </c>
       <c r="D60">
-        <v>27716.971288133063</v>
+        <v>23636.475406808386</v>
       </c>
       <c r="E60">
-        <v>516143.52713702142</v>
+        <v>513126.51337785792</v>
       </c>
       <c r="F60">
         <v>1609.8116709526118</v>
       </c>
       <c r="G60">
-        <v>0.13493683899834505</v>
+        <v>0.11507142116290285</v>
       </c>
       <c r="H60">
-        <v>2.5127845065505139</v>
+        <v>2.4980965272744253</v>
       </c>
       <c r="I60" t="s">
         <v>23</v>
@@ -3025,22 +3025,22 @@
         <v>500876</v>
       </c>
       <c r="C61">
-        <v>622308643.63224947</v>
+        <v>611094336.38496614</v>
       </c>
       <c r="D61">
         <v>0</v>
       </c>
       <c r="E61">
-        <v>59879580.207631305</v>
+        <v>58466210.330757692</v>
       </c>
       <c r="F61">
-        <v>1242.4405314533926</v>
+        <v>1220.0511431671034</v>
       </c>
       <c r="G61">
         <v>0</v>
       </c>
       <c r="H61">
-        <v>119.54970932452603</v>
+        <v>116.72791335731337</v>
       </c>
       <c r="I61" t="s">
         <v>23</v>
@@ -3066,22 +3066,22 @@
         <v>869762</v>
       </c>
       <c r="C62">
-        <v>999338636.91433191</v>
+        <v>994354404.31126797</v>
       </c>
       <c r="D62">
         <v>0</v>
       </c>
       <c r="E62">
-        <v>96721996.318200037</v>
+        <v>94201996.197909668</v>
       </c>
       <c r="F62">
-        <v>1148.9794184090956</v>
+        <v>1143.2488477437137</v>
       </c>
       <c r="G62">
         <v>0</v>
       </c>
       <c r="H62">
-        <v>111.20513004500086</v>
+        <v>108.30778557572033</v>
       </c>
       <c r="I62" t="s">
         <v>23</v>
@@ -3107,22 +3107,22 @@
         <v>296202</v>
       </c>
       <c r="C63">
-        <v>250812025.54796636</v>
+        <v>245714088.76657572</v>
       </c>
       <c r="D63">
         <v>0</v>
       </c>
       <c r="E63">
-        <v>21201885.722224906</v>
+        <v>21118611.623245534</v>
       </c>
       <c r="F63">
-        <v>846.7600676159052</v>
+        <v>829.54905357349287</v>
       </c>
       <c r="G63">
         <v>0</v>
       </c>
       <c r="H63">
-        <v>71.579144375206468</v>
+        <v>71.298004818487158</v>
       </c>
       <c r="I63" t="s">
         <v>24</v>
@@ -3148,22 +3148,22 @@
         <v>1615868</v>
       </c>
       <c r="C64">
-        <v>1473280310.8439538</v>
+        <v>1460632800.4840896</v>
       </c>
       <c r="D64">
         <v>0</v>
       </c>
       <c r="E64">
-        <v>132928541.92131743</v>
+        <v>125124239.63254012</v>
       </c>
       <c r="F64">
-        <v>911.75783593954077</v>
+        <v>903.93076692161094</v>
       </c>
       <c r="G64">
         <v>0</v>
       </c>
       <c r="H64">
-        <v>82.26448071334876</v>
+        <v>77.434691220161625</v>
       </c>
       <c r="I64" t="s">
         <v>25</v>
@@ -3189,22 +3189,22 @@
         <v>1420063</v>
       </c>
       <c r="C65">
-        <v>1701840070.8304718</v>
+        <v>1703556899.6877995</v>
       </c>
       <c r="D65">
         <v>0</v>
       </c>
       <c r="E65">
-        <v>164720140.26954892</v>
+        <v>164336859.79713625</v>
       </c>
       <c r="F65">
-        <v>1198.4257535267602</v>
+        <v>1199.6347342954498</v>
       </c>
       <c r="G65">
         <v>0</v>
       </c>
       <c r="H65">
-        <v>115.99495252643645</v>
+        <v>115.7250486754012</v>
       </c>
       <c r="I65" t="s">
         <v>26</v>
@@ -3230,22 +3230,22 @@
         <v>2037047</v>
       </c>
       <c r="C66">
-        <v>1933090065.1818376</v>
+        <v>1949344590.5758328</v>
       </c>
       <c r="D66">
         <v>0</v>
       </c>
       <c r="E66">
-        <v>163262061.46051437</v>
+        <v>160163925.49184996</v>
       </c>
       <c r="F66">
-        <v>948.96684523324086</v>
+        <v>956.94630049077557</v>
       </c>
       <c r="G66">
         <v>0</v>
       </c>
       <c r="H66">
-        <v>80.146438182582116</v>
+        <v>78.625542509254799</v>
       </c>
       <c r="I66" t="s">
         <v>26</v>
@@ -3277,7 +3277,7 @@
         <v>0</v>
       </c>
       <c r="E67">
-        <v>11457490.089074763</v>
+        <v>11187095.552819559</v>
       </c>
       <c r="F67">
         <v>506.84632329731045</v>
@@ -3286,7 +3286,7 @@
         <v>0</v>
       </c>
       <c r="H67">
-        <v>49.068480038864081</v>
+        <v>47.910473459612675</v>
       </c>
       <c r="I67" t="s">
         <v>26</v>
@@ -3312,22 +3312,22 @@
         <v>16042082</v>
       </c>
       <c r="C68">
-        <v>16772312795.696297</v>
+        <v>16812594024.452826</v>
       </c>
       <c r="D68">
         <v>0</v>
       </c>
       <c r="E68">
-        <v>1609384689.3525987</v>
+        <v>1602349332.6473701</v>
       </c>
       <c r="F68">
-        <v>1045.5197022242062</v>
+        <v>1048.0306748496128</v>
       </c>
       <c r="G68">
         <v>0</v>
       </c>
       <c r="H68">
-        <v>100.3226818908293</v>
+        <v>99.884125554735988</v>
       </c>
       <c r="I68" t="s">
         <v>26</v>
@@ -3353,22 +3353,22 @@
         <v>2119428</v>
       </c>
       <c r="C69">
-        <v>2468855124.6599083</v>
+        <v>2473003720.2582598</v>
       </c>
       <c r="D69">
         <v>0</v>
       </c>
       <c r="E69">
-        <v>239166044.18590999</v>
+        <v>237654290.77300692</v>
       </c>
       <c r="F69">
-        <v>1164.8685988200157</v>
+        <v>1166.826011668365</v>
       </c>
       <c r="G69">
         <v>0</v>
       </c>
       <c r="H69">
-        <v>112.84461854137531</v>
+        <v>112.13133485686087</v>
       </c>
       <c r="I69" t="s">
         <v>26</v>
@@ -3394,22 +3394,22 @@
         <v>4495381</v>
       </c>
       <c r="C70">
-        <v>8607437145.9593372</v>
+        <v>8532148223.7443237</v>
       </c>
       <c r="D70">
-        <v>533558.13926516497</v>
+        <v>524274.95510363573</v>
       </c>
       <c r="E70">
-        <v>8798881.5729345549</v>
+        <v>8514761.4875421785</v>
       </c>
       <c r="F70">
-        <v>1914.7291733357722</v>
+        <v>1897.9811107766668</v>
       </c>
       <c r="G70">
-        <v>0.11869030439581539</v>
+        <v>0.11662525492358394</v>
       </c>
       <c r="H70">
-        <v>1.9573160924367823</v>
+        <v>1.8941134216526205</v>
       </c>
       <c r="I70" t="s">
         <v>26</v>
@@ -3476,22 +3476,22 @@
         <v>6594728</v>
       </c>
       <c r="C72">
-        <v>7085344768.9259186</v>
+        <v>7030056378.302597</v>
       </c>
       <c r="D72">
         <v>0</v>
       </c>
       <c r="E72">
-        <v>679721019.80724704</v>
+        <v>687719674.04817295</v>
       </c>
       <c r="F72">
-        <v>1074.3953001436782</v>
+        <v>1066.0115744428879</v>
       </c>
       <c r="G72">
         <v>0</v>
       </c>
       <c r="H72">
-        <v>103.07036466208265</v>
+        <v>104.28325081006722</v>
       </c>
       <c r="I72" t="s">
         <v>26</v>
@@ -3517,22 +3517,22 @@
         <v>7672769</v>
       </c>
       <c r="C73">
-        <v>8266906511.4709949</v>
+        <v>8268093837.5213861</v>
       </c>
       <c r="D73">
         <v>0</v>
       </c>
       <c r="E73">
-        <v>786088293.32903552</v>
+        <v>790003691.16176319</v>
       </c>
       <c r="F73">
-        <v>1077.4345626032784</v>
+        <v>1077.5893080479011</v>
       </c>
       <c r="G73">
         <v>0</v>
       </c>
       <c r="H73">
-        <v>102.45170854603279</v>
+        <v>102.96200643623744</v>
       </c>
       <c r="I73" t="s">
         <v>26</v>
@@ -3558,22 +3558,22 @@
         <v>306727</v>
       </c>
       <c r="C74">
-        <v>151757416.51667878</v>
+        <v>150296070.25339317</v>
       </c>
       <c r="D74">
         <v>0</v>
       </c>
       <c r="E74">
-        <v>140083769.09231886</v>
+        <v>138734834.08005524</v>
       </c>
       <c r="F74">
-        <v>494.76380141519587</v>
+        <v>489.99947918961544</v>
       </c>
       <c r="G74">
         <v>0</v>
       </c>
       <c r="H74">
-        <v>456.70504746018077</v>
+        <v>452.307211559645</v>
       </c>
       <c r="I74" t="s">
         <v>10</v>
@@ -3599,22 +3599,22 @@
         <v>3095082</v>
       </c>
       <c r="C75">
-        <v>3797056685.1019464</v>
+        <v>3753897314.5088596</v>
       </c>
       <c r="D75">
         <v>0</v>
       </c>
       <c r="E75">
-        <v>368343511.43114221</v>
+        <v>360646594.38061333</v>
       </c>
       <c r="F75">
-        <v>1226.8032592034544</v>
+        <v>1212.8587593184477</v>
       </c>
       <c r="G75">
         <v>0</v>
       </c>
       <c r="H75">
-        <v>119.00929003856513</v>
+        <v>116.52246834837116</v>
       </c>
       <c r="I75" t="s">
         <v>10</v>
@@ -3640,22 +3640,22 @@
         <v>134547</v>
       </c>
       <c r="C76">
-        <v>734528397.58288193</v>
+        <v>728371258.23833895</v>
       </c>
       <c r="D76">
-        <v>50531.18931826108</v>
+        <v>45686.367706183082</v>
       </c>
       <c r="E76">
-        <v>880147.05082734313</v>
+        <v>774741.94258873514</v>
       </c>
       <c r="F76">
-        <v>5459.2699769068204</v>
+        <v>5413.5079803959879</v>
       </c>
       <c r="G76">
-        <v>0.37556533641226547</v>
+        <v>0.3395569407432576</v>
       </c>
       <c r="H76">
-        <v>6.5415583463573554</v>
+        <v>5.7581509999385725</v>
       </c>
       <c r="I76" t="s">
         <v>27</v>
@@ -3681,22 +3681,22 @@
         <v>531521</v>
       </c>
       <c r="C77">
-        <v>3103450112.0281372</v>
+        <v>3099434774.9028263</v>
       </c>
       <c r="D77">
-        <v>195151.95253217922</v>
+        <v>190840.2552102693</v>
       </c>
       <c r="E77">
-        <v>3597740.5189629034</v>
+        <v>3571424.3018528367</v>
       </c>
       <c r="F77">
-        <v>5838.8099661690458</v>
+        <v>5831.2555381684379</v>
       </c>
       <c r="G77">
-        <v>0.36715755827555113</v>
+        <v>0.3590455602135556</v>
       </c>
       <c r="H77">
-        <v>6.7687645811979271</v>
+        <v>6.7192534290326007</v>
       </c>
       <c r="I77" t="s">
         <v>28</v>
@@ -3722,22 +3722,22 @@
         <v>1438500</v>
       </c>
       <c r="C78">
-        <v>9527313405.5729351</v>
+        <v>9588614587.4529305</v>
       </c>
       <c r="D78">
-        <v>629810.07024677773</v>
+        <v>624331.62204713176</v>
       </c>
       <c r="E78">
-        <v>10582650.650748828</v>
+        <v>10562847.295436576</v>
       </c>
       <c r="F78">
-        <v>6623.0889159353046</v>
+        <v>6665.7035713958503</v>
       </c>
       <c r="G78">
-        <v>0.43782417118302241</v>
+        <v>0.43401572613634465</v>
       </c>
       <c r="H78">
-        <v>7.3567262083759672</v>
+        <v>7.3429595380163892</v>
       </c>
       <c r="I78" t="s">
         <v>29</v>
@@ -3763,22 +3763,22 @@
         <v>4871389</v>
       </c>
       <c r="C79">
-        <v>24578150165.469845</v>
+        <v>24919933273.956844</v>
       </c>
       <c r="D79">
-        <v>1395824.7679576497</v>
+        <v>1439611.1084915141</v>
       </c>
       <c r="E79">
-        <v>23748724.380702619</v>
+        <v>25554725.555442598</v>
       </c>
       <c r="F79">
-        <v>5045.4090538591445</v>
+        <v>5115.5703791992064</v>
       </c>
       <c r="G79">
-        <v>0.28653527114292243</v>
+        <v>0.29552374250783792</v>
       </c>
       <c r="H79">
-        <v>4.8751443131933456</v>
+        <v>5.2458807037258977</v>
       </c>
       <c r="I79" t="s">
         <v>29</v>
@@ -3804,22 +3804,22 @@
         <v>1656996</v>
       </c>
       <c r="C80">
-        <v>8621582161.141552</v>
+        <v>8614146770.4875431</v>
       </c>
       <c r="D80">
-        <v>520233.17588493519</v>
+        <v>514303.38599995093</v>
       </c>
       <c r="E80">
-        <v>9664451.0799634121</v>
+        <v>9802833.0126781799</v>
       </c>
       <c r="F80">
-        <v>5203.1399961988755</v>
+        <v>5198.6527248632729</v>
       </c>
       <c r="G80">
-        <v>0.31396163653076725</v>
+        <v>0.31038299790702628</v>
       </c>
       <c r="H80">
-        <v>5.8325132227014498</v>
+        <v>5.9160269624538504</v>
       </c>
       <c r="I80" t="s">
         <v>29</v>
@@ -3845,22 +3845,22 @@
         <v>967351</v>
       </c>
       <c r="C81">
-        <v>6509694112.6033192</v>
+        <v>6461620822.5435209</v>
       </c>
       <c r="D81">
-        <v>380495.01827665581</v>
+        <v>383624.72019366396</v>
       </c>
       <c r="E81">
-        <v>6302476.6917944327</v>
+        <v>6974562.0787803736</v>
       </c>
       <c r="F81">
-        <v>6729.4023706010739</v>
+        <v>6679.7065620891699</v>
       </c>
       <c r="G81">
-        <v>0.39333708062187955</v>
+        <v>0.39657241290251827</v>
       </c>
       <c r="H81">
-        <v>6.5151911682465133</v>
+        <v>7.2099600649406197</v>
       </c>
       <c r="I81" t="s">
         <v>29</v>
@@ -3886,22 +3886,22 @@
         <v>7658910</v>
       </c>
       <c r="C82">
-        <v>35272486068.170151</v>
+        <v>34470685408.441223</v>
       </c>
       <c r="D82">
-        <v>2177080.6700207121</v>
+        <v>2124944.3411712185</v>
       </c>
       <c r="E82">
-        <v>42194189.296797574</v>
+        <v>40637685.547053471</v>
       </c>
       <c r="F82">
-        <v>4605.4185345134165</v>
+        <v>4500.7299222005777</v>
       </c>
       <c r="G82">
-        <v>0.28425463545344076</v>
+        <v>0.27744735754450939</v>
       </c>
       <c r="H82">
-        <v>5.5091637448145461</v>
+        <v>5.305935903027124</v>
       </c>
       <c r="I82" t="s">
         <v>29</v>
@@ -3927,22 +3927,22 @@
         <v>500630</v>
       </c>
       <c r="C83">
-        <v>2716744085.6717839</v>
+        <v>2725929947.2674451</v>
       </c>
       <c r="D83">
         <v>0</v>
       </c>
       <c r="E83">
-        <v>219364430.63715208</v>
+        <v>217117725.06419396</v>
       </c>
       <c r="F83">
-        <v>5426.6505915981543</v>
+        <v>5444.9991955484993</v>
       </c>
       <c r="G83">
         <v>0</v>
       </c>
       <c r="H83">
-        <v>438.17675855852042</v>
+        <v>433.68900198588574</v>
       </c>
       <c r="I83" t="s">
         <v>30</v>
@@ -3968,22 +3968,22 @@
         <v>3581670</v>
       </c>
       <c r="C84">
-        <v>20857201115.927502</v>
+        <v>20886264504.297894</v>
       </c>
       <c r="D84">
-        <v>1144948.2471166323</v>
+        <v>1171070.6242164974</v>
       </c>
       <c r="E84">
-        <v>18696720.394150905</v>
+        <v>18151785.151220843</v>
       </c>
       <c r="F84">
-        <v>5823.3173675764383</v>
+        <v>5831.4318472382702</v>
       </c>
       <c r="G84">
-        <v>0.31966882686473974</v>
+        <v>0.32696217803887501</v>
       </c>
       <c r="H84">
-        <v>5.2201125157121968</v>
+        <v>5.0679669403437062</v>
       </c>
       <c r="I84" t="s">
         <v>30</v>
@@ -4009,19 +4009,19 @@
         <v>4902363</v>
       </c>
       <c r="C85">
-        <v>37717043764.634956</v>
+        <v>34409584401.703629</v>
       </c>
       <c r="D85">
-        <v>1989614.9927260079</v>
+        <v>1945944.8634491358</v>
       </c>
       <c r="E85">
         <v>34275124.305252805</v>
       </c>
       <c r="F85">
-        <v>7693.6456489727416</v>
+        <v>7018.9792966582909</v>
       </c>
       <c r="G85">
-        <v>0.40584815786305661</v>
+        <v>0.39694018240777679</v>
       </c>
       <c r="H85">
         <v>6.9915516874725121</v>
@@ -4050,22 +4050,22 @@
         <v>8835500</v>
       </c>
       <c r="C86">
-        <v>45952653149.089622</v>
+        <v>46777520043.067787</v>
       </c>
       <c r="D86">
-        <v>7899336.4751523491</v>
+        <v>8088812.5346621498</v>
       </c>
       <c r="E86">
-        <v>153463690.13458154</v>
+        <v>147615809.31886861</v>
       </c>
       <c r="F86">
-        <v>5200.9114536913157</v>
+        <v>5294.2697123046555</v>
       </c>
       <c r="G86">
-        <v>0.89404521251229119</v>
+        <v>0.91549007239682534</v>
       </c>
       <c r="H86">
-        <v>17.368987622045331</v>
+        <v>16.707125722241933</v>
       </c>
       <c r="I86" t="s">
         <v>31</v>
@@ -4091,22 +4091,22 @@
         <v>6233147</v>
       </c>
       <c r="C87">
-        <v>26186481492.60463</v>
+        <v>26162721145.82354</v>
       </c>
       <c r="D87">
-        <v>1571420.5213747283</v>
+        <v>1559688.1044381103</v>
       </c>
       <c r="E87">
-        <v>28969746.837189801</v>
+        <v>28016852.84849396</v>
       </c>
       <c r="F87">
-        <v>4201.1653972872182</v>
+        <v>4197.3534629976702</v>
       </c>
       <c r="G87">
-        <v>0.25210708513287561</v>
+        <v>0.25022482294066067</v>
       </c>
       <c r="H87">
-        <v>4.6476919022108421</v>
+        <v>4.4948166389295743</v>
       </c>
       <c r="I87" t="s">
         <v>31</v>
@@ -4132,22 +4132,22 @@
         <v>2753681</v>
       </c>
       <c r="C88">
-        <v>12004987434.696236</v>
+        <v>11895421123.76668</v>
       </c>
       <c r="D88">
         <v>0</v>
       </c>
       <c r="E88">
-        <v>991569937.51495445</v>
+        <v>961827708.46126676</v>
       </c>
       <c r="F88">
-        <v>4359.6144341687495</v>
+        <v>4319.8253987178177</v>
       </c>
       <c r="G88">
         <v>0</v>
       </c>
       <c r="H88">
-        <v>360.0888910207662</v>
+        <v>349.28799249487025</v>
       </c>
       <c r="I88" t="s">
         <v>31</v>
@@ -4173,22 +4173,22 @@
         <v>5168266</v>
       </c>
       <c r="C89">
-        <v>17744679411.502251</v>
+        <v>17584668350.292683</v>
       </c>
       <c r="D89">
-        <v>993483.20232611103</v>
+        <v>988947.31148653198</v>
       </c>
       <c r="E89">
-        <v>16598082.17993639</v>
+        <v>16708326.177034609</v>
       </c>
       <c r="F89">
-        <v>3433.3912789129372</v>
+        <v>3402.4309798088339</v>
       </c>
       <c r="G89">
-        <v>0.19222756768442473</v>
+        <v>0.1913499250012542</v>
       </c>
       <c r="H89">
-        <v>3.2115379084467381</v>
+        <v>3.2328688533126213</v>
       </c>
       <c r="I89" t="s">
         <v>31</v>
@@ -4214,22 +4214,22 @@
         <v>9849064</v>
       </c>
       <c r="C90">
-        <v>52601120515.847397</v>
+        <v>52911629082.147911</v>
       </c>
       <c r="D90">
-        <v>3049912.5410577385</v>
+        <v>3093892.842112714</v>
       </c>
       <c r="E90">
-        <v>52568079.099117294</v>
+        <v>53176630.148461223</v>
       </c>
       <c r="F90">
-        <v>5340.7227850126055</v>
+        <v>5372.2494931648234</v>
       </c>
       <c r="G90">
-        <v>0.30966521702546945</v>
+        <v>0.31413064653785516</v>
       </c>
       <c r="H90">
-        <v>5.3373680076723327</v>
+        <v>5.3991557114931146</v>
       </c>
       <c r="I90" t="s">
         <v>31</v>
@@ -4255,22 +4255,22 @@
         <v>6246911</v>
       </c>
       <c r="C91">
-        <v>30288058646.71949</v>
+        <v>29912126620.518883</v>
       </c>
       <c r="D91">
-        <v>1799639.1844831179</v>
+        <v>1793041.4489864483</v>
       </c>
       <c r="E91">
-        <v>32777034.931335457</v>
+        <v>32494226.130202021</v>
       </c>
       <c r="F91">
-        <v>4848.4856990470153</v>
+        <v>4788.3068320516941</v>
       </c>
       <c r="G91">
-        <v>0.28808465247593856</v>
+        <v>0.28702849280011328</v>
       </c>
       <c r="H91">
-        <v>5.2469188261743218</v>
+        <v>5.2016470428667896</v>
       </c>
       <c r="I91" t="s">
         <v>31</v>
@@ -4296,22 +4296,22 @@
         <v>3681044</v>
       </c>
       <c r="C92">
-        <v>16386335922.480608</v>
+        <v>16572232452.390163</v>
       </c>
       <c r="D92">
-        <v>1087076.2390119007</v>
+        <v>1090933.3290594337</v>
       </c>
       <c r="E92">
-        <v>16905717.091036901</v>
+        <v>17266804.967155807</v>
       </c>
       <c r="F92">
-        <v>4451.5457904009318</v>
+        <v>4502.0468248654897</v>
       </c>
       <c r="G92">
-        <v>0.29531737165105898</v>
+        <v>0.2963651966831784</v>
       </c>
       <c r="H92">
-        <v>4.5926419491418473</v>
+        <v>4.6907358258026273</v>
       </c>
       <c r="I92" t="s">
         <v>31</v>
@@ -4337,22 +4337,22 @@
         <v>4626240</v>
       </c>
       <c r="C93">
-        <v>4867091779.0211535</v>
+        <v>4938232800.2314663</v>
       </c>
       <c r="D93">
         <v>0</v>
       </c>
       <c r="E93">
-        <v>468631852.01106274</v>
+        <v>481318011.00471866</v>
       </c>
       <c r="F93">
-        <v>1052.0621020572114</v>
+        <v>1067.4398215897718</v>
       </c>
       <c r="G93">
         <v>0</v>
       </c>
       <c r="H93">
-        <v>101.29864685166847</v>
+        <v>104.04086493669128</v>
       </c>
       <c r="I93" t="s">
         <v>15</v>
@@ -4378,22 +4378,22 @@
         <v>6322841</v>
       </c>
       <c r="C94">
-        <v>7120943386.3922758</v>
+        <v>7133882790.7655869</v>
       </c>
       <c r="D94">
         <v>0</v>
       </c>
       <c r="E94">
-        <v>685720568.19362748</v>
+        <v>694801094.09035707</v>
       </c>
       <c r="F94">
-        <v>1126.2252817036322</v>
+        <v>1128.271735880372</v>
       </c>
       <c r="G94">
         <v>0</v>
       </c>
       <c r="H94">
-        <v>108.45133828189377</v>
+        <v>109.88748476995659</v>
       </c>
       <c r="I94" t="s">
         <v>15</v>
@@ -4419,22 +4419,22 @@
         <v>9036684</v>
       </c>
       <c r="C95">
-        <v>84640377905.838074</v>
+        <v>84771928792.091766</v>
       </c>
       <c r="D95">
-        <v>1956163.5054122107</v>
+        <v>1933363.4328747848</v>
       </c>
       <c r="E95">
-        <v>3768233667.6259503</v>
+        <v>3749476363.4505134</v>
       </c>
       <c r="F95">
-        <v>9366.3093570427027</v>
+        <v>9380.8667861011581</v>
       </c>
       <c r="G95">
-        <v>0.21646917225524437</v>
+        <v>0.21394611484420445</v>
       </c>
       <c r="H95">
-        <v>416.99296640514933</v>
+        <v>414.91728198645802</v>
       </c>
       <c r="I95" t="s">
         <v>32</v>
@@ -4460,22 +4460,22 @@
         <v>916991</v>
       </c>
       <c r="C96">
-        <v>8778175483.5641861</v>
+        <v>8905861731.5980453</v>
       </c>
       <c r="D96">
         <v>0</v>
       </c>
       <c r="E96">
-        <v>754644766.65718055</v>
+        <v>767043695.47001982</v>
       </c>
       <c r="F96">
-        <v>9572.8044043662212</v>
+        <v>9712.049225780891</v>
       </c>
       <c r="G96">
         <v>0</v>
       </c>
       <c r="H96">
-        <v>822.95765897067747</v>
+        <v>836.47897904125534</v>
       </c>
       <c r="I96" t="s">
         <v>32</v>
@@ -4501,22 +4501,22 @@
         <v>317344</v>
       </c>
       <c r="C97">
-        <v>2203748675.923028</v>
+        <v>2219409538.6199012</v>
       </c>
       <c r="D97">
         <v>0</v>
       </c>
       <c r="E97">
-        <v>186264150.20201263</v>
+        <v>186435597.97533229</v>
       </c>
       <c r="F97">
-        <v>6944.3527400014746</v>
+        <v>6993.7025392630749</v>
       </c>
       <c r="G97">
         <v>0</v>
       </c>
       <c r="H97">
-        <v>586.94713056497881</v>
+        <v>587.48738900162687</v>
       </c>
       <c r="I97" t="s">
         <v>32</v>
@@ -4542,22 +4542,22 @@
         <v>4078252</v>
       </c>
       <c r="C98">
-        <v>22622920616.807831</v>
+        <v>23069484449.998943</v>
       </c>
       <c r="D98">
-        <v>1335151.4880643066</v>
+        <v>1350452.556137081</v>
       </c>
       <c r="E98">
-        <v>22737737.164493274</v>
+        <v>23173694.900920525</v>
       </c>
       <c r="F98">
-        <v>5547.210083341547</v>
+        <v>5656.7089159764882</v>
       </c>
       <c r="G98">
-        <v>0.32738327304548775</v>
+        <v>0.33113514224650192</v>
       </c>
       <c r="H98">
-        <v>5.5753634558367837</v>
+        <v>5.6822616407520981</v>
       </c>
       <c r="I98" t="s">
         <v>32</v>
@@ -4583,22 +4583,22 @@
         <v>3399679</v>
       </c>
       <c r="C99">
-        <v>17756845212.651413</v>
+        <v>17813998849.980263</v>
       </c>
       <c r="D99">
-        <v>1132116.0091883158</v>
+        <v>1120769.9156904374</v>
       </c>
       <c r="E99">
-        <v>18651942.080812216</v>
+        <v>18763320.183896486</v>
       </c>
       <c r="F99">
-        <v>5223.0946547163458</v>
+        <v>5239.9061352499057</v>
       </c>
       <c r="G99">
-        <v>0.33300673657375179</v>
+        <v>0.32966933516088942</v>
       </c>
       <c r="H99">
-        <v>5.4863832970148696</v>
+        <v>5.5191446556855768</v>
       </c>
       <c r="I99" t="s">
         <v>32</v>
@@ -4624,22 +4624,22 @@
         <v>3734928</v>
       </c>
       <c r="C100">
-        <v>18501532253.954369</v>
+        <v>18510240447.171295</v>
       </c>
       <c r="D100">
-        <v>1112216.3124183146</v>
+        <v>1074478.1812998452</v>
       </c>
       <c r="E100">
-        <v>17921506.377608832</v>
+        <v>18722211.587212786</v>
       </c>
       <c r="F100">
-        <v>4953.651651103949</v>
+        <v>4955.9832069510567</v>
       </c>
       <c r="G100">
-        <v>0.29778788571515025</v>
+        <v>0.28768377363629105</v>
       </c>
       <c r="H100">
-        <v>4.7983539114030664</v>
+        <v>5.0127369489352365</v>
       </c>
       <c r="I100" t="s">
         <v>12</v>
@@ -4665,22 +4665,22 @@
         <v>2487210</v>
       </c>
       <c r="C101">
-        <v>20945120872.213665</v>
+        <v>21095127063.848053</v>
       </c>
       <c r="D101">
-        <v>1218598.4321859977</v>
+        <v>1203753.4570909953</v>
       </c>
       <c r="E101">
-        <v>23050705.901408106</v>
+        <v>22253426.769947082</v>
       </c>
       <c r="F101">
-        <v>8421.1308543362502</v>
+        <v>8481.4418822086009</v>
       </c>
       <c r="G101">
-        <v>0.48994593628443023</v>
+        <v>0.48397741127246807</v>
       </c>
       <c r="H101">
-        <v>9.2676958927505542</v>
+        <v>8.9471442982084675</v>
       </c>
       <c r="I101" t="s">
         <v>33</v>
@@ -4706,22 +4706,22 @@
         <v>14438617</v>
       </c>
       <c r="C102">
-        <v>43981676108.351997</v>
+        <v>44441870265.094589</v>
       </c>
       <c r="D102">
-        <v>2797242.9727432746</v>
+        <v>2794253.0032189162</v>
       </c>
       <c r="E102">
-        <v>49573923.444285281</v>
+        <v>51411474.290751114</v>
       </c>
       <c r="F102">
-        <v>3046.1141886616979</v>
+        <v>3077.9866427023162</v>
       </c>
       <c r="G102">
-        <v>0.19373344225027056</v>
+        <v>0.1935263608155072</v>
       </c>
       <c r="H102">
-        <v>3.4334260299504642</v>
+        <v>3.5606924327136813</v>
       </c>
       <c r="I102" t="s">
         <v>33</v>
@@ -4747,22 +4747,22 @@
         <v>2911161</v>
       </c>
       <c r="C103">
-        <v>3316278928.4001369</v>
+        <v>3317704801.0087538</v>
       </c>
       <c r="D103">
         <v>0</v>
       </c>
       <c r="E103">
-        <v>317675670.82319045</v>
+        <v>317775359.69960833</v>
       </c>
       <c r="F103">
-        <v>1139.1602623146357</v>
+        <v>1139.6500574886629</v>
       </c>
       <c r="G103">
         <v>0</v>
       </c>
       <c r="H103">
-        <v>109.12336034427173</v>
+        <v>109.15760402794911</v>
       </c>
       <c r="I103" t="s">
         <v>33</v>
@@ -4788,22 +4788,22 @@
         <v>3857821</v>
       </c>
       <c r="C104">
-        <v>20331182744.141212</v>
+        <v>20363377509.357719</v>
       </c>
       <c r="D104">
-        <v>1206517.0199602428</v>
+        <v>1241908.8349998561</v>
       </c>
       <c r="E104">
-        <v>20210793.960938245</v>
+        <v>20538958.817721281</v>
       </c>
       <c r="F104">
-        <v>5270.1208127959317</v>
+        <v>5278.466136546439</v>
       </c>
       <c r="G104">
-        <v>0.31274572354711189</v>
+        <v>0.32191976636548353</v>
       </c>
       <c r="H104">
-        <v>5.2389143925905959</v>
+        <v>5.3239792146191549</v>
       </c>
       <c r="I104" t="s">
         <v>33</v>
@@ -4829,7 +4829,7 @@
         <v>393144</v>
       </c>
       <c r="C105">
-        <v>1320660117.33708</v>
+        <v>1397110549.2935388</v>
       </c>
       <c r="D105">
         <v>0</v>
@@ -4838,7 +4838,7 @@
         <v>123445976.8768561</v>
       </c>
       <c r="F105">
-        <v>3359.2274518677127</v>
+        <v>3553.6865608874582</v>
       </c>
       <c r="G105">
         <v>0</v>
@@ -4870,22 +4870,22 @@
         <v>2485399</v>
       </c>
       <c r="C106">
-        <v>14485712224.513735</v>
+        <v>14235597487.909796</v>
       </c>
       <c r="D106">
-        <v>851121.54688539519</v>
+        <v>853517.86304080253</v>
       </c>
       <c r="E106">
-        <v>14628486.060927361</v>
+        <v>14811232.102019832</v>
       </c>
       <c r="F106">
-        <v>5828.3246370155193</v>
+        <v>5727.6910016901893</v>
       </c>
       <c r="G106">
-        <v>0.34244865588398288</v>
+        <v>0.3434128134117711</v>
       </c>
       <c r="H106">
-        <v>5.8857696735724776</v>
+        <v>5.9592975220557474</v>
       </c>
       <c r="I106" t="s">
         <v>34</v>
@@ -4911,22 +4911,22 @@
         <v>261201</v>
       </c>
       <c r="C107">
-        <v>485843073.10361695</v>
+        <v>492912285.22083044</v>
       </c>
       <c r="D107">
         <v>0</v>
       </c>
       <c r="E107">
-        <v>46252512.976116002</v>
+        <v>46529982.602552682</v>
       </c>
       <c r="F107">
-        <v>1860.0352720840156</v>
+        <v>1887.0995333893454</v>
       </c>
       <c r="G107">
         <v>0</v>
       </c>
       <c r="H107">
-        <v>177.0763242717907</v>
+        <v>178.13860820805695</v>
       </c>
       <c r="I107" t="s">
         <v>34</v>
@@ -4952,22 +4952,22 @@
         <v>14072154</v>
       </c>
       <c r="C108">
-        <v>58872729419.619743</v>
+        <v>59905043249.929779</v>
       </c>
       <c r="D108">
-        <v>3573495.1551564126</v>
+        <v>3597642.4921723371</v>
       </c>
       <c r="E108">
-        <v>63671139.279884189</v>
+        <v>62748775.29782705</v>
       </c>
       <c r="F108">
-        <v>4183.6331111512663</v>
+        <v>4256.9917334567099</v>
       </c>
       <c r="G108">
-        <v>0.25394087892702233</v>
+        <v>0.25565684487053913</v>
       </c>
       <c r="H108">
-        <v>4.5246192786039856</v>
+        <v>4.4590739482972577</v>
       </c>
       <c r="I108" t="s">
         <v>35</v>
@@ -4993,22 +4993,22 @@
         <v>543145</v>
       </c>
       <c r="C109">
-        <v>938359439.28786027</v>
+        <v>923180166.10594833</v>
       </c>
       <c r="D109">
         <v>0</v>
       </c>
       <c r="E109">
-        <v>87248951.726106152</v>
+        <v>80690041.79092063</v>
       </c>
       <c r="F109">
-        <v>1727.6407576022245</v>
+        <v>1699.6937578472568</v>
       </c>
       <c r="G109">
         <v>0</v>
       </c>
       <c r="H109">
-        <v>160.63657352291958</v>
+        <v>148.56077436213283</v>
       </c>
       <c r="I109" t="s">
         <v>35</v>
@@ -5034,22 +5034,22 @@
         <v>7296430</v>
       </c>
       <c r="C110">
-        <v>32164787184.062927</v>
+        <v>32225127537.238914</v>
       </c>
       <c r="D110">
-        <v>2065090.1252026653</v>
+        <v>2079047.7906007543</v>
       </c>
       <c r="E110">
-        <v>41679992.39988625</v>
+        <v>40058813.210322693</v>
       </c>
       <c r="F110">
-        <v>4408.291066187564</v>
+        <v>4416.5609122870928</v>
       </c>
       <c r="G110">
-        <v>0.28302747031118852</v>
+        <v>0.28494041477828941</v>
       </c>
       <c r="H110">
-        <v>5.7123815893370118</v>
+        <v>5.4901935892378457</v>
       </c>
       <c r="I110" t="s">
         <v>35</v>
@@ -5075,22 +5075,22 @@
         <v>11269955</v>
       </c>
       <c r="C111">
-        <v>23675153682.263424</v>
+        <v>23674031314.164898</v>
       </c>
       <c r="D111">
-        <v>1843844.0437459955</v>
+        <v>1851013.0423539439</v>
       </c>
       <c r="E111">
-        <v>33841223.329871006</v>
+        <v>33845520.703881033</v>
       </c>
       <c r="F111">
-        <v>2100.7318735756639</v>
+        <v>2100.632284171933</v>
       </c>
       <c r="G111">
-        <v>0.16360704579086566</v>
+        <v>0.16424316178316098</v>
       </c>
       <c r="H111">
-        <v>3.00278247161333</v>
+        <v>3.0031637840506935</v>
       </c>
       <c r="I111" t="s">
         <v>35</v>
@@ -5116,22 +5116,22 @@
         <v>5367819</v>
       </c>
       <c r="C112">
-        <v>21311902138.952171</v>
+        <v>21277333832.879292</v>
       </c>
       <c r="D112">
-        <v>1318307.4295536042</v>
+        <v>1330839.8402873415</v>
       </c>
       <c r="E112">
-        <v>22361052.263493933</v>
+        <v>22631069.934466936</v>
       </c>
       <c r="F112">
-        <v>3970.3093824423236</v>
+        <v>3963.8694659561529</v>
       </c>
       <c r="G112">
-        <v>0.24559461292446788</v>
+        <v>0.24792934342371484</v>
       </c>
       <c r="H112">
-        <v>4.1657612269515667</v>
+        <v>4.2160642775896386</v>
       </c>
       <c r="I112" t="s">
         <v>35</v>
@@ -5157,22 +5157,22 @@
         <v>9846148</v>
       </c>
       <c r="C113">
-        <v>64356411575.093399</v>
+        <v>64903680203.243248</v>
       </c>
       <c r="D113">
-        <v>3888860.8187661129</v>
+        <v>3967200.8210855569</v>
       </c>
       <c r="E113">
-        <v>70333449.134599</v>
+        <v>71058902.497514278</v>
       </c>
       <c r="F113">
-        <v>6536.2019314653198</v>
+        <v>6591.7839345136035</v>
       </c>
       <c r="G113">
-        <v>0.39496266141501357</v>
+        <v>0.40291907262470122</v>
       </c>
       <c r="H113">
-        <v>7.1432451690345298</v>
+        <v>7.2169240699524604</v>
       </c>
       <c r="I113" t="s">
         <v>35</v>
@@ -5198,22 +5198,22 @@
         <v>5178344</v>
       </c>
       <c r="C114">
-        <v>6030792661.0012817</v>
+        <v>6117079819.765583</v>
       </c>
       <c r="D114">
-        <v>447950.73168617109</v>
+        <v>453285.10626055778</v>
       </c>
       <c r="E114">
-        <v>7300576.2221713746</v>
+        <v>7460883.2348668296</v>
       </c>
       <c r="F114">
-        <v>1164.6180054861711</v>
+        <v>1181.2810851819777</v>
       </c>
       <c r="G114">
-        <v>8.6504629991010856E-2</v>
+        <v>8.7534761356247826E-2</v>
       </c>
       <c r="H114">
-        <v>1.4098283586743898</v>
+        <v>1.4407855551633553</v>
       </c>
       <c r="I114" t="s">
         <v>36</v>
@@ -5239,22 +5239,22 @@
         <v>3896653</v>
       </c>
       <c r="C115">
-        <v>4264839946.4074869</v>
+        <v>4218231921.9606962</v>
       </c>
       <c r="D115">
         <v>0</v>
       </c>
       <c r="E115">
-        <v>404134165.07612884</v>
+        <v>405774635.14170504</v>
       </c>
       <c r="F115">
-        <v>1094.48799942091</v>
+        <v>1082.5269588954152</v>
       </c>
       <c r="G115">
         <v>0</v>
       </c>
       <c r="H115">
-        <v>103.71315205026694</v>
+        <v>104.13414670018219</v>
       </c>
       <c r="I115" t="s">
         <v>36</v>
@@ -5280,22 +5280,22 @@
         <v>419820</v>
       </c>
       <c r="C116">
-        <v>424740511.9627288</v>
+        <v>425075629.01140189</v>
       </c>
       <c r="D116">
         <v>0</v>
       </c>
       <c r="E116">
-        <v>35117176.609045073</v>
+        <v>34795876.649727635</v>
       </c>
       <c r="F116">
-        <v>1011.720527756488</v>
+        <v>1012.5187675942116</v>
       </c>
       <c r="G116">
         <v>0</v>
       </c>
       <c r="H116">
-        <v>83.648174477264234</v>
+        <v>82.882846576455705</v>
       </c>
       <c r="I116" t="s">
         <v>36</v>
@@ -5321,22 +5321,22 @@
         <v>12685</v>
       </c>
       <c r="C117">
-        <v>12471921.271523749</v>
+        <v>12627789.308144944</v>
       </c>
       <c r="D117">
         <v>0</v>
       </c>
       <c r="E117">
-        <v>1222378.7682689303</v>
+        <v>1189127.9144836015</v>
       </c>
       <c r="F117">
-        <v>983.20230756986598</v>
+        <v>995.48989421718125</v>
       </c>
       <c r="G117">
         <v>0</v>
       </c>
       <c r="H117">
-        <v>96.364112595106846</v>
+        <v>93.742839139424632</v>
       </c>
       <c r="I117" t="s">
         <v>36</v>
@@ -5362,22 +5362,22 @@
         <v>1522254</v>
       </c>
       <c r="C118">
-        <v>2139953796.1769292</v>
+        <v>2126401123.0181949</v>
       </c>
       <c r="D118">
         <v>0</v>
       </c>
       <c r="E118">
-        <v>206893321.68310916</v>
+        <v>201002744.54576856</v>
       </c>
       <c r="F118">
-        <v>1405.779716247702</v>
+        <v>1396.876686162884</v>
       </c>
       <c r="G118">
         <v>0</v>
       </c>
       <c r="H118">
-        <v>135.9124835166202</v>
+        <v>132.04284209190357</v>
       </c>
       <c r="I118" t="s">
         <v>37</v>
@@ -5444,22 +5444,22 @@
         <v>214384</v>
       </c>
       <c r="C120">
-        <v>1761611094.8859448</v>
+        <v>1811913255.4563468</v>
       </c>
       <c r="D120">
-        <v>106401.37113911042</v>
+        <v>110643.11032863639</v>
       </c>
       <c r="E120">
-        <v>1716021.6750235669</v>
+        <v>1734495.2774398425</v>
       </c>
       <c r="F120">
-        <v>8217.0828741228124</v>
+        <v>8451.7186704994165</v>
       </c>
       <c r="G120">
-        <v>0.49631209017049038</v>
+        <v>0.51609779801028244</v>
       </c>
       <c r="H120">
-        <v>8.0044297849819337</v>
+        <v>8.0906004059997123</v>
       </c>
       <c r="I120" t="s">
         <v>23</v>
@@ -5485,22 +5485,22 @@
         <v>13572760</v>
       </c>
       <c r="C121">
-        <v>6339900705.5328321</v>
+        <v>6371448563.8321648</v>
       </c>
       <c r="D121">
         <v>2621533.9661828708</v>
       </c>
       <c r="E121">
-        <v>75946749.485087454</v>
+        <v>101217527.65185121</v>
       </c>
       <c r="F121">
-        <v>467.1047528677168</v>
+        <v>469.42910386923256</v>
       </c>
       <c r="G121">
         <v>0.19314671195710165</v>
       </c>
       <c r="H121">
-        <v>5.59552732716761</v>
+        <v>7.457402006065915</v>
       </c>
       <c r="I121" t="s">
         <v>14</v>
@@ -5526,22 +5526,22 @@
         <v>17815891</v>
       </c>
       <c r="C122">
-        <v>20547513886.85305</v>
+        <v>21271520961.28759</v>
       </c>
       <c r="D122">
-        <v>1409768.0773081863</v>
+        <v>1456941.8788097498</v>
       </c>
       <c r="E122">
-        <v>23096421.651233036</v>
+        <v>23886508.87153738</v>
       </c>
       <c r="F122">
-        <v>1153.3250785410087</v>
+        <v>1193.9633533505335</v>
       </c>
       <c r="G122">
-        <v>7.9129810420830837E-2</v>
+        <v>8.1777660113083864E-2</v>
       </c>
       <c r="H122">
-        <v>1.2963944184005749</v>
+        <v>1.3407417496850076</v>
       </c>
       <c r="I122" t="s">
         <v>9</v>
@@ -5567,22 +5567,22 @@
         <v>7047532</v>
       </c>
       <c r="C123">
-        <v>30890840892.992508</v>
+        <v>30907078147.451797</v>
       </c>
       <c r="D123">
-        <v>2023652.9200207551</v>
+        <v>2085953.7194761841</v>
       </c>
       <c r="E123">
-        <v>33655340.06795302</v>
+        <v>34206817.636711881</v>
       </c>
       <c r="F123">
-        <v>4383.2139950542269</v>
+        <v>4385.5179582656447</v>
       </c>
       <c r="G123">
-        <v>0.28714348796440442</v>
+        <v>0.29598357545253917</v>
       </c>
       <c r="H123">
-        <v>4.775478858124095</v>
+        <v>4.8537300201988272</v>
       </c>
       <c r="I123" t="s">
         <v>35</v>
@@ -5608,22 +5608,22 @@
         <v>6223129</v>
       </c>
       <c r="C124">
-        <v>6990346203.5029345</v>
+        <v>6929031166.1697416</v>
       </c>
       <c r="D124">
         <v>0</v>
       </c>
       <c r="E124">
-        <v>679229428.64073026</v>
+        <v>673705170.22657657</v>
       </c>
       <c r="F124">
-        <v>1123.2847982908493</v>
+        <v>1113.4320317270849</v>
       </c>
       <c r="G124">
         <v>0</v>
       </c>
       <c r="H124">
-        <v>109.14596638455193</v>
+        <v>108.2582685055342</v>
       </c>
       <c r="I124" t="s">
         <v>38</v>
@@ -5649,22 +5649,22 @@
         <v>2129192</v>
       </c>
       <c r="C125">
-        <v>2546611132.2940063</v>
+        <v>2546731865.2209973</v>
       </c>
       <c r="D125">
-        <v>184612.73166592175</v>
+        <v>189753.00503444404</v>
       </c>
       <c r="E125">
-        <v>3033971.6044044243</v>
+        <v>3177083.4725367082</v>
       </c>
       <c r="F125">
-        <v>1196.04579215684</v>
+        <v>1196.1024957922994</v>
       </c>
       <c r="G125">
-        <v>8.6705535088391156E-2</v>
+        <v>8.9119724775616305E-2</v>
       </c>
       <c r="H125">
-        <v>1.4249403550287736</v>
+        <v>1.4921545227188098</v>
       </c>
       <c r="I125" t="s">
         <v>17</v>
@@ -5690,22 +5690,22 @@
         <v>4998069</v>
       </c>
       <c r="C126">
-        <v>4701151015.9143782</v>
+        <v>4636738975.1342287</v>
       </c>
       <c r="D126">
         <v>0</v>
       </c>
       <c r="E126">
-        <v>385605432.31843591</v>
+        <v>395024231.07814586</v>
       </c>
       <c r="F126">
-        <v>940.59346037727335</v>
+        <v>927.70607511305445</v>
       </c>
       <c r="G126">
         <v>0</v>
       </c>
       <c r="H126">
-        <v>77.150882134367478</v>
+        <v>79.035369675397817</v>
       </c>
       <c r="I126" t="s">
         <v>17</v>
@@ -5731,22 +5731,22 @@
         <v>4031692</v>
       </c>
       <c r="C127">
-        <v>31556703640.913544</v>
+        <v>32462084563.024048</v>
       </c>
       <c r="D127">
-        <v>12894007.241531136</v>
+        <v>13246698.96835652</v>
       </c>
       <c r="E127">
-        <v>189497951.54433119</v>
+        <v>166793970.5981864</v>
       </c>
       <c r="F127">
-        <v>7827.1613111600645</v>
+        <v>8051.7273053159934</v>
       </c>
       <c r="G127">
-        <v>3.1981627667815733</v>
+        <v>3.2856425958025861</v>
       </c>
       <c r="H127">
-        <v>47.002090324442243</v>
+        <v>41.370712494453052</v>
       </c>
       <c r="I127" t="s">
         <v>21</v>
@@ -5772,22 +5772,22 @@
         <v>5936999</v>
       </c>
       <c r="C128">
-        <v>27944001555.338829</v>
+        <v>28009963334.308266</v>
       </c>
       <c r="D128">
-        <v>1591246.9098549862</v>
+        <v>1575082.6432349135</v>
       </c>
       <c r="E128">
-        <v>28734027.252789363</v>
+        <v>28226093.385246754</v>
       </c>
       <c r="F128">
-        <v>4706.7553077470329</v>
+        <v>4717.8655974690691</v>
       </c>
       <c r="G128">
-        <v>0.2680220949767696</v>
+        <v>0.26529946244473235</v>
       </c>
       <c r="H128">
-        <v>4.8398234954712578</v>
+        <v>4.7542695198780986</v>
       </c>
       <c r="I128" t="s">
         <v>31</v>
@@ -5813,19 +5813,19 @@
         <v>8834166</v>
       </c>
       <c r="C129">
-        <v>53803807832.392258</v>
+        <v>53869692984.185715</v>
       </c>
       <c r="D129">
-        <v>2848571.1691900212</v>
+        <v>3169654.7221121597</v>
       </c>
       <c r="E129">
         <v>50094780.845352754</v>
       </c>
       <c r="F129">
-        <v>6090.4230045476006</v>
+        <v>6097.8809979556318</v>
       </c>
       <c r="G129">
-        <v>0.32244935958754017</v>
+        <v>0.35879501495807975</v>
       </c>
       <c r="H129">
         <v>5.6705727337875196</v>
@@ -5854,22 +5854,22 @@
         <v>3440952</v>
       </c>
       <c r="C130">
-        <v>17397357256.450649</v>
+        <v>17472230367.965454</v>
       </c>
       <c r="D130">
-        <v>7105603.7848933134</v>
+        <v>7136121.9209022</v>
       </c>
       <c r="E130">
-        <v>100380721.97039926</v>
+        <v>90964234.364870578</v>
       </c>
       <c r="F130">
-        <v>5055.972084600613</v>
+        <v>5077.7315022021385</v>
       </c>
       <c r="G130">
-        <v>2.0650110158157724</v>
+        <v>2.0738801125102007</v>
       </c>
       <c r="H130">
-        <v>29.172369149700216</v>
+        <v>26.435775437980702</v>
       </c>
       <c r="I130" t="s">
         <v>31</v>
@@ -5895,22 +5895,22 @@
         <v>3273953</v>
       </c>
       <c r="C131">
-        <v>24084984758.972076</v>
+        <v>24052937208.038948</v>
       </c>
       <c r="D131">
-        <v>12902635.039648566</v>
+        <v>12888002.416297529</v>
       </c>
       <c r="E131">
-        <v>327441519.39395344</v>
+        <v>322747465.36849964</v>
       </c>
       <c r="F131">
-        <v>7356.5456678736919</v>
+        <v>7346.7570267621277</v>
       </c>
       <c r="G131">
-        <v>3.9409958052692162</v>
+        <v>3.9365263998284425</v>
       </c>
       <c r="H131">
-        <v>100.01411730527391</v>
+        <v>98.580360001655379</v>
       </c>
       <c r="I131" t="s">
         <v>21</v>
@@ -5936,22 +5936,22 @@
         <v>4469578</v>
       </c>
       <c r="C132">
-        <v>11389160256.762962</v>
+        <v>11432824610.053396</v>
       </c>
       <c r="D132">
-        <v>706434.52238912904</v>
+        <v>701475.43001384242</v>
       </c>
       <c r="E132">
-        <v>13190232.006797824</v>
+        <v>13865511.902981661</v>
       </c>
       <c r="F132">
-        <v>2548.1511356917727</v>
+        <v>2557.9203696754807</v>
       </c>
       <c r="G132">
-        <v>0.15805396446580169</v>
+        <v>0.15694444308027344</v>
       </c>
       <c r="H132">
-        <v>2.9511135070912342</v>
+        <v>3.1021970984691758</v>
       </c>
       <c r="I132" t="s">
         <v>16</v>
@@ -5977,22 +5977,22 @@
         <v>5464804</v>
       </c>
       <c r="C133">
-        <v>6914074308.2245588</v>
+        <v>6808311626.713892</v>
       </c>
       <c r="D133">
         <v>0</v>
       </c>
       <c r="E133">
-        <v>664645067.2638936</v>
+        <v>657978449.29767299</v>
       </c>
       <c r="F133">
-        <v>1265.2007845523021</v>
+        <v>1245.8473582426545</v>
       </c>
       <c r="G133">
         <v>0</v>
       </c>
       <c r="H133">
-        <v>121.62285550660071</v>
+        <v>120.40293655502978</v>
       </c>
       <c r="I133" t="s">
         <v>39</v>
@@ -6018,22 +6018,22 @@
         <v>245854</v>
       </c>
       <c r="C134">
-        <v>588873633.78891814</v>
+        <v>602386585.17014229</v>
       </c>
       <c r="D134">
-        <v>238666.63529984772</v>
+        <v>243240.38615054172</v>
       </c>
       <c r="E134">
-        <v>4769582.1812927965</v>
+        <v>4845692.5352495965</v>
       </c>
       <c r="F134">
-        <v>2395.2168107450689</v>
+        <v>2450.1801279220281</v>
       </c>
       <c r="G134">
-        <v>0.97076571989818239</v>
+        <v>0.98936924414710237</v>
       </c>
       <c r="H134">
-        <v>19.400059308747455</v>
+        <v>19.709634723248744</v>
       </c>
       <c r="I134" t="s">
         <v>25</v>
@@ -6059,7 +6059,7 @@
         <v>1204962</v>
       </c>
       <c r="C135">
-        <v>1574810759.4612119</v>
+        <v>1568622730.1839328</v>
       </c>
       <c r="D135">
         <v>0</v>
@@ -6068,7 +6068,7 @@
         <v>150376666.50494289</v>
       </c>
       <c r="F135">
-        <v>1306.9381104642403</v>
+        <v>1301.8026545102109</v>
       </c>
       <c r="G135">
         <v>0</v>
@@ -6100,22 +6100,22 @@
         <v>11346108</v>
       </c>
       <c r="C136">
-        <v>15433852900.587957</v>
+        <v>15368932176.666138</v>
       </c>
       <c r="D136">
-        <v>1143499.6171640868</v>
+        <v>1149136.2841472591</v>
       </c>
       <c r="E136">
-        <v>18561262.53767778</v>
+        <v>18746016.927348763</v>
       </c>
       <c r="F136">
-        <v>1360.2772775111921</v>
+        <v>1354.5554278758971</v>
       </c>
       <c r="G136">
-        <v>0.10078342433934939</v>
+        <v>0.10128021733507729</v>
       </c>
       <c r="H136">
-        <v>1.6359144948803395</v>
+        <v>1.6521979984104473</v>
       </c>
       <c r="I136" t="s">
         <v>20</v>
@@ -6141,22 +6141,22 @@
         <v>2439887</v>
       </c>
       <c r="C137">
-        <v>2617936410.6769152</v>
+        <v>2588432548.2116833</v>
       </c>
       <c r="D137">
-        <v>159703.30033394796</v>
+        <v>161243.45894326048</v>
       </c>
       <c r="E137">
-        <v>2645703.3026877483</v>
+        <v>2701237.1365026943</v>
       </c>
       <c r="F137">
-        <v>1072.9744495039793</v>
+        <v>1060.882142579424</v>
       </c>
       <c r="G137">
-        <v>6.5455203595063197E-2</v>
+        <v>6.6086445373601518E-2</v>
       </c>
       <c r="H137">
-        <v>1.0843548503220635</v>
+        <v>1.107115672366259</v>
       </c>
       <c r="I137" t="s">
         <v>25</v>
@@ -6182,22 +6182,22 @@
         <v>14844275</v>
       </c>
       <c r="C138">
-        <v>16395518510.549278</v>
+        <v>16695236560.346279</v>
       </c>
       <c r="D138">
-        <v>14154797.647440881</v>
+        <v>14413554.230432291</v>
       </c>
       <c r="E138">
-        <v>354141381.5831092</v>
+        <v>370522646.20239127</v>
       </c>
       <c r="F138">
-        <v>1104.5011299338821</v>
+        <v>1124.6919475923398</v>
       </c>
       <c r="G138">
-        <v>0.9535526421762518</v>
+        <v>0.9709840480880535</v>
       </c>
       <c r="H138">
-        <v>23.857101918625812</v>
+        <v>24.960642820372922</v>
       </c>
       <c r="I138" t="s">
         <v>40</v>
@@ -6223,22 +6223,22 @@
         <v>614883</v>
       </c>
       <c r="C139">
-        <v>3343047128.3181963</v>
+        <v>3320653089.0944014</v>
       </c>
       <c r="D139">
-        <v>180106.6887409554</v>
+        <v>186959.86633533629</v>
       </c>
       <c r="E139">
-        <v>2847753.7775054188</v>
+        <v>2967647.3607132668</v>
       </c>
       <c r="F139">
-        <v>5436.8833230357586</v>
+        <v>5400.4633224441095</v>
       </c>
       <c r="G139">
-        <v>0.29291212920336945</v>
+        <v>0.3040576277687565</v>
       </c>
       <c r="H139">
-        <v>4.6313750380241752</v>
+        <v>4.826361048708887</v>
       </c>
       <c r="I139" t="s">
         <v>28</v>
@@ -6264,22 +6264,22 @@
         <v>5372955</v>
       </c>
       <c r="C140">
-        <v>15646897545.02968</v>
+        <v>15782419670.229256</v>
       </c>
       <c r="D140">
-        <v>1036512.6854658893</v>
+        <v>1032619.5533630811</v>
       </c>
       <c r="E140">
-        <v>18308658.797187932</v>
+        <v>18128587.56380941</v>
       </c>
       <c r="F140">
-        <v>2912.1586808431634</v>
+        <v>2937.3816959623255</v>
       </c>
       <c r="G140">
-        <v>0.19291296604305996</v>
+        <v>0.19218838671886906</v>
       </c>
       <c r="H140">
-        <v>3.4075585589657704</v>
+        <v>3.374044183100251</v>
       </c>
       <c r="I140" t="s">
         <v>18</v>
@@ -6305,22 +6305,22 @@
         <v>222191</v>
       </c>
       <c r="C141">
-        <v>1377927439.2125008</v>
+        <v>1316070346.4397974</v>
       </c>
       <c r="D141">
-        <v>1189610.6891867926</v>
+        <v>1136207.3990930251</v>
       </c>
       <c r="E141">
-        <v>32838503.983139992</v>
+        <v>11631548.457432184</v>
       </c>
       <c r="F141">
-        <v>6201.5447934997401</v>
+        <v>5923.1487613800618</v>
       </c>
       <c r="G141">
-        <v>5.3540003383881105</v>
+        <v>5.113651763991454</v>
       </c>
       <c r="H141">
-        <v>147.79403298576446</v>
+        <v>52.349323138345767</v>
       </c>
       <c r="I141" t="s">
         <v>40</v>
@@ -6346,22 +6346,22 @@
         <v>7152189</v>
       </c>
       <c r="C142">
-        <v>10506964556.986982</v>
+        <v>10445701214.324686</v>
       </c>
       <c r="D142">
-        <v>9071012.7341987621</v>
+        <v>9018122.0483669806</v>
       </c>
       <c r="E142">
-        <v>162645907.94026181</v>
+        <v>169739588.32473457</v>
       </c>
       <c r="F142">
-        <v>1469.0557753698879</v>
+        <v>1460.4900981118767</v>
       </c>
       <c r="G142">
-        <v>1.2682848194026699</v>
+        <v>1.2608897847032539</v>
       </c>
       <c r="H142">
-        <v>22.740717274146672</v>
+        <v>23.732536755493257</v>
       </c>
       <c r="I142" t="s">
         <v>24</v>
@@ -6387,22 +6387,22 @@
         <v>13610817</v>
       </c>
       <c r="C143">
-        <v>58652409882.993179</v>
+        <v>57736244002.330208</v>
       </c>
       <c r="D143">
-        <v>33418751.02748286</v>
+        <v>32840986.996123247</v>
       </c>
       <c r="E143">
-        <v>695950420.43518615</v>
+        <v>725225571.07163513</v>
       </c>
       <c r="F143">
-        <v>4309.249759437158</v>
+        <v>4241.9381586226755</v>
       </c>
       <c r="G143">
-        <v>2.4553082322305015</v>
+        <v>2.4128593453371128</v>
       </c>
       <c r="H143">
-        <v>51.132156169257591</v>
+        <v>53.283030039389637</v>
       </c>
       <c r="I143" t="s">
         <v>32</v>
@@ -6428,22 +6428,22 @@
         <v>5621453</v>
       </c>
       <c r="C144">
-        <v>5684271919.7832432</v>
+        <v>5613207792.6343374</v>
       </c>
       <c r="D144">
         <v>0</v>
       </c>
       <c r="E144">
-        <v>557024539.90599418</v>
+        <v>523967172.29755771</v>
       </c>
       <c r="F144">
-        <v>1011.1748545764312</v>
+        <v>998.53326046385826</v>
       </c>
       <c r="G144">
         <v>0</v>
       </c>
       <c r="H144">
-        <v>99.089068236627469</v>
+        <v>93.208494725039543</v>
       </c>
       <c r="I144" t="s">
         <v>15</v>
@@ -6469,7 +6469,7 @@
         <v>4776449</v>
       </c>
       <c r="C145">
-        <v>5417734423.6636906</v>
+        <v>5305072294.2163801</v>
       </c>
       <c r="D145">
         <v>0</v>
@@ -6478,7 +6478,7 @@
         <v>508919839.40061837</v>
       </c>
       <c r="F145">
-        <v>1134.259870389842</v>
+        <v>1110.6728647613279</v>
       </c>
       <c r="G145">
         <v>0</v>
@@ -6510,7 +6510,7 @@
         <v>2383346</v>
       </c>
       <c r="C146">
-        <v>2636355036.6267657</v>
+        <v>2649569848.8404336</v>
       </c>
       <c r="D146">
         <v>0</v>
@@ -6519,7 +6519,7 @@
         <v>256441285.96453649</v>
       </c>
       <c r="F146">
-        <v>1106.1570735540563</v>
+        <v>1111.7017205392895</v>
       </c>
       <c r="G146">
         <v>0</v>
@@ -6551,22 +6551,22 @@
         <v>14585886</v>
       </c>
       <c r="C147">
-        <v>146392249196.88651</v>
+        <v>146416937571.41907</v>
       </c>
       <c r="D147">
-        <v>7046333.115594862</v>
+        <v>7093139.2579163872</v>
       </c>
       <c r="E147">
-        <v>150570820.70772916</v>
+        <v>142152984.31266299</v>
       </c>
       <c r="F147">
-        <v>10036.568858202136</v>
+        <v>10038.261479036588</v>
       </c>
       <c r="G147">
-        <v>0.48309256740350653</v>
+        <v>0.48630156974464128</v>
       </c>
       <c r="H147">
-        <v>10.32304933054661</v>
+        <v>9.7459272828995775</v>
       </c>
       <c r="I147" t="s">
         <v>18</v>
@@ -6592,22 +6592,22 @@
         <v>93260</v>
       </c>
       <c r="C148">
-        <v>130094975.29131168</v>
+        <v>128860909.37590754</v>
       </c>
       <c r="D148">
         <v>0</v>
       </c>
       <c r="E148">
-        <v>10409132.809462368</v>
+        <v>10578091.096767589</v>
       </c>
       <c r="F148">
-        <v>1394.9707837369899</v>
+        <v>1381.7382519398193</v>
       </c>
       <c r="G148">
         <v>0</v>
       </c>
       <c r="H148">
-        <v>111.61411976691366</v>
+        <v>113.42581060226881</v>
       </c>
       <c r="I148" t="s">
         <v>16</v>
@@ -6633,22 +6633,22 @@
         <v>2184313</v>
       </c>
       <c r="C149">
-        <v>2900496947.1264281</v>
+        <v>2895634600.7664504</v>
       </c>
       <c r="D149">
         <v>214620.25697716986</v>
       </c>
       <c r="E149">
-        <v>3455996.6990086655</v>
+        <v>3488600.4414521432</v>
       </c>
       <c r="F149">
-        <v>1327.8760631495707</v>
+        <v>1325.6500331071832</v>
       </c>
       <c r="G149">
         <v>9.8255266977383668E-2</v>
       </c>
       <c r="H149">
-        <v>1.5821893194833641</v>
+        <v>1.5971156338181127</v>
       </c>
       <c r="I149" t="s">
         <v>11</v>
@@ -6674,22 +6674,22 @@
         <v>1131899</v>
       </c>
       <c r="C150">
-        <v>2086674340.2625053</v>
+        <v>2279159523.4737415</v>
       </c>
       <c r="D150">
-        <v>156240.29170437515</v>
+        <v>158676.23645821604</v>
       </c>
       <c r="E150">
-        <v>2747104.8031988242</v>
+        <v>2856175.1124228579</v>
       </c>
       <c r="F150">
-        <v>1843.5163740426533</v>
+        <v>2013.571461299764</v>
       </c>
       <c r="G150">
-        <v>0.13803377483713225</v>
+        <v>0.14018586151080267</v>
       </c>
       <c r="H150">
-        <v>2.4269875697379573</v>
+        <v>2.5233480305423521</v>
       </c>
       <c r="I150" t="s">
         <v>18</v>
@@ -6797,22 +6797,22 @@
         <v>9975515</v>
       </c>
       <c r="C153">
-        <v>28321840697.925453</v>
+        <v>27798213035.860031</v>
       </c>
       <c r="D153">
-        <v>1734038.6377814848</v>
+        <v>1726774.4666442028</v>
       </c>
       <c r="E153">
-        <v>33045287.940479718</v>
+        <v>32468740.334353346</v>
       </c>
       <c r="F153">
-        <v>2839.1356935381737</v>
+        <v>2786.6444024052926</v>
       </c>
       <c r="G153">
-        <v>0.17382948527283903</v>
+        <v>0.17310128516113732</v>
       </c>
       <c r="H153">
-        <v>3.3126397925801041</v>
+        <v>3.2548435177886401</v>
       </c>
       <c r="I153" t="s">
         <v>11</v>
@@ -6838,22 +6838,22 @@
         <v>2161126</v>
       </c>
       <c r="C154">
-        <v>5395323255.0460415</v>
+        <v>5369149957.2001266</v>
       </c>
       <c r="D154">
-        <v>338077.71601952508</v>
+        <v>345673.93689425953</v>
       </c>
       <c r="E154">
-        <v>5513368.5526777394</v>
+        <v>5868258.6835834831</v>
       </c>
       <c r="F154">
-        <v>2496.5334066806108</v>
+        <v>2484.4224525548843</v>
       </c>
       <c r="G154">
-        <v>0.15643591165879503</v>
+        <v>0.15995084825885189</v>
       </c>
       <c r="H154">
-        <v>2.5511555331238158</v>
+        <v>2.7153709147839984</v>
       </c>
       <c r="I154" t="s">
         <v>11</v>
@@ -6879,22 +6879,22 @@
         <v>7465222</v>
       </c>
       <c r="C155">
-        <v>8265844841.2501507</v>
+        <v>8166131361.3769703</v>
       </c>
       <c r="D155">
         <v>0</v>
       </c>
       <c r="E155">
-        <v>792586005.52361882</v>
+        <v>778631668.13484907</v>
       </c>
       <c r="F155">
-        <v>1107.2470237656898</v>
+        <v>1093.8899554999127</v>
       </c>
       <c r="G155">
         <v>0</v>
       </c>
       <c r="H155">
-        <v>106.1704535409153</v>
+        <v>104.30120740345687</v>
       </c>
       <c r="I155" t="s">
         <v>26</v>
@@ -6920,22 +6920,22 @@
         <v>12442473</v>
       </c>
       <c r="C156">
-        <v>50619044397.958069</v>
+        <v>50415444958.014381</v>
       </c>
       <c r="D156">
         <v>0</v>
       </c>
       <c r="E156">
-        <v>4186707202.1589308</v>
+        <v>4101050874.3888392</v>
       </c>
       <c r="F156">
-        <v>4068.2462721002544</v>
+        <v>4051.8830105570155</v>
       </c>
       <c r="G156">
         <v>0</v>
       </c>
       <c r="H156">
-        <v>336.48513459976414</v>
+        <v>329.6009462418636</v>
       </c>
       <c r="I156" t="s">
         <v>18</v>
@@ -6961,22 +6961,22 @@
         <v>6659324</v>
       </c>
       <c r="C157">
-        <v>8979239181.6478844</v>
+        <v>8965682085.6413422</v>
       </c>
       <c r="D157">
-        <v>654376.4440569724</v>
+        <v>664804.29765628115</v>
       </c>
       <c r="E157">
-        <v>10780038.084939033</v>
+        <v>10420732.652367352</v>
       </c>
       <c r="F157">
-        <v>1348.3709730368855</v>
+        <v>1346.3351663984727</v>
       </c>
       <c r="G157">
-        <v>9.8264695343997732E-2</v>
+        <v>9.9830598069155535E-2</v>
       </c>
       <c r="H157">
-        <v>1.6187886465561718</v>
+        <v>1.5648334053677748</v>
       </c>
       <c r="I157" t="s">
         <v>36</v>
@@ -7002,22 +7002,22 @@
         <v>4935387</v>
       </c>
       <c r="C158">
-        <v>7117142261.4898701</v>
+        <v>7222535525.2929993</v>
       </c>
       <c r="D158">
-        <v>2897658.5735439397</v>
+        <v>2948524.2912095911</v>
       </c>
       <c r="E158">
-        <v>62820490.34730874</v>
+        <v>60555041.667665347</v>
       </c>
       <c r="F158">
-        <v>1442.0636642050299</v>
+        <v>1463.418274046797</v>
       </c>
       <c r="G158">
-        <v>0.58711881632462459</v>
+        <v>0.59742514441311112</v>
       </c>
       <c r="H158">
-        <v>12.72858447520098</v>
+        <v>12.26956298820444</v>
       </c>
       <c r="I158" t="s">
         <v>14</v>
@@ -7043,22 +7043,22 @@
         <v>8727176</v>
       </c>
       <c r="C159">
-        <v>11421464882.325718</v>
+        <v>11419000592.727285</v>
       </c>
       <c r="D159">
-        <v>855136.23088376923</v>
+        <v>840467.04736804799</v>
       </c>
       <c r="E159">
-        <v>13855881.845774967</v>
+        <v>13601481.878736233</v>
       </c>
       <c r="F159">
-        <v>1308.7240227910745</v>
+        <v>1308.4416531449904</v>
       </c>
       <c r="G159">
-        <v>9.7985445794122772E-2</v>
+        <v>9.630458322005285E-2</v>
       </c>
       <c r="H159">
-        <v>1.5876707248455821</v>
+        <v>1.5585204055396882</v>
       </c>
       <c r="I159" t="s">
         <v>11</v>
@@ -7084,22 +7084,22 @@
         <v>2169628</v>
       </c>
       <c r="C160">
-        <v>8584584078.3339901</v>
+        <v>8583615375.6504688</v>
       </c>
       <c r="D160">
-        <v>555770.46747655189</v>
+        <v>523105.71846845327</v>
       </c>
       <c r="E160">
-        <v>10741786.757523069</v>
+        <v>9770441.9836489055</v>
       </c>
       <c r="F160">
-        <v>3956.7078219556488</v>
+        <v>3956.2613386490534</v>
       </c>
       <c r="G160">
-        <v>0.25615933582925365</v>
+        <v>0.24110387516590553</v>
       </c>
       <c r="H160">
-        <v>4.9509808859044355</v>
+        <v>4.5032798173921549</v>
       </c>
       <c r="I160" t="s">
         <v>11</v>
@@ -7166,22 +7166,22 @@
         <v>10724956</v>
       </c>
       <c r="C162">
-        <v>10620056632.280073</v>
+        <v>10425469587.02766</v>
       </c>
       <c r="D162">
-        <v>3261765.6835613428</v>
+        <v>3207728.0127566252</v>
       </c>
       <c r="E162">
-        <v>2487305275.2294555</v>
+        <v>2418246669.3153625</v>
       </c>
       <c r="F162">
-        <v>990.21913304633358</v>
+        <v>972.07574436926927</v>
       </c>
       <c r="G162">
-        <v>0.30412858416960803</v>
+        <v>0.29909008603453713</v>
       </c>
       <c r="H162">
-        <v>231.9175272354922</v>
+        <v>225.47846996438611</v>
       </c>
       <c r="I162" t="s">
         <v>37</v>
@@ -7207,22 +7207,22 @@
         <v>5178428</v>
       </c>
       <c r="C163">
-        <v>19875657958.687317</v>
+        <v>19980480085.140694</v>
       </c>
       <c r="D163">
-        <v>1232925.5332846274</v>
+        <v>1221995.1603264823</v>
       </c>
       <c r="E163">
-        <v>20035578.243300565</v>
+        <v>20045330.697291009</v>
       </c>
       <c r="F163">
-        <v>3838.1643924927248</v>
+        <v>3858.4064672021495</v>
       </c>
       <c r="G163">
-        <v>0.23808876618244521</v>
+        <v>0.2359780150127572</v>
       </c>
       <c r="H163">
-        <v>3.869046406226091</v>
+        <v>3.8709296908812885</v>
       </c>
       <c r="I163" t="s">
         <v>18</v>
@@ -7248,22 +7248,22 @@
         <v>3910602</v>
       </c>
       <c r="C164">
-        <v>24286922579.402706</v>
+        <v>24158847589.511581</v>
       </c>
       <c r="D164">
-        <v>1413616.5339252795</v>
+        <v>1421985.7958612321</v>
       </c>
       <c r="E164">
-        <v>24278048.08501314</v>
+        <v>23864242.948842369</v>
       </c>
       <c r="F164">
-        <v>6210.5329510399433</v>
+        <v>6177.7822415862265</v>
       </c>
       <c r="G164">
-        <v>0.36148310002533612</v>
+        <v>0.36362324671782814</v>
       </c>
       <c r="H164">
-        <v>6.2082636087776617</v>
+        <v>6.102447385042602</v>
       </c>
       <c r="I164" t="s">
         <v>12</v>
@@ -7289,22 +7289,22 @@
         <v>7463219</v>
       </c>
       <c r="C165">
-        <v>35632498840.84864</v>
+        <v>35862686411.744858</v>
       </c>
       <c r="D165">
-        <v>2123357.2751112944</v>
+        <v>2200971.0106013315</v>
       </c>
       <c r="E165">
-        <v>37234874.367517248</v>
+        <v>37768465.224384777</v>
       </c>
       <c r="F165">
-        <v>4774.4142093175396</v>
+        <v>4805.2571432976656</v>
       </c>
       <c r="G165">
-        <v>0.2845095762446867</v>
+        <v>0.29490907483772505</v>
       </c>
       <c r="H165">
-        <v>4.9891172116907256</v>
+        <v>5.0606132855520896</v>
       </c>
       <c r="I165" t="s">
         <v>35</v>
@@ -7330,22 +7330,22 @@
         <v>2584028</v>
       </c>
       <c r="C166">
-        <v>12432825577.412834</v>
+        <v>12326394440.129141</v>
       </c>
       <c r="D166">
-        <v>759687.51816099219</v>
+        <v>771933.34572621109</v>
       </c>
       <c r="E166">
-        <v>12715206.677337125</v>
+        <v>12701073.870002463</v>
       </c>
       <c r="F166">
-        <v>4811.4128706859346</v>
+        <v>4770.2247963757127</v>
       </c>
       <c r="G166">
-        <v>0.29399353186613775</v>
+        <v>0.29873257786920693</v>
       </c>
       <c r="H166">
-        <v>4.9206922979693424</v>
+        <v>4.9152230045504393</v>
       </c>
       <c r="I166" t="s">
         <v>21</v>
@@ -7371,22 +7371,22 @@
         <v>5184267</v>
       </c>
       <c r="C167">
-        <v>6026776425.0285912</v>
+        <v>6052041161.5600872</v>
       </c>
       <c r="D167">
         <v>0</v>
       </c>
       <c r="E167">
-        <v>573328541.26179194</v>
+        <v>581990123.3983084</v>
       </c>
       <c r="F167">
-        <v>1162.5127380647236</v>
+        <v>1167.3860859327051</v>
       </c>
       <c r="G167">
         <v>0</v>
       </c>
       <c r="H167">
-        <v>110.59008752091509</v>
+        <v>112.2608313573179</v>
       </c>
       <c r="I167" t="s">
         <v>38</v>
@@ -7412,19 +7412,19 @@
         <v>4104611</v>
       </c>
       <c r="C168">
-        <v>12886845542.978453</v>
+        <v>12787535470.864618</v>
       </c>
       <c r="D168">
-        <v>713821.82619293011</v>
+        <v>714910.72294082458</v>
       </c>
       <c r="E168">
         <v>14428829.484429255</v>
       </c>
       <c r="F168">
-        <v>3139.6021554730651</v>
+        <v>3115.4073969164479</v>
       </c>
       <c r="G168">
-        <v>0.1739073023467827</v>
+        <v>0.17417258856949527</v>
       </c>
       <c r="H168">
         <v>3.5152733071244158</v>
@@ -7453,22 +7453,22 @@
         <v>5491581</v>
       </c>
       <c r="C169">
-        <v>18063080162.013489</v>
+        <v>18193718922.610939</v>
       </c>
       <c r="D169">
-        <v>1076598.40418173</v>
+        <v>1089204.8459812249</v>
       </c>
       <c r="E169">
-        <v>17729970.754746933</v>
+        <v>17889888.804999016</v>
       </c>
       <c r="F169">
-        <v>3289.2313091646083</v>
+        <v>3313.0202254343403</v>
       </c>
       <c r="G169">
-        <v>0.19604525621705843</v>
+        <v>0.19834085047297398</v>
       </c>
       <c r="H169">
-        <v>3.2285731112309795</v>
+        <v>3.2576936960410885</v>
       </c>
       <c r="I169" t="s">
         <v>18</v>
@@ -7494,7 +7494,7 @@
         <v>1299004</v>
       </c>
       <c r="C170">
-        <v>1518524233.896852</v>
+        <v>1518334891.7230492</v>
       </c>
       <c r="D170">
         <v>0</v>
@@ -7503,7 +7503,7 @@
         <v>144278736.43758133</v>
       </c>
       <c r="F170">
-        <v>1168.99119163363</v>
+        <v>1168.8454321334261</v>
       </c>
       <c r="G170">
         <v>0</v>
@@ -7535,22 +7535,22 @@
         <v>2477354</v>
       </c>
       <c r="C171">
-        <v>2995113567.9064379</v>
+        <v>3050350208.7238903</v>
       </c>
       <c r="D171">
         <v>0</v>
       </c>
       <c r="E171">
-        <v>284663242.26212734</v>
+        <v>295382202.56321412</v>
       </c>
       <c r="F171">
-        <v>1208.9970056384504</v>
+        <v>1231.2936337414396</v>
       </c>
       <c r="G171">
         <v>0</v>
       </c>
       <c r="H171">
-        <v>114.90616289078079</v>
+        <v>119.23294069527977</v>
       </c>
       <c r="I171" t="s">
         <v>15</v>
@@ -7576,22 +7576,22 @@
         <v>3250811</v>
       </c>
       <c r="C172">
-        <v>10667953187.849194</v>
+        <v>10925233515.455673</v>
       </c>
       <c r="D172">
-        <v>714170.98500738386</v>
+        <v>755749.08654561965</v>
       </c>
       <c r="E172">
-        <v>11818960.157403491</v>
+        <v>11500956.300113961</v>
       </c>
       <c r="F172">
-        <v>3281.6282422599143</v>
+        <v>3360.7716706556221</v>
       </c>
       <c r="G172">
-        <v>0.21969009733490624</v>
+        <v>0.23248016773218119</v>
       </c>
       <c r="H172">
-        <v>3.6356958793985537</v>
+        <v>3.5378729492775682</v>
       </c>
       <c r="I172" t="s">
         <v>21</v>
@@ -7617,22 +7617,22 @@
         <v>602999</v>
       </c>
       <c r="C173">
-        <v>861083591.2955054</v>
+        <v>876963912.347718</v>
       </c>
       <c r="D173">
         <v>0</v>
       </c>
       <c r="E173">
-        <v>81839583.508090928</v>
+        <v>84921243.225410223</v>
       </c>
       <c r="F173">
-        <v>1428.0016903767757</v>
+        <v>1454.3372581840401</v>
       </c>
       <c r="G173">
         <v>0</v>
       </c>
       <c r="H173">
-        <v>135.72092741130737</v>
+        <v>140.83148268141443</v>
       </c>
       <c r="I173" t="s">
         <v>37</v>
@@ -7661,7 +7661,7 @@
         <v>18582229037.965981</v>
       </c>
       <c r="D174">
-        <v>1081499.1944933962</v>
+        <v>876813.02018039476</v>
       </c>
       <c r="E174">
         <v>12226858.55359629</v>
@@ -7670,7 +7670,7 @@
         <v>4054.4171564546696</v>
       </c>
       <c r="G174">
-        <v>0.23597001629282999</v>
+        <v>0.19130997388736068</v>
       </c>
       <c r="H174">
         <v>2.667752344886154</v>
@@ -7699,22 +7699,22 @@
         <v>12498933</v>
       </c>
       <c r="C175">
-        <v>70598878377.982941</v>
+        <v>70603922934.736328</v>
       </c>
       <c r="D175">
-        <v>4035599.4731404739</v>
+        <v>4055465.1239535492</v>
       </c>
       <c r="E175">
-        <v>73463965.90983744</v>
+        <v>76137002.877174169</v>
       </c>
       <c r="F175">
-        <v>5648.3924170153514</v>
+        <v>5648.7960160068324</v>
       </c>
       <c r="G175">
-        <v>0.32287551850549756</v>
+        <v>0.32446490624068064</v>
       </c>
       <c r="H175">
-        <v>5.8776189863436699</v>
+        <v>6.0914801989237137</v>
       </c>
       <c r="I175" t="s">
         <v>29</v>
@@ -7740,22 +7740,22 @@
         <v>13439341</v>
       </c>
       <c r="C176">
-        <v>15531924169.306095</v>
+        <v>15105662691.280113</v>
       </c>
       <c r="D176">
-        <v>1131131.091551784</v>
+        <v>1097776.6923288633</v>
       </c>
       <c r="E176">
-        <v>20568751.895263888</v>
+        <v>19511186.579168767</v>
       </c>
       <c r="F176">
-        <v>1155.7057871592137</v>
+        <v>1123.9883481846405</v>
       </c>
       <c r="G176">
-        <v>8.4165666423062252E-2</v>
+        <v>8.1683818598610097E-2</v>
       </c>
       <c r="H176">
-        <v>1.530488131468938</v>
+        <v>1.4517963774539813</v>
       </c>
       <c r="I176" t="s">
         <v>37</v>
@@ -7781,22 +7781,22 @@
         <v>14171621</v>
       </c>
       <c r="C177">
-        <v>78222345652.821045</v>
+        <v>78296181136.799957</v>
       </c>
       <c r="D177">
-        <v>4977129.755814922</v>
+        <v>5066269.9569673399</v>
       </c>
       <c r="E177">
-        <v>84488360.821266845</v>
+        <v>83653410.756396711</v>
       </c>
       <c r="F177">
-        <v>5519.6470222299231</v>
+        <v>5524.8571166841084</v>
       </c>
       <c r="G177">
-        <v>0.3512039840618742</v>
+        <v>0.35749403381358702</v>
       </c>
       <c r="H177">
-        <v>5.9617993468260861</v>
+        <v>5.9028822995193497</v>
       </c>
       <c r="I177" t="s">
         <v>31</v>
@@ -7822,22 +7822,22 @@
         <v>1940463</v>
       </c>
       <c r="C178">
-        <v>10293955010.040094</v>
+        <v>10266595288.886259</v>
       </c>
       <c r="D178">
-        <v>619256.15879474033</v>
+        <v>602722.67876512592</v>
       </c>
       <c r="E178">
-        <v>10502533.998061985</v>
+        <v>10278918.421266159</v>
       </c>
       <c r="F178">
-        <v>5304.8963108495727</v>
+        <v>5290.7967268050252</v>
       </c>
       <c r="G178">
-        <v>0.3191280425314682</v>
+        <v>0.31060766361694397</v>
       </c>
       <c r="H178">
-        <v>5.4123855997573695</v>
+        <v>5.2971473412614198</v>
       </c>
       <c r="I178" t="s">
         <v>32</v>
@@ -7863,22 +7863,22 @@
         <v>825950</v>
       </c>
       <c r="C179">
-        <v>1149168110.3168855</v>
+        <v>1147422996.7629929</v>
       </c>
       <c r="D179">
         <v>0</v>
       </c>
       <c r="E179">
-        <v>101151933.99479468</v>
+        <v>101658931.87196769</v>
       </c>
       <c r="F179">
-        <v>1391.3289064917797</v>
+        <v>1389.2160503214393</v>
       </c>
       <c r="G179">
         <v>0</v>
       </c>
       <c r="H179">
-        <v>122.46738179647035</v>
+        <v>123.08121783639166</v>
       </c>
       <c r="I179" t="s">
         <v>24</v>
@@ -7904,22 +7904,22 @@
         <v>166824</v>
       </c>
       <c r="C180">
-        <v>448567995.39237118</v>
+        <v>444353475.03682202</v>
       </c>
       <c r="D180">
         <v>0</v>
       </c>
       <c r="E180">
-        <v>38720498.092561334</v>
+        <v>38865552.372459792</v>
       </c>
       <c r="F180">
-        <v>2688.8696793768954</v>
+        <v>2663.6064057738818</v>
       </c>
       <c r="G180">
         <v>0</v>
       </c>
       <c r="H180">
-        <v>232.10388249029717</v>
+        <v>232.97338735709366</v>
       </c>
       <c r="I180" t="s">
         <v>36</v>
@@ -8027,22 +8027,22 @@
         <v>334348.61</v>
       </c>
       <c r="C183">
-        <v>1434359105.2761424</v>
+        <v>1418685819.4807439</v>
       </c>
       <c r="D183">
         <v>0</v>
       </c>
       <c r="E183">
-        <v>122145686.28092997</v>
+        <v>124068833.48149748</v>
       </c>
       <c r="F183">
-        <v>4290.0106726214372</v>
+        <v>4243.1335948450451</v>
       </c>
       <c r="G183">
         <v>0</v>
       </c>
       <c r="H183">
-        <v>365.3243429991528</v>
+        <v>371.07626522358652</v>
       </c>
       <c r="I183" t="s">
         <v>35</v>
@@ -8109,22 +8109,22 @@
         <v>11106837</v>
       </c>
       <c r="C185">
-        <v>18263142973.661293</v>
+        <v>18265024826.869141</v>
       </c>
       <c r="D185">
-        <v>1379434.6294000295</v>
+        <v>1376086.8387690091</v>
       </c>
       <c r="E185">
-        <v>28316041.726716772</v>
+        <v>27738152.910544947</v>
       </c>
       <c r="F185">
-        <v>1644.3153864292142</v>
+        <v>1644.4848183933141</v>
       </c>
       <c r="G185">
-        <v>0.1241968914642422</v>
+        <v>0.1238954743613334</v>
       </c>
       <c r="H185">
-        <v>2.5494244425048076</v>
+        <v>2.4973944346662282</v>
       </c>
       <c r="I185" t="s">
         <v>17</v>

</xml_diff>